<commit_message>
Atualização contratos 068 Wells e 069 José Naves
</commit_message>
<xml_diff>
--- a/vendas_cafe_em_reais.xlsx
+++ b/vendas_cafe_em_reais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotocastro/PycharmProjects/Vendas Cafe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3D1F88-A0EE-DD4C-904E-2AC13FCA024D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC356FB8-A029-C147-BB5E-C918FB43C6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="940" windowWidth="24960" windowHeight="16540" activeTab="2" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
+    <workbookView xWindow="4440" yWindow="940" windowWidth="24960" windowHeight="16540" activeTab="1" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2 (2)" sheetId="16" state="hidden" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="CashFlow_Edson_Luiz" sheetId="3" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Q$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Q$69</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'VENDA CAFÉ 220125'!$A$3:$Z$61</definedName>
     <definedName name="LITRAGEM" localSheetId="7">#REF!</definedName>
     <definedName name="LITRAGEM" localSheetId="5">#REF!</definedName>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="352">
   <si>
     <t>026/24</t>
   </si>
@@ -1108,6 +1108,24 @@
   </si>
   <si>
     <t>060-064</t>
+  </si>
+  <si>
+    <t>067/25</t>
+  </si>
+  <si>
+    <t>068/25</t>
+  </si>
+  <si>
+    <t>069/25</t>
+  </si>
+  <si>
+    <t>Paulo Henrique Teixeira</t>
+  </si>
+  <si>
+    <t>Wells Coffee</t>
+  </si>
+  <si>
+    <t>Naves Comércio de Café</t>
   </si>
 </sst>
 </file>
@@ -4504,10 +4522,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T66"/>
+  <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -4582,25 +4601,25 @@
         <v>2023</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="D2" s="159" t="s">
-        <v>86</v>
+        <v>264</v>
       </c>
       <c r="E2" s="2">
-        <v>0.5</v>
+        <v>320</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H2" s="2">
-        <v>0</v>
+        <v>13.7</v>
       </c>
       <c r="I2" s="158">
         <v>45371</v>
@@ -4609,18 +4628,27 @@
         <v>1</v>
       </c>
       <c r="K2" s="158">
-        <v>45371</v>
+        <f>I2+90</f>
+        <v>45461</v>
       </c>
       <c r="L2" s="155"/>
-      <c r="M2" s="155"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="160"/>
+      <c r="M2" s="155">
+        <v>271.5</v>
+      </c>
+      <c r="N2" s="3">
+        <f>M2*E2</f>
+        <v>86880</v>
+      </c>
+      <c r="O2" s="160">
+        <v>4.9740000000000002</v>
+      </c>
       <c r="P2" s="3">
-        <v>1400</v>
+        <f>O2*M2</f>
+        <v>1350.441</v>
       </c>
       <c r="Q2" s="3">
-        <f t="shared" ref="Q2:Q23" si="0">P2*E2</f>
-        <v>700</v>
+        <f>P2*E2</f>
+        <v>432141.12</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -4628,7 +4656,7 @@
         <v>2023</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>42</v>
@@ -4649,33 +4677,33 @@
         <v>13.7</v>
       </c>
       <c r="I3" s="158">
-        <v>45371</v>
+        <v>45442</v>
       </c>
       <c r="J3" s="2">
         <v>1</v>
       </c>
       <c r="K3" s="158">
         <f>I3+90</f>
-        <v>45461</v>
+        <v>45532</v>
       </c>
       <c r="L3" s="155"/>
       <c r="M3" s="155">
         <v>271.5</v>
       </c>
       <c r="N3" s="3">
-        <f t="shared" ref="N3:N9" si="1">M3*E3</f>
+        <f>M3*E3</f>
         <v>86880</v>
       </c>
       <c r="O3" s="160">
-        <v>4.9740000000000002</v>
+        <v>5.0419999999999998</v>
       </c>
       <c r="P3" s="3">
         <f>O3*M3</f>
-        <v>1350.441</v>
+        <v>1368.903</v>
       </c>
       <c r="Q3" s="3">
-        <f t="shared" si="0"/>
-        <v>432141.12</v>
+        <f>P3*E3</f>
+        <v>438048.96</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -4718,7 +4746,7 @@
         <v>271.5</v>
       </c>
       <c r="N4" s="3">
-        <f t="shared" si="1"/>
+        <f>M4*E4</f>
         <v>86880</v>
       </c>
       <c r="O4" s="160">
@@ -4729,7 +4757,7 @@
         <v>1368.903</v>
       </c>
       <c r="Q4" s="3">
-        <f t="shared" si="0"/>
+        <f>P4*E4</f>
         <v>438048.96</v>
       </c>
     </row>
@@ -4773,7 +4801,7 @@
         <v>271.5</v>
       </c>
       <c r="N5" s="3">
-        <f t="shared" si="1"/>
+        <f>M5*E5</f>
         <v>86880</v>
       </c>
       <c r="O5" s="160">
@@ -4784,7 +4812,7 @@
         <v>1368.903</v>
       </c>
       <c r="Q5" s="3">
-        <f t="shared" si="0"/>
+        <f>P5*E5</f>
         <v>438048.96</v>
       </c>
     </row>
@@ -4827,7 +4855,7 @@
         <v>326.8</v>
       </c>
       <c r="N6" s="3">
-        <f t="shared" si="1"/>
+        <f>M6*E6</f>
         <v>104576</v>
       </c>
       <c r="O6" s="160">
@@ -4839,7 +4867,7 @@
         <v>1856.0115799999999</v>
       </c>
       <c r="Q6" s="3">
-        <f t="shared" si="0"/>
+        <f>P6*E6</f>
         <v>593923.70559999999</v>
       </c>
     </row>
@@ -4848,16 +4876,16 @@
         <v>2023</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>277</v>
+        <v>332</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D7" s="159" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="E7" s="2">
-        <v>280</v>
+        <v>0.5</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>32</v>
@@ -4866,36 +4894,27 @@
         <v>32</v>
       </c>
       <c r="H7" s="2">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="I7" s="158">
-        <v>45383</v>
+        <v>45371</v>
       </c>
       <c r="J7" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" s="158">
-        <v>45597</v>
+        <v>45371</v>
       </c>
       <c r="L7" s="155"/>
-      <c r="M7" s="155">
-        <v>316.81060714285712</v>
-      </c>
-      <c r="N7" s="3">
-        <f t="shared" si="1"/>
-        <v>88706.97</v>
-      </c>
-      <c r="O7" s="160">
-        <f>5.76</f>
-        <v>5.76</v>
-      </c>
+      <c r="M7" s="155"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="160"/>
       <c r="P7" s="3">
-        <f>M7*O7</f>
-        <v>1824.8290971428569</v>
+        <v>1400</v>
       </c>
       <c r="Q7" s="3">
-        <f t="shared" si="0"/>
-        <v>510952.14719999995</v>
+        <f>P7*E7</f>
+        <v>700</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -4903,54 +4922,54 @@
         <v>2023</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>334</v>
+        <v>277</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D8" s="159" t="s">
-        <v>264</v>
+        <v>46</v>
       </c>
       <c r="E8" s="2">
-        <v>320</v>
+        <v>280</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H8" s="2">
-        <v>13.7</v>
+        <v>18</v>
       </c>
       <c r="I8" s="158">
-        <v>45442</v>
+        <v>45383</v>
       </c>
       <c r="J8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K8" s="158">
-        <f>I8+90</f>
-        <v>45532</v>
+        <v>45597</v>
       </c>
       <c r="L8" s="155"/>
       <c r="M8" s="155">
-        <v>271.5</v>
+        <v>316.81060714285712</v>
       </c>
       <c r="N8" s="3">
-        <f t="shared" si="1"/>
-        <v>86880</v>
+        <f>M8*E8</f>
+        <v>88706.97</v>
       </c>
       <c r="O8" s="160">
-        <v>5.0419999999999998</v>
+        <f>5.76</f>
+        <v>5.76</v>
       </c>
       <c r="P8" s="3">
-        <f>O8*M8</f>
-        <v>1368.903</v>
+        <f>M8*O8</f>
+        <v>1824.8290971428569</v>
       </c>
       <c r="Q8" s="3">
-        <f t="shared" si="0"/>
-        <v>438048.96</v>
+        <f>P8*E8</f>
+        <v>510952.14719999995</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -4993,7 +5012,7 @@
         <v>300.27999999999997</v>
       </c>
       <c r="N9" s="3">
-        <f t="shared" si="1"/>
+        <f>M9*E9</f>
         <v>15013.999999999998</v>
       </c>
       <c r="O9" s="160">
@@ -5004,7 +5023,7 @@
         <v>1629.3192799999999</v>
       </c>
       <c r="Q9" s="3">
-        <f t="shared" si="0"/>
+        <f>P9*E9</f>
         <v>81465.963999999993</v>
       </c>
     </row>
@@ -5013,45 +5032,55 @@
         <v>2023</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="D10" s="159" t="s">
-        <v>86</v>
+        <v>264</v>
       </c>
       <c r="E10" s="2">
-        <v>3</v>
+        <v>320</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H10" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I10" s="158">
         <v>45473</v>
       </c>
       <c r="J10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" s="158">
-        <v>45580</v>
+        <f>I10+90</f>
+        <v>45563</v>
       </c>
       <c r="L10" s="155"/>
-      <c r="M10" s="155"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="160"/>
+      <c r="M10" s="155">
+        <v>308.54000000000002</v>
+      </c>
+      <c r="N10" s="3">
+        <f>M10*E10</f>
+        <v>98732.800000000003</v>
+      </c>
+      <c r="O10" s="160">
+        <f>572795/N10</f>
+        <v>5.8014661794256819</v>
+      </c>
       <c r="P10" s="3">
-        <v>1500</v>
+        <f>M10*O10</f>
+        <v>1789.984375</v>
       </c>
       <c r="Q10" s="3">
-        <f t="shared" si="0"/>
-        <v>4500</v>
+        <f>P10*E10</f>
+        <v>572795</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -5059,7 +5088,7 @@
         <v>2023</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>42</v>
@@ -5080,14 +5109,14 @@
         <v>15</v>
       </c>
       <c r="I11" s="158">
-        <v>45473</v>
+        <v>45503</v>
       </c>
       <c r="J11" s="2">
         <v>1</v>
       </c>
       <c r="K11" s="158">
         <f>I11+90</f>
-        <v>45563</v>
+        <v>45593</v>
       </c>
       <c r="L11" s="155"/>
       <c r="M11" s="155">
@@ -5098,16 +5127,16 @@
         <v>98732.800000000003</v>
       </c>
       <c r="O11" s="160">
-        <f>572795/N11</f>
-        <v>5.8014661794256819</v>
+        <f>579189/N11</f>
+        <v>5.8662268263434241</v>
       </c>
       <c r="P11" s="3">
         <f>M11*O11</f>
-        <v>1789.984375</v>
+        <v>1809.9656250000003</v>
       </c>
       <c r="Q11" s="3">
-        <f t="shared" si="0"/>
-        <v>572795</v>
+        <f>P11*E11</f>
+        <v>579189.00000000012</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -5115,19 +5144,19 @@
         <v>2023</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D12" s="159" t="s">
-        <v>343</v>
+        <v>86</v>
       </c>
       <c r="E12" s="2">
-        <v>138</v>
+        <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>32</v>
@@ -5136,32 +5165,32 @@
         <v>0</v>
       </c>
       <c r="I12" s="158">
-        <v>45485</v>
+        <v>45473</v>
       </c>
       <c r="J12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" s="158">
-        <v>45485</v>
+        <v>45580</v>
       </c>
       <c r="L12" s="155"/>
       <c r="M12" s="155"/>
       <c r="N12" s="3"/>
       <c r="O12" s="160"/>
       <c r="P12" s="3">
-        <v>1520</v>
+        <v>1500</v>
       </c>
       <c r="Q12" s="3">
-        <f t="shared" si="0"/>
-        <v>209760</v>
+        <f>P12*E12</f>
+        <v>4500</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>339</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>42</v>
@@ -5176,40 +5205,40 @@
         <v>27</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H13" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I13" s="158">
-        <v>45503</v>
+        <v>45564</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
       </c>
       <c r="K13" s="158">
-        <f>I13+90</f>
-        <v>45593</v>
-      </c>
-      <c r="L13" s="155"/>
+        <v>45627</v>
+      </c>
+      <c r="L13" s="155">
+        <v>251.05</v>
+      </c>
       <c r="M13" s="155">
-        <v>308.54000000000002</v>
+        <v>345.31693999999999</v>
       </c>
       <c r="N13" s="3">
-        <f t="shared" ref="N13:N23" si="2">M13*E13</f>
-        <v>98732.800000000003</v>
+        <f>M13*E13</f>
+        <v>110501.42079999999</v>
       </c>
       <c r="O13" s="160">
-        <f>579189/N13</f>
-        <v>5.8662268263434241</v>
+        <v>5.8349509259259262</v>
       </c>
       <c r="P13" s="3">
-        <f t="shared" ref="P13:P23" si="3">M13*O13</f>
-        <v>1809.9656250000003</v>
+        <f>M13*O13</f>
+        <v>2014.9073987909073</v>
       </c>
       <c r="Q13" s="3">
-        <f t="shared" si="0"/>
-        <v>579189.00000000012</v>
+        <f>P13*E13</f>
+        <v>644770.36761309032</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5217,7 +5246,7 @@
         <v>2024</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>42</v>
@@ -5226,103 +5255,92 @@
         <v>264</v>
       </c>
       <c r="E14" s="2">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H14" s="2">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="I14" s="158">
-        <v>45349</v>
+        <v>45564</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
       <c r="K14" s="158">
-        <v>45778</v>
+        <v>45627</v>
       </c>
       <c r="L14" s="155">
-        <v>393.05</v>
+        <v>251.05</v>
       </c>
       <c r="M14" s="155">
-        <v>557.75861999999995</v>
+        <v>345.31693999999999</v>
       </c>
       <c r="N14" s="3">
-        <f t="shared" si="2"/>
-        <v>89241.379199999996</v>
+        <f>M14*E14</f>
+        <v>110501.42079999999</v>
       </c>
       <c r="O14" s="160">
-        <v>5.5049999999999999</v>
+        <v>5.8349509259259262</v>
       </c>
       <c r="P14" s="3">
-        <f t="shared" si="3"/>
-        <v>3070.4612030999997</v>
+        <f>M14*O14</f>
+        <v>2014.9073987909073</v>
       </c>
       <c r="Q14" s="3">
-        <f t="shared" si="0"/>
-        <v>491273.79249599995</v>
+        <f>P14*E14</f>
+        <v>644770.36761309032</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>4</v>
+        <v>341</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D15" s="159" t="s">
-        <v>264</v>
+        <v>343</v>
       </c>
       <c r="E15" s="2">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H15" s="2">
-        <v>-8</v>
+        <v>0</v>
       </c>
       <c r="I15" s="158">
-        <v>45349</v>
+        <v>45485</v>
       </c>
       <c r="J15" s="2">
         <v>1</v>
       </c>
       <c r="K15" s="158">
-        <v>45748</v>
-      </c>
-      <c r="L15" s="155">
-        <v>393.05</v>
-      </c>
-      <c r="M15" s="155">
-        <v>526.34211999999991</v>
-      </c>
-      <c r="N15" s="3">
-        <f t="shared" si="2"/>
-        <v>84214.739199999982</v>
-      </c>
-      <c r="O15" s="160">
-        <f>(499233.9/(SUM(N14:N15)/2))</f>
-        <v>5.7563135230403049</v>
-      </c>
+        <v>45485</v>
+      </c>
+      <c r="L15" s="155"/>
+      <c r="M15" s="155"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="160"/>
       <c r="P15" s="3">
-        <f t="shared" si="3"/>
-        <v>3029.7902631017023</v>
+        <v>1520</v>
       </c>
       <c r="Q15" s="3">
-        <f t="shared" si="0"/>
-        <v>484766.44209627237</v>
+        <f>P15*E15</f>
+        <v>209760</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
@@ -5330,13 +5348,13 @@
         <v>2024</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="159" t="s">
-        <v>264</v>
+        <v>91</v>
       </c>
       <c r="E16" s="2">
         <v>320</v>
@@ -5345,40 +5363,38 @@
         <v>27</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H16" s="2">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="I16" s="158">
-        <v>45564</v>
+        <v>45666</v>
       </c>
       <c r="J16" s="2">
         <v>1</v>
       </c>
       <c r="K16" s="158">
-        <v>45627</v>
-      </c>
-      <c r="L16" s="155">
-        <v>251.05</v>
-      </c>
+        <v>45658</v>
+      </c>
+      <c r="L16" s="155"/>
       <c r="M16" s="155">
-        <v>345.31693999999999</v>
+        <v>468.27119999999996</v>
       </c>
       <c r="N16" s="3">
-        <f t="shared" si="2"/>
-        <v>110501.42079999999</v>
+        <f>M16*E16</f>
+        <v>149846.78399999999</v>
       </c>
       <c r="O16" s="160">
-        <v>5.8349509259259262</v>
+        <v>5.8236999999999997</v>
       </c>
       <c r="P16" s="3">
-        <f t="shared" si="3"/>
-        <v>2014.9073987909073</v>
+        <f>M16*O16</f>
+        <v>2727.0709874399995</v>
       </c>
       <c r="Q16" s="3">
-        <f t="shared" si="0"/>
-        <v>644770.36761309032</v>
+        <f>P16*E16</f>
+        <v>872662.71598079987</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -5386,7 +5402,7 @@
         <v>2024</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>42</v>
@@ -5401,7 +5417,7 @@
         <v>27</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H17" s="2">
         <v>10</v>
@@ -5422,18 +5438,18 @@
         <v>345.31693999999999</v>
       </c>
       <c r="N17" s="3">
-        <f t="shared" si="2"/>
+        <f>M17*E17</f>
         <v>110501.42079999999</v>
       </c>
       <c r="O17" s="160">
         <v>5.8349509259259262</v>
       </c>
       <c r="P17" s="3">
-        <f t="shared" si="3"/>
+        <f>M17*O17</f>
         <v>2014.9073987909073</v>
       </c>
       <c r="Q17" s="3">
-        <f t="shared" si="0"/>
+        <f>P17*E17</f>
         <v>644770.36761309032</v>
       </c>
     </row>
@@ -5442,7 +5458,7 @@
         <v>2024</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>42</v>
@@ -5463,34 +5479,34 @@
         <v>10</v>
       </c>
       <c r="I18" s="158">
-        <v>45564</v>
+        <v>45678</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
       </c>
       <c r="K18" s="158">
-        <v>45627</v>
+        <v>45717</v>
       </c>
       <c r="L18" s="155">
-        <v>251.05</v>
+        <v>342</v>
       </c>
       <c r="M18" s="155">
-        <v>345.31693999999999</v>
+        <v>465.62559999999996</v>
       </c>
       <c r="N18" s="3">
-        <f t="shared" si="2"/>
-        <v>110501.42079999999</v>
+        <f>M18*E18</f>
+        <v>149000.19199999998</v>
       </c>
       <c r="O18" s="160">
-        <v>5.8349509259259262</v>
+        <v>5.7249999999999996</v>
       </c>
       <c r="P18" s="3">
-        <f t="shared" si="3"/>
-        <v>2014.9073987909073</v>
+        <f>M18*O18</f>
+        <v>2665.7065599999996</v>
       </c>
       <c r="Q18" s="3">
-        <f t="shared" si="0"/>
-        <v>644770.36761309032</v>
+        <f>P18*E18</f>
+        <v>853026.09919999982</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
@@ -5498,7 +5514,7 @@
         <v>2024</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>42</v>
@@ -5507,46 +5523,46 @@
         <v>264</v>
       </c>
       <c r="E19" s="2">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H19" s="2">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="I19" s="158">
-        <v>45599</v>
+        <v>45630</v>
       </c>
       <c r="J19" s="2">
         <v>1</v>
       </c>
       <c r="K19" s="158">
-        <v>45658</v>
+        <v>45689</v>
       </c>
       <c r="L19" s="155">
-        <v>280.75</v>
+        <v>323.25</v>
       </c>
       <c r="M19" s="155">
-        <v>404.4461</v>
+        <v>440.82310000000001</v>
       </c>
       <c r="N19" s="3">
-        <f t="shared" si="2"/>
-        <v>64711.376000000004</v>
+        <f>M19*E19</f>
+        <v>141063.39199999999</v>
       </c>
       <c r="O19" s="160">
-        <v>5.7499741972351099</v>
+        <v>5.7669999035936632</v>
       </c>
       <c r="P19" s="3">
-        <f t="shared" si="3"/>
-        <v>2325.554639172371</v>
+        <f>M19*O19</f>
+        <v>2542.2267752018597</v>
       </c>
       <c r="Q19" s="3">
-        <f t="shared" si="0"/>
-        <v>372088.74226757936</v>
+        <f>P19*E19</f>
+        <v>813512.56806459511</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -5554,7 +5570,7 @@
         <v>2024</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>42</v>
@@ -5563,46 +5579,46 @@
         <v>264</v>
       </c>
       <c r="E20" s="2">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>37</v>
       </c>
       <c r="H20" s="2">
-        <v>-8</v>
+        <v>10</v>
       </c>
       <c r="I20" s="158">
-        <v>45599</v>
+        <v>45678</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
       </c>
       <c r="K20" s="158">
-        <v>45658</v>
+        <v>45717</v>
       </c>
       <c r="L20" s="155">
-        <v>280.75</v>
+        <v>342</v>
       </c>
       <c r="M20" s="155">
-        <v>360.7937</v>
+        <v>465.62559999999996</v>
       </c>
       <c r="N20" s="3">
-        <f t="shared" si="2"/>
-        <v>57726.991999999998</v>
+        <f>M20*E20</f>
+        <v>149000.19199999998</v>
       </c>
       <c r="O20" s="160">
-        <v>5.7499741972351099</v>
+        <v>5.7249999999999996</v>
       </c>
       <c r="P20" s="3">
-        <f t="shared" si="3"/>
-        <v>2074.5544655249851</v>
+        <f>M20*O20</f>
+        <v>2665.7065599999996</v>
       </c>
       <c r="Q20" s="3">
-        <f t="shared" si="0"/>
-        <v>331928.71448399761</v>
+        <f>P20*E20</f>
+        <v>853026.09919999982</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
@@ -5610,7 +5626,7 @@
         <v>2024</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>42</v>
@@ -5631,34 +5647,35 @@
         <v>10</v>
       </c>
       <c r="I21" s="158">
-        <v>45630</v>
+        <v>45746</v>
       </c>
       <c r="J21" s="2">
         <v>1</v>
       </c>
       <c r="K21" s="158">
-        <v>45689</v>
+        <v>45809</v>
       </c>
       <c r="L21" s="155">
-        <v>323.25</v>
+        <v>329.5</v>
       </c>
       <c r="M21" s="155">
-        <v>440.82310000000001</v>
+        <v>449.09059999999999</v>
       </c>
       <c r="N21" s="3">
-        <f t="shared" si="2"/>
-        <v>141063.39199999999</v>
+        <f>M21*E21</f>
+        <v>143708.992</v>
       </c>
       <c r="O21" s="160">
-        <v>5.7669999035936632</v>
+        <f>798447.15/N21</f>
+        <v>5.5559999335323429</v>
       </c>
       <c r="P21" s="3">
-        <f t="shared" si="3"/>
-        <v>2542.2267752018597</v>
+        <f>M21*O21</f>
+        <v>2495.1473437499999</v>
       </c>
       <c r="Q21" s="3">
-        <f t="shared" si="0"/>
-        <v>813512.56806459511</v>
+        <f>P21*E21</f>
+        <v>798447.14999999991</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
@@ -5666,7 +5683,7 @@
         <v>2024</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>42</v>
@@ -5675,47 +5692,46 @@
         <v>264</v>
       </c>
       <c r="E22" s="2">
-        <v>320</v>
+        <v>160</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H22" s="2">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="I22" s="158">
-        <f>I21</f>
-        <v>45630</v>
+        <v>45349</v>
       </c>
       <c r="J22" s="2">
         <v>1</v>
       </c>
       <c r="K22" s="158">
-        <v>45689</v>
+        <v>45778</v>
       </c>
       <c r="L22" s="155">
-        <v>323.25</v>
+        <v>393.05</v>
       </c>
       <c r="M22" s="155">
-        <v>493.73509999999999</v>
+        <v>557.75861999999995</v>
       </c>
       <c r="N22" s="3">
-        <f t="shared" si="2"/>
-        <v>157995.23199999999</v>
+        <f>M22*E22</f>
+        <v>89241.379199999996</v>
       </c>
       <c r="O22" s="160">
-        <v>5.7669999035936632</v>
+        <v>5.5049999999999999</v>
       </c>
       <c r="P22" s="3">
-        <f t="shared" si="3"/>
-        <v>2847.3702741008078</v>
+        <f>M22*O22</f>
+        <v>3070.4612030999997</v>
       </c>
       <c r="Q22" s="3">
-        <f t="shared" si="0"/>
-        <v>911158.48771225847</v>
+        <f>P22*E22</f>
+        <v>491273.79249599995</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -5723,7 +5739,7 @@
         <v>2024</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>42</v>
@@ -5732,47 +5748,46 @@
         <v>264</v>
       </c>
       <c r="E23" s="2">
-        <v>320</v>
+        <v>160</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H23" s="2">
-        <v>-8</v>
+        <v>25</v>
       </c>
       <c r="I23" s="158">
-        <f>I22</f>
-        <v>45630</v>
+        <v>45599</v>
       </c>
       <c r="J23" s="2">
         <v>1</v>
       </c>
       <c r="K23" s="158">
-        <v>45689</v>
+        <v>45658</v>
       </c>
       <c r="L23" s="155">
-        <v>323.25</v>
+        <v>280.75</v>
       </c>
       <c r="M23" s="155">
-        <v>417.0127</v>
+        <v>404.4461</v>
       </c>
       <c r="N23" s="3">
-        <f t="shared" si="2"/>
-        <v>133444.06400000001</v>
+        <f>M23*E23</f>
+        <v>64711.376000000004</v>
       </c>
       <c r="O23" s="160">
-        <v>5.7669999035936632</v>
+        <v>5.7499741972351099</v>
       </c>
       <c r="P23" s="3">
-        <f t="shared" si="3"/>
-        <v>2404.912200697333</v>
+        <f>M23*O23</f>
+        <v>2325.554639172371</v>
       </c>
       <c r="Q23" s="3">
-        <f t="shared" si="0"/>
-        <v>769571.90422314662</v>
+        <f>P23*E23</f>
+        <v>372088.74226757936</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
@@ -5780,45 +5795,56 @@
         <v>2024</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="D24" s="159" t="s">
-        <v>31</v>
+        <v>264</v>
       </c>
       <c r="E24" s="2">
-        <v>500</v>
+        <v>160</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H24" s="2">
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="I24" s="158">
-        <v>45631</v>
+        <v>45349</v>
       </c>
       <c r="J24" s="2">
         <v>1</v>
       </c>
       <c r="K24" s="158">
-        <v>45631</v>
-      </c>
-      <c r="L24" s="158"/>
-      <c r="M24" s="155"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="160"/>
+        <v>45748</v>
+      </c>
+      <c r="L24" s="155">
+        <v>393.05</v>
+      </c>
+      <c r="M24" s="155">
+        <v>526.34211999999991</v>
+      </c>
+      <c r="N24" s="3">
+        <f>M24*E24</f>
+        <v>84214.739199999982</v>
+      </c>
+      <c r="O24" s="160">
+        <f>(499233.9/(SUM(N23:N24)/2))</f>
+        <v>6.7044507181236135</v>
+      </c>
       <c r="P24" s="3">
-        <v>2105</v>
+        <f>M24*O24</f>
+        <v>3528.8348044127047</v>
       </c>
       <c r="Q24" s="3">
-        <f>E24*P24</f>
-        <v>1052500</v>
+        <f>P24*E24</f>
+        <v>564613.5687060327</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
@@ -5826,45 +5852,55 @@
         <v>2024</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="D25" s="159" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="E25" s="2">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H25" s="2">
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="I25" s="158">
-        <v>45632</v>
+        <v>45599</v>
       </c>
       <c r="J25" s="2">
         <v>1</v>
       </c>
       <c r="K25" s="158">
-        <v>45632</v>
-      </c>
-      <c r="L25" s="158"/>
-      <c r="M25" s="155"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="160"/>
+        <v>45658</v>
+      </c>
+      <c r="L25" s="155">
+        <v>280.75</v>
+      </c>
+      <c r="M25" s="155">
+        <v>360.7937</v>
+      </c>
+      <c r="N25" s="3">
+        <f>M25*E25</f>
+        <v>57726.991999999998</v>
+      </c>
+      <c r="O25" s="160">
+        <v>5.7499741972351099</v>
+      </c>
       <c r="P25" s="3">
-        <v>2200</v>
+        <f>M25*O25</f>
+        <v>2074.5544655249851</v>
       </c>
       <c r="Q25" s="3">
-        <f>E25*P25</f>
-        <v>44000</v>
+        <f>P25*E25</f>
+        <v>331928.71448399761</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
@@ -5872,45 +5908,56 @@
         <v>2024</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="D26" s="159" t="s">
-        <v>24</v>
+        <v>264</v>
       </c>
       <c r="E26" s="2">
-        <v>4</v>
+        <v>320</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H26" s="2">
-        <v>0</v>
+        <v>-28</v>
       </c>
       <c r="I26" s="158">
-        <v>45656</v>
+        <v>45746</v>
       </c>
       <c r="J26" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K26" s="158">
-        <v>45717</v>
-      </c>
-      <c r="L26" s="158"/>
-      <c r="M26" s="155"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="160"/>
+        <v>45809</v>
+      </c>
+      <c r="L26" s="155">
+        <v>370.95</v>
+      </c>
+      <c r="M26" s="155">
+        <v>453.65425999999997</v>
+      </c>
+      <c r="N26" s="3">
+        <f>M26*E26</f>
+        <v>145169.36319999999</v>
+      </c>
+      <c r="O26" s="160">
+        <f>806560.96/N26</f>
+        <v>5.5559998488716937</v>
+      </c>
       <c r="P26" s="3">
-        <v>2500</v>
+        <f>M26*O26</f>
+        <v>2520.5029999999997</v>
       </c>
       <c r="Q26" s="3">
-        <f>E26*P26</f>
-        <v>10000</v>
+        <f>P26*E26</f>
+        <v>806560.96</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
@@ -5918,46 +5965,56 @@
         <v>2024</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="D27" s="159" t="s">
-        <v>24</v>
+        <v>264</v>
       </c>
       <c r="E27" s="2">
-        <v>4</v>
+        <v>320</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H27" s="2">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I27" s="158">
         <f>I26</f>
-        <v>45656</v>
+        <v>45746</v>
       </c>
       <c r="J27" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K27" s="158">
-        <v>45717</v>
-      </c>
-      <c r="L27" s="158"/>
-      <c r="M27" s="155"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="160"/>
+        <v>45689</v>
+      </c>
+      <c r="L27" s="155">
+        <v>323.25</v>
+      </c>
+      <c r="M27" s="155">
+        <v>493.73509999999999</v>
+      </c>
+      <c r="N27" s="3">
+        <f>M27*E27</f>
+        <v>157995.23199999999</v>
+      </c>
+      <c r="O27" s="160">
+        <v>5.7669999035936632</v>
+      </c>
       <c r="P27" s="3">
-        <v>2137</v>
+        <f>M27*O27</f>
+        <v>2847.3702741008078</v>
       </c>
       <c r="Q27" s="3">
-        <f>E27*P27</f>
-        <v>8548</v>
+        <f>P27*E27</f>
+        <v>911158.48771225847</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
@@ -5965,13 +6022,13 @@
         <v>2024</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D28" s="159" t="s">
-        <v>91</v>
+        <v>19</v>
       </c>
       <c r="E28" s="2">
         <v>320</v>
@@ -5980,38 +6037,39 @@
         <v>27</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H28" s="2">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I28" s="158">
-        <v>45666</v>
+        <v>45671</v>
       </c>
       <c r="J28" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K28" s="158">
-        <v>45658</v>
+        <f>I28</f>
+        <v>45671</v>
       </c>
       <c r="L28" s="155"/>
       <c r="M28" s="155">
-        <v>468.27119999999996</v>
+        <v>325</v>
       </c>
       <c r="N28" s="3">
         <f>M28*E28</f>
-        <v>149846.78399999999</v>
+        <v>104000</v>
       </c>
       <c r="O28" s="160">
-        <v>5.8236999999999997</v>
+        <v>5.8079999999999998</v>
       </c>
       <c r="P28" s="3">
         <f>M28*O28</f>
-        <v>2727.0709874399995</v>
+        <v>1887.6</v>
       </c>
       <c r="Q28" s="3">
         <f>P28*E28</f>
-        <v>872662.71598079987</v>
+        <v>604032</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
@@ -6019,7 +6077,7 @@
         <v>2024</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>42</v>
@@ -6031,23 +6089,23 @@
         <v>320</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H29" s="2">
         <v>0</v>
       </c>
       <c r="I29" s="158">
-        <v>45671</v>
+        <v>45702</v>
       </c>
       <c r="J29" s="2">
         <v>4</v>
       </c>
       <c r="K29" s="158">
         <f>I29</f>
-        <v>45671</v>
+        <v>45702</v>
       </c>
       <c r="L29" s="155"/>
       <c r="M29" s="155">
@@ -6074,55 +6132,45 @@
         <v>2024</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D30" s="159" t="s">
-        <v>264</v>
+        <v>24</v>
       </c>
       <c r="E30" s="2">
-        <v>320</v>
+        <v>4</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H30" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I30" s="158">
-        <v>45678</v>
+        <v>45656</v>
       </c>
       <c r="J30" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K30" s="158">
         <v>45717</v>
       </c>
-      <c r="L30" s="155">
-        <v>342</v>
-      </c>
-      <c r="M30" s="155">
-        <v>465.62559999999996</v>
-      </c>
-      <c r="N30" s="3">
-        <f>M30*E30</f>
-        <v>149000.19199999998</v>
-      </c>
-      <c r="O30" s="160">
-        <v>5.7249999999999996</v>
-      </c>
+      <c r="L30" s="158"/>
+      <c r="M30" s="155"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="160"/>
       <c r="P30" s="3">
-        <f>M30*O30</f>
-        <v>2665.7065599999996</v>
+        <v>2500</v>
       </c>
       <c r="Q30" s="3">
-        <f>P30*E30</f>
-        <v>853026.09919999982</v>
+        <f>E30*P30</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
@@ -6130,55 +6178,46 @@
         <v>2024</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D31" s="159" t="s">
-        <v>264</v>
+        <v>24</v>
       </c>
       <c r="E31" s="2">
-        <v>320</v>
+        <v>4</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H31" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I31" s="158">
-        <v>45678</v>
+        <f>I30</f>
+        <v>45656</v>
       </c>
       <c r="J31" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K31" s="158">
         <v>45717</v>
       </c>
-      <c r="L31" s="155">
-        <v>342</v>
-      </c>
-      <c r="M31" s="155">
-        <v>465.62559999999996</v>
-      </c>
-      <c r="N31" s="3">
-        <f>M31*E31</f>
-        <v>149000.19199999998</v>
-      </c>
-      <c r="O31" s="160">
-        <v>5.7249999999999996</v>
-      </c>
+      <c r="L31" s="158"/>
+      <c r="M31" s="155"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="160"/>
       <c r="P31" s="3">
-        <f>M31*O31</f>
-        <v>2665.7065599999996</v>
+        <v>2137</v>
       </c>
       <c r="Q31" s="3">
-        <f>P31*E31</f>
-        <v>853026.09919999982</v>
+        <f>E31*P31</f>
+        <v>8548</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
@@ -6186,45 +6225,56 @@
         <v>2024</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="D32" s="159" t="s">
-        <v>44</v>
+        <v>264</v>
       </c>
       <c r="E32" s="2">
-        <v>500</v>
+        <v>320</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H32" s="2">
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="I32" s="158">
-        <v>45679</v>
+        <f>I31</f>
+        <v>45656</v>
       </c>
       <c r="J32" s="2">
         <v>1</v>
       </c>
       <c r="K32" s="158">
-        <v>45679</v>
-      </c>
-      <c r="L32" s="158"/>
-      <c r="M32" s="155"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="160"/>
+        <v>45689</v>
+      </c>
+      <c r="L32" s="155">
+        <v>323.25</v>
+      </c>
+      <c r="M32" s="155">
+        <v>417.0127</v>
+      </c>
+      <c r="N32" s="3">
+        <f>M32*E32</f>
+        <v>133444.06400000001</v>
+      </c>
+      <c r="O32" s="160">
+        <v>5.7669999035936632</v>
+      </c>
       <c r="P32" s="3">
-        <v>2000</v>
+        <f>M32*O32</f>
+        <v>2404.912200697333</v>
       </c>
       <c r="Q32" s="3">
-        <f>E32*P32</f>
-        <v>1000000</v>
+        <f>P32*E32</f>
+        <v>769571.90422314662</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -6232,45 +6282,45 @@
         <v>2024</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>181</v>
+        <v>41</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D33" s="159" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="E33" s="2">
-        <v>486.3</v>
+        <v>500</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="H33" s="2">
         <v>0</v>
       </c>
       <c r="I33" s="158">
-        <v>45684</v>
+        <v>45631</v>
       </c>
       <c r="J33" s="2">
         <v>1</v>
       </c>
       <c r="K33" s="158">
-        <v>45684</v>
+        <v>45631</v>
       </c>
       <c r="L33" s="158"/>
       <c r="M33" s="155"/>
       <c r="N33" s="3"/>
       <c r="O33" s="160"/>
       <c r="P33" s="3">
-        <v>810</v>
+        <v>2105</v>
       </c>
       <c r="Q33" s="3">
         <f>E33*P33</f>
-        <v>393903</v>
+        <v>1052500</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
@@ -6278,43 +6328,45 @@
         <v>2024</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>183</v>
+        <v>43</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D34" s="159" t="s">
-        <v>94</v>
+        <v>257</v>
       </c>
       <c r="E34" s="2">
-        <v>363</v>
+        <v>20</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H34" s="2">
         <v>0</v>
       </c>
       <c r="I34" s="158">
-        <v>45684</v>
+        <v>45632</v>
       </c>
       <c r="J34" s="2">
         <v>1</v>
       </c>
       <c r="K34" s="158">
-        <v>45684</v>
+        <v>45632</v>
       </c>
       <c r="L34" s="158"/>
+      <c r="M34" s="155"/>
       <c r="N34" s="3"/>
+      <c r="O34" s="160"/>
       <c r="P34" s="3">
-        <v>1750</v>
+        <v>2200</v>
       </c>
       <c r="Q34" s="3">
         <f>E34*P34</f>
-        <v>635250</v>
+        <v>44000</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
@@ -6322,51 +6374,53 @@
         <v>2024</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D35" s="159" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E35" s="2">
-        <v>320</v>
+        <v>500</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H35" s="2">
         <v>0</v>
       </c>
       <c r="I35" s="158">
-        <v>45695</v>
+        <v>45679</v>
       </c>
       <c r="J35" s="2">
         <v>1</v>
       </c>
       <c r="K35" s="158">
-        <v>45809</v>
-      </c>
-      <c r="L35" s="155"/>
-      <c r="M35" s="155">
-        <v>413</v>
-      </c>
-      <c r="N35" s="3">
-        <f>M35*E35</f>
-        <v>132160</v>
-      </c>
+        <v>45679</v>
+      </c>
+      <c r="L35" s="158"/>
+      <c r="M35" s="155"/>
+      <c r="N35" s="3"/>
       <c r="O35" s="160"/>
+      <c r="P35" s="3">
+        <v>2000</v>
+      </c>
+      <c r="Q35" s="3">
+        <f>E35*P35</f>
+        <v>1000000</v>
+      </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>2024</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>42</v>
@@ -6397,11 +6451,11 @@
       </c>
       <c r="L36" s="155"/>
       <c r="M36" s="155">
-        <v>450</v>
+        <v>413</v>
       </c>
       <c r="N36" s="3">
         <f>M36*E36</f>
-        <v>144000</v>
+        <v>132160</v>
       </c>
       <c r="O36" s="160"/>
     </row>
@@ -6410,7 +6464,7 @@
         <v>2024</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>42</v>
@@ -6419,13 +6473,13 @@
         <v>46</v>
       </c>
       <c r="E37" s="2">
-        <v>223</v>
+        <v>320</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H37" s="2">
         <v>0</v>
@@ -6441,11 +6495,11 @@
       </c>
       <c r="L37" s="155"/>
       <c r="M37" s="155">
-        <v>409.35</v>
+        <v>450</v>
       </c>
       <c r="N37" s="3">
         <f>M37*E37</f>
-        <v>91285.05</v>
+        <v>144000</v>
       </c>
       <c r="O37" s="160"/>
       <c r="T37" s="161"/>
@@ -6455,19 +6509,19 @@
         <v>2024</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>182</v>
+        <v>85</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="D38" s="159" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="E38" s="2">
-        <v>632.20000000000005</v>
+        <v>223</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>32</v>
@@ -6476,44 +6530,42 @@
         <v>0</v>
       </c>
       <c r="I38" s="158">
-        <v>45700</v>
+        <v>45695</v>
       </c>
       <c r="J38" s="2">
         <v>1</v>
       </c>
       <c r="K38" s="158">
-        <v>45700</v>
-      </c>
-      <c r="L38" s="158"/>
-      <c r="M38" s="155"/>
-      <c r="N38" s="3"/>
+        <v>45809</v>
+      </c>
+      <c r="L38" s="155"/>
+      <c r="M38" s="155">
+        <v>409.35</v>
+      </c>
+      <c r="N38" s="3">
+        <f>M38*E38</f>
+        <v>91285.05</v>
+      </c>
       <c r="O38" s="160"/>
-      <c r="P38" s="3">
-        <v>2220</v>
-      </c>
-      <c r="Q38" s="3">
-        <f>E38*P38</f>
-        <v>1403484</v>
-      </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>2024</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>184</v>
+        <v>87</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D39" s="159" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E39" s="2">
-        <v>44.2</v>
+        <v>0.5</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>32</v>
@@ -6522,22 +6574,24 @@
         <v>0</v>
       </c>
       <c r="I39" s="158">
-        <v>45700</v>
+        <v>45708</v>
       </c>
       <c r="J39" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K39" s="158">
-        <v>45700</v>
+        <v>45839</v>
       </c>
       <c r="L39" s="158"/>
+      <c r="M39" s="155"/>
       <c r="N39" s="3"/>
+      <c r="O39" s="160"/>
       <c r="P39" s="3">
-        <v>2400</v>
+        <v>2293.33</v>
       </c>
       <c r="Q39" s="3">
         <f>E39*P39</f>
-        <v>106080</v>
+        <v>1146.665</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
@@ -6545,54 +6599,45 @@
         <v>2024</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D40" s="159" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="E40" s="2">
-        <v>320</v>
+        <v>7</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H40" s="2">
         <v>0</v>
       </c>
       <c r="I40" s="158">
-        <v>45702</v>
+        <v>45708</v>
       </c>
       <c r="J40" s="2">
         <v>4</v>
       </c>
       <c r="K40" s="158">
-        <f>I40</f>
-        <v>45702</v>
-      </c>
-      <c r="L40" s="155"/>
-      <c r="M40" s="155">
-        <v>325</v>
-      </c>
-      <c r="N40" s="3">
-        <f>M40*E40</f>
-        <v>104000</v>
-      </c>
-      <c r="O40" s="160">
-        <v>5.8079999999999998</v>
-      </c>
+        <v>45839</v>
+      </c>
+      <c r="L40" s="158"/>
+      <c r="M40" s="155"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="160"/>
       <c r="P40" s="3">
-        <f>M40*O40</f>
-        <v>1887.6</v>
+        <v>2616.61</v>
       </c>
       <c r="Q40" s="3">
-        <f>P40*E40</f>
-        <v>604032</v>
+        <f>E40*P40</f>
+        <v>18316.27</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
@@ -6600,19 +6645,19 @@
         <v>2024</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>87</v>
+        <v>181</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D41" s="159" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E41" s="2">
-        <v>0.5</v>
+        <v>486.3</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>32</v>
@@ -6621,24 +6666,24 @@
         <v>0</v>
       </c>
       <c r="I41" s="158">
-        <v>45708</v>
+        <v>45684</v>
       </c>
       <c r="J41" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K41" s="158">
-        <v>45839</v>
+        <v>45684</v>
       </c>
       <c r="L41" s="158"/>
       <c r="M41" s="155"/>
       <c r="N41" s="3"/>
       <c r="O41" s="160"/>
       <c r="P41" s="3">
-        <v>2293.33</v>
+        <v>810</v>
       </c>
       <c r="Q41" s="3">
         <f>E41*P41</f>
-        <v>1146.665</v>
+        <v>393903</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
@@ -6646,45 +6691,45 @@
         <v>2024</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>88</v>
+        <v>182</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D42" s="159" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E42" s="2">
-        <v>7</v>
+        <v>632.20000000000005</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H42" s="2">
         <v>0</v>
       </c>
       <c r="I42" s="158">
-        <v>45708</v>
+        <v>45700</v>
       </c>
       <c r="J42" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K42" s="158">
-        <v>45839</v>
+        <v>45700</v>
       </c>
       <c r="L42" s="158"/>
       <c r="M42" s="155"/>
       <c r="N42" s="3"/>
       <c r="O42" s="160"/>
       <c r="P42" s="3">
-        <v>2616.61</v>
+        <v>2220</v>
       </c>
       <c r="Q42" s="3">
         <f>E42*P42</f>
-        <v>18316.27</v>
+        <v>1403484</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
@@ -6692,56 +6737,43 @@
         <v>2024</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>2</v>
+        <v>183</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D43" s="159" t="s">
-        <v>264</v>
+        <v>94</v>
       </c>
       <c r="E43" s="2">
-        <v>320</v>
+        <v>363</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H43" s="2">
-        <v>-28</v>
+        <v>0</v>
       </c>
       <c r="I43" s="158">
-        <v>45746</v>
+        <v>45684</v>
       </c>
       <c r="J43" s="2">
         <v>1</v>
       </c>
       <c r="K43" s="158">
-        <v>45809</v>
-      </c>
-      <c r="L43" s="155">
-        <v>370.95</v>
-      </c>
-      <c r="M43" s="155">
-        <v>453.65425999999997</v>
-      </c>
-      <c r="N43" s="3">
-        <f>M43*E43</f>
-        <v>145169.36319999999</v>
-      </c>
-      <c r="O43" s="160">
-        <f>806560.96/N43</f>
-        <v>5.5559998488716937</v>
-      </c>
+        <v>45684</v>
+      </c>
+      <c r="L43" s="158"/>
+      <c r="N43" s="3"/>
       <c r="P43" s="3">
-        <f>M43*O43</f>
-        <v>2520.5029999999997</v>
+        <v>1750</v>
       </c>
       <c r="Q43" s="3">
-        <f>P43*E43</f>
-        <v>806560.96</v>
+        <f>E43*P43</f>
+        <v>635250</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
@@ -6749,56 +6781,43 @@
         <v>2024</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" s="159" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" s="2">
+        <v>44.2</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H44" s="2">
         <v>0</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D44" s="159" t="s">
-        <v>264</v>
-      </c>
-      <c r="E44" s="2">
-        <v>320</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H44" s="2">
-        <v>10</v>
-      </c>
       <c r="I44" s="158">
-        <v>45746</v>
+        <v>45700</v>
       </c>
       <c r="J44" s="2">
         <v>1</v>
       </c>
       <c r="K44" s="158">
-        <v>45809</v>
-      </c>
-      <c r="L44" s="155">
-        <v>329.5</v>
-      </c>
-      <c r="M44" s="155">
-        <v>449.09059999999999</v>
-      </c>
-      <c r="N44" s="3">
-        <f>M44*E44</f>
-        <v>143708.992</v>
-      </c>
-      <c r="O44" s="160">
-        <f>798447.15/N44</f>
-        <v>5.5559999335323429</v>
-      </c>
+        <v>45700</v>
+      </c>
+      <c r="L44" s="158"/>
+      <c r="N44" s="3"/>
       <c r="P44" s="3">
-        <f>M44*O44</f>
-        <v>2495.1473437499999</v>
+        <v>2400</v>
       </c>
       <c r="Q44" s="3">
-        <f>P44*E44</f>
-        <v>798447.14999999991</v>
+        <f>E44*P44</f>
+        <v>106080</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
@@ -6806,131 +6825,131 @@
         <v>2024</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D45" s="159" t="s">
-        <v>257</v>
+        <v>86</v>
       </c>
       <c r="E45" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H45" s="2">
         <v>0</v>
       </c>
       <c r="I45" s="158">
-        <v>45778</v>
+        <v>45789</v>
       </c>
       <c r="J45" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K45" s="158">
-        <v>45870</v>
+        <v>45789</v>
       </c>
       <c r="L45" s="158"/>
       <c r="N45" s="3"/>
       <c r="P45" s="3">
-        <v>2700</v>
+        <v>2616.61</v>
       </c>
       <c r="Q45" s="3">
         <f>E45*P45</f>
-        <v>13500</v>
+        <v>18316.27</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="D46" s="159" t="s">
-        <v>86</v>
+        <v>264</v>
       </c>
       <c r="E46" s="2">
-        <v>7</v>
+        <v>320</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H46" s="2">
         <v>0</v>
       </c>
       <c r="I46" s="158">
-        <v>45789</v>
+        <v>45870</v>
       </c>
       <c r="J46" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K46" s="158">
-        <v>45789</v>
+        <f>I46+65</f>
+        <v>45935</v>
       </c>
       <c r="L46" s="158"/>
-      <c r="N46" s="3"/>
-      <c r="P46" s="3">
-        <v>2616.61</v>
-      </c>
-      <c r="Q46" s="3">
-        <f>E46*P46</f>
-        <v>18316.27</v>
+      <c r="M46" s="155">
+        <v>505</v>
+      </c>
+      <c r="N46" s="3">
+        <f>M46*E46</f>
+        <v>161600</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D47" s="159" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E47" s="2">
-        <v>320</v>
+        <v>5</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H47" s="2">
         <v>0</v>
       </c>
       <c r="I47" s="158">
+        <v>45778</v>
+      </c>
+      <c r="J47" s="2">
+        <v>4</v>
+      </c>
+      <c r="K47" s="158">
         <v>45870</v>
       </c>
-      <c r="J47" s="2">
-        <v>1</v>
-      </c>
-      <c r="K47" s="158">
-        <f t="shared" ref="K47:K52" si="4">I47+65</f>
-        <v>45935</v>
-      </c>
       <c r="L47" s="158"/>
-      <c r="M47" s="155">
-        <v>505</v>
-      </c>
-      <c r="N47" s="3">
-        <f t="shared" ref="N47:N57" si="5">M47*E47</f>
-        <v>161600</v>
+      <c r="N47" s="3"/>
+      <c r="P47" s="3">
+        <v>2700</v>
+      </c>
+      <c r="Q47" s="3">
+        <f>E47*P47</f>
+        <v>13500</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
@@ -6965,7 +6984,7 @@
         <v>1</v>
       </c>
       <c r="K48" s="158">
-        <f t="shared" si="4"/>
+        <f>I48+65</f>
         <v>45966</v>
       </c>
       <c r="L48" s="155">
@@ -6976,7 +6995,7 @@
         <v>476.20799999999997</v>
       </c>
       <c r="N48" s="3">
-        <f t="shared" si="5"/>
+        <f>M48*E48</f>
         <v>152386.56</v>
       </c>
     </row>
@@ -7012,7 +7031,7 @@
         <v>1</v>
       </c>
       <c r="K49" s="158">
-        <f t="shared" si="4"/>
+        <f>I49+65</f>
         <v>45996</v>
       </c>
       <c r="L49" s="155">
@@ -7023,7 +7042,7 @@
         <v>476.20799999999997</v>
       </c>
       <c r="N49" s="3">
-        <f t="shared" si="5"/>
+        <f>M49*E49</f>
         <v>152386.56</v>
       </c>
     </row>
@@ -7059,7 +7078,7 @@
         <v>1</v>
       </c>
       <c r="K50" s="158">
-        <f t="shared" si="4"/>
+        <f>I50+65</f>
         <v>45966</v>
       </c>
       <c r="L50" s="155">
@@ -7070,7 +7089,7 @@
         <v>476.20799999999997</v>
       </c>
       <c r="N50" s="3">
-        <f t="shared" si="5"/>
+        <f>M50*E50</f>
         <v>152386.56</v>
       </c>
     </row>
@@ -7106,7 +7125,7 @@
         <v>1</v>
       </c>
       <c r="K51" s="158">
-        <f t="shared" si="4"/>
+        <f>I51+65</f>
         <v>45996</v>
       </c>
       <c r="L51" s="155">
@@ -7117,7 +7136,7 @@
         <v>476.20799999999997</v>
       </c>
       <c r="N51" s="3">
-        <f t="shared" si="5"/>
+        <f>M51*E51</f>
         <v>152386.56</v>
       </c>
     </row>
@@ -7153,7 +7172,7 @@
         <v>1</v>
       </c>
       <c r="K52" s="158">
-        <f t="shared" si="4"/>
+        <f>I52+65</f>
         <v>46119</v>
       </c>
       <c r="L52" s="155">
@@ -7164,7 +7183,7 @@
         <v>476.20799999999997</v>
       </c>
       <c r="N52" s="3">
-        <f t="shared" si="5"/>
+        <f>M52*E52</f>
         <v>152386.56</v>
       </c>
     </row>
@@ -7206,7 +7225,7 @@
         <v>488</v>
       </c>
       <c r="N53" s="3">
-        <f t="shared" si="5"/>
+        <f>M53*E53</f>
         <v>156160</v>
       </c>
     </row>
@@ -7248,22 +7267,22 @@
         <v>500</v>
       </c>
       <c r="N54" s="3">
-        <f t="shared" si="5"/>
+        <f>M54*E54</f>
         <v>160000</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D55" s="159" t="s">
-        <v>264</v>
+        <v>19</v>
       </c>
       <c r="E55" s="2">
         <v>320</v>
@@ -7272,45 +7291,41 @@
         <v>27</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H55" s="2">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="I55" s="158">
-        <v>45901</v>
+        <v>46327</v>
       </c>
       <c r="J55" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K55" s="158">
-        <f>I55+65</f>
-        <v>45966</v>
-      </c>
-      <c r="L55" s="155">
-        <v>325</v>
+        <f>I55+120</f>
+        <v>46447</v>
       </c>
       <c r="M55" s="155">
-        <f>(L55+H55)*1.3228</f>
-        <v>466.94839999999999</v>
+        <v>423</v>
       </c>
       <c r="N55" s="3">
-        <f t="shared" si="5"/>
-        <v>149423.48800000001</v>
+        <f>M55*E55</f>
+        <v>135360</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D56" s="159" t="s">
-        <v>264</v>
+        <v>19</v>
       </c>
       <c r="E56" s="2">
         <v>320</v>
@@ -7319,31 +7334,27 @@
         <v>27</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>37</v>
+        <v>289</v>
       </c>
       <c r="H56" s="2">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="I56" s="158">
-        <v>45962</v>
+        <v>46327</v>
       </c>
       <c r="J56" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K56" s="158">
-        <f>I56+65</f>
-        <v>46027</v>
-      </c>
-      <c r="L56" s="155">
-        <v>325</v>
+        <f>I56+120</f>
+        <v>46447</v>
       </c>
       <c r="M56" s="155">
-        <f>(L56+H56)*1.3228</f>
-        <v>466.94839999999999</v>
+        <v>436</v>
       </c>
       <c r="N56" s="3">
-        <f t="shared" si="5"/>
-        <v>149423.48800000001</v>
+        <f>M56*E56</f>
+        <v>139520</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
@@ -7351,7 +7362,7 @@
         <v>2025</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>42</v>
@@ -7372,14 +7383,14 @@
         <v>28</v>
       </c>
       <c r="I57" s="158">
-        <v>46023</v>
+        <v>45901</v>
       </c>
       <c r="J57" s="2">
         <v>1</v>
       </c>
       <c r="K57" s="158">
         <f>I57+65</f>
-        <v>46088</v>
+        <v>45966</v>
       </c>
       <c r="L57" s="155">
         <v>325</v>
@@ -7389,7 +7400,7 @@
         <v>466.94839999999999</v>
       </c>
       <c r="N57" s="3">
-        <f t="shared" si="5"/>
+        <f>M57*E57</f>
         <v>149423.48800000001</v>
       </c>
     </row>
@@ -7397,127 +7408,141 @@
       <c r="A58" s="2">
         <v>2025</v>
       </c>
+      <c r="B58" s="2" t="s">
+        <v>284</v>
+      </c>
       <c r="C58" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="D58" s="159" t="s">
-        <v>331</v>
+        <v>264</v>
       </c>
       <c r="E58" s="2">
-        <v>4000</v>
+        <v>320</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="H58" s="2">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="I58" s="158">
-        <v>45992</v>
+        <v>45962</v>
       </c>
       <c r="J58" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K58" s="158">
-        <v>45992</v>
-      </c>
-      <c r="L58" s="158"/>
-      <c r="N58" s="3"/>
-      <c r="P58" s="3">
-        <v>1600</v>
-      </c>
-      <c r="Q58" s="3">
-        <f>E58*P58</f>
-        <v>6400000</v>
+        <f>I58+65</f>
+        <v>46027</v>
+      </c>
+      <c r="L58" s="155">
+        <v>325</v>
+      </c>
+      <c r="M58" s="155">
+        <f>(L58+H58)*1.3228</f>
+        <v>466.94839999999999</v>
+      </c>
+      <c r="N58" s="3">
+        <f>M58*E58</f>
+        <v>149423.48800000001</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>2025</v>
       </c>
+      <c r="B59" s="2" t="s">
+        <v>285</v>
+      </c>
       <c r="C59" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D59" s="159" t="s">
-        <v>331</v>
+        <v>264</v>
       </c>
       <c r="E59" s="2">
-        <v>2500</v>
+        <v>320</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="H59" s="2">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="I59" s="158">
-        <v>45992</v>
+        <v>46023</v>
       </c>
       <c r="J59" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K59" s="158">
-        <v>45992</v>
+        <f>I59+65</f>
+        <v>46088</v>
       </c>
       <c r="L59" s="155">
         <v>325</v>
       </c>
       <c r="M59" s="155">
-        <f t="shared" ref="M59:M64" si="6">(L59+H59)*1.3228</f>
-        <v>429.90999999999997</v>
+        <f>(L59+H59)*1.3228</f>
+        <v>466.94839999999999</v>
       </c>
       <c r="N59" s="3">
-        <f t="shared" ref="N59:N66" si="7">M59*E59</f>
-        <v>1074775</v>
+        <f>M59*E59</f>
+        <v>149423.48800000001</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>2025</v>
       </c>
+      <c r="B60" s="2" t="s">
+        <v>286</v>
+      </c>
       <c r="C60" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D60" s="159" t="s">
-        <v>331</v>
+        <v>264</v>
       </c>
       <c r="E60" s="2">
-        <v>64.5</v>
+        <v>320</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="H60" s="2">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="I60" s="158">
-        <v>45992</v>
+        <v>46082</v>
       </c>
       <c r="J60" s="2">
         <v>1</v>
       </c>
       <c r="K60" s="158">
-        <v>45992</v>
+        <f>I60+65</f>
+        <v>46147</v>
       </c>
       <c r="L60" s="155">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="M60" s="155">
-        <f t="shared" si="6"/>
-        <v>436.524</v>
+        <f>(L60+H60)*1.3228</f>
+        <v>466.94839999999999</v>
       </c>
       <c r="N60" s="3">
-        <f t="shared" si="7"/>
-        <v>28155.797999999999</v>
+        <f>M60*E60</f>
+        <v>149423.48800000001</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
@@ -7525,7 +7550,7 @@
         <v>2025</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>42</v>
@@ -7537,34 +7562,34 @@
         <v>320</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H61" s="2">
-        <v>28</v>
+        <v>-22</v>
       </c>
       <c r="I61" s="158">
-        <v>46082</v>
+        <v>45992</v>
       </c>
       <c r="J61" s="2">
         <v>1</v>
       </c>
       <c r="K61" s="158">
         <f>I61+65</f>
-        <v>46147</v>
+        <v>46057</v>
       </c>
       <c r="L61" s="155">
         <v>325</v>
       </c>
       <c r="M61" s="155">
-        <f t="shared" si="6"/>
-        <v>466.94839999999999</v>
+        <f>(L61+H61)*1.3228</f>
+        <v>400.80840000000001</v>
       </c>
       <c r="N61" s="3">
-        <f t="shared" si="7"/>
-        <v>149423.48800000001</v>
+        <f>M61*E61</f>
+        <v>128258.68799999999</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
@@ -7572,7 +7597,7 @@
         <v>2025</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>42</v>
@@ -7584,51 +7609,51 @@
         <v>320</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>32</v>
+        <v>290</v>
       </c>
       <c r="H62" s="2">
-        <v>-22</v>
+        <v>53</v>
       </c>
       <c r="I62" s="158">
-        <v>45992</v>
+        <v>45931</v>
       </c>
       <c r="J62" s="2">
         <v>1</v>
       </c>
       <c r="K62" s="158">
         <f>I62+65</f>
-        <v>46057</v>
+        <v>45996</v>
       </c>
       <c r="L62" s="155">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="M62" s="155">
-        <f t="shared" si="6"/>
-        <v>400.80840000000001</v>
+        <f>(L62+H62)*1.3228</f>
+        <v>506.63240000000002</v>
       </c>
       <c r="N62" s="3">
-        <f t="shared" si="7"/>
-        <v>128258.68799999999</v>
+        <f>M62*E62</f>
+        <v>162122.36800000002</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>288</v>
+        <v>346</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D63" s="159" t="s">
-        <v>264</v>
+        <v>349</v>
       </c>
       <c r="E63" s="2">
-        <v>320</v>
+        <v>0.5</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>27</v>
@@ -7637,171 +7662,295 @@
         <v>290</v>
       </c>
       <c r="H63" s="2">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="I63" s="158">
-        <v>45931</v>
+        <v>45809</v>
       </c>
       <c r="J63" s="2">
         <v>1</v>
       </c>
       <c r="K63" s="158">
-        <f>I63+65</f>
-        <v>45996</v>
-      </c>
-      <c r="L63" s="155">
-        <v>330</v>
-      </c>
-      <c r="M63" s="155">
-        <f t="shared" si="6"/>
-        <v>506.63240000000002</v>
-      </c>
-      <c r="N63" s="3">
-        <f t="shared" si="7"/>
-        <v>162122.36800000002</v>
+        <v>45809</v>
+      </c>
+      <c r="L63" s="155"/>
+      <c r="M63" s="155"/>
+      <c r="N63" s="3"/>
+      <c r="P63" s="3">
+        <v>3000</v>
+      </c>
+      <c r="Q63" s="3">
+        <f>E63*P63</f>
+        <v>1500</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>2025</v>
       </c>
+      <c r="B64" s="2" t="s">
+        <v>347</v>
+      </c>
       <c r="C64" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D64" s="159" t="s">
-        <v>331</v>
+        <v>350</v>
       </c>
       <c r="E64" s="2">
-        <v>449</v>
+        <v>320</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H64" s="2">
         <v>0</v>
       </c>
       <c r="I64" s="158">
-        <v>46082</v>
+        <v>45931</v>
       </c>
       <c r="J64" s="2">
         <v>1</v>
       </c>
       <c r="K64" s="158">
-        <v>46082</v>
-      </c>
-      <c r="L64" s="155">
-        <v>325</v>
-      </c>
+        <v>45931</v>
+      </c>
+      <c r="L64" s="155"/>
       <c r="M64" s="155">
-        <f t="shared" si="6"/>
-        <v>429.90999999999997</v>
+        <v>463.2</v>
       </c>
       <c r="N64" s="3">
-        <f t="shared" si="7"/>
-        <v>193029.59</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+        <f>M64*E64</f>
+        <v>148224</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>281</v>
+        <v>348</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D65" s="159" t="s">
-        <v>19</v>
+        <v>351</v>
       </c>
       <c r="E65" s="2">
-        <v>320</v>
+        <v>12</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H65" s="2">
         <v>0</v>
       </c>
       <c r="I65" s="158">
-        <v>46327</v>
+        <v>45880</v>
       </c>
       <c r="J65" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K65" s="158">
-        <f>I65+120</f>
-        <v>46447</v>
-      </c>
-      <c r="M65" s="155">
-        <v>423</v>
-      </c>
-      <c r="N65" s="3">
-        <f t="shared" si="7"/>
-        <v>135360</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+        <v>45880</v>
+      </c>
+      <c r="L65" s="155"/>
+      <c r="M65" s="155"/>
+      <c r="N65" s="3"/>
+      <c r="P65" s="3">
+        <v>2350</v>
+      </c>
+      <c r="Q65" s="3">
+        <f>E65*P65</f>
+        <v>28200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>2026</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>282</v>
+        <v>2025</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D66" s="159" t="s">
-        <v>19</v>
+        <v>331</v>
       </c>
       <c r="E66" s="2">
-        <v>320</v>
+        <v>4000</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>289</v>
+        <v>32</v>
       </c>
       <c r="H66" s="2">
         <v>0</v>
       </c>
       <c r="I66" s="158">
-        <v>46327</v>
+        <v>45992</v>
       </c>
       <c r="J66" s="2">
         <v>4</v>
       </c>
       <c r="K66" s="158">
-        <f>I66+120</f>
-        <v>46447</v>
-      </c>
-      <c r="M66" s="155">
-        <v>436</v>
-      </c>
-      <c r="N66" s="3">
-        <f t="shared" si="7"/>
-        <v>139520</v>
+        <v>45992</v>
+      </c>
+      <c r="L66" s="158"/>
+      <c r="N66" s="3"/>
+      <c r="P66" s="3">
+        <v>1600</v>
+      </c>
+      <c r="Q66" s="3">
+        <f>E66*P66</f>
+        <v>6400000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="159" t="s">
+        <v>331</v>
+      </c>
+      <c r="E67" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H67" s="2">
+        <v>0</v>
+      </c>
+      <c r="I67" s="158">
+        <v>45992</v>
+      </c>
+      <c r="J67" s="2">
+        <v>4</v>
+      </c>
+      <c r="K67" s="158">
+        <v>45992</v>
+      </c>
+      <c r="L67" s="155">
+        <v>325</v>
+      </c>
+      <c r="M67" s="155">
+        <f>(L67+H67)*1.3228</f>
+        <v>429.90999999999997</v>
+      </c>
+      <c r="N67" s="3">
+        <f>M67*E67</f>
+        <v>1074775</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" s="159" t="s">
+        <v>331</v>
+      </c>
+      <c r="E68" s="2">
+        <v>64.5</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H68" s="2">
+        <v>0</v>
+      </c>
+      <c r="I68" s="158">
+        <v>45992</v>
+      </c>
+      <c r="J68" s="2">
+        <v>1</v>
+      </c>
+      <c r="K68" s="158">
+        <v>45992</v>
+      </c>
+      <c r="L68" s="155">
+        <v>330</v>
+      </c>
+      <c r="M68" s="155">
+        <f>(L68+H68)*1.3228</f>
+        <v>436.524</v>
+      </c>
+      <c r="N68" s="3">
+        <f>M68*E68</f>
+        <v>28155.797999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A69" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" s="159" t="s">
+        <v>331</v>
+      </c>
+      <c r="E69" s="2">
+        <v>449</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H69" s="2">
+        <v>0</v>
+      </c>
+      <c r="I69" s="158">
+        <v>46082</v>
+      </c>
+      <c r="J69" s="2">
+        <v>1</v>
+      </c>
+      <c r="K69" s="158">
+        <v>46082</v>
+      </c>
+      <c r="L69" s="155">
+        <v>325</v>
+      </c>
+      <c r="M69" s="155">
+        <f>(L69+H69)*1.3228</f>
+        <v>429.90999999999997</v>
+      </c>
+      <c r="N69" s="3">
+        <f>M69*E69</f>
+        <v>193029.59</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q66" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A47:Q63">
-      <sortCondition ref="B1:B66"/>
+  <autoFilter ref="A1:Q69" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q69">
+      <sortCondition ref="B1:B69"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="Q40" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -7809,8 +7958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62549E7F-C2F6-E740-8F49-EDB7C93FB4DD}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adicionado 5 lotes de hedge Z27 a 263
</commit_message>
<xml_diff>
--- a/vendas_cafe_em_reais.xlsx
+++ b/vendas_cafe_em_reais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotocastro/PycharmProjects/Vendas Cafe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062E2DC9-1AE3-8B4B-AA9A-30D22E4DF0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2D4A16-BED4-6447-A560-755CC4CD77C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="940" windowWidth="24960" windowHeight="16540" activeTab="2" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
+    <workbookView xWindow="4440" yWindow="940" windowWidth="24960" windowHeight="16540" activeTab="3" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2 (2)" sheetId="16" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="352">
   <si>
     <t>026/24</t>
   </si>
@@ -7958,7 +7958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62549E7F-C2F6-E740-8F49-EDB7C93FB4DD}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -8137,10 +8137,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435A83C4-FEBA-7F44-BF8C-E9ADE9845E60}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9233,9 +9233,7 @@
       <c r="B26" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C26" s="2">
-        <v>29575268</v>
-      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="213">
         <f t="shared" ref="D26" si="7">283.5*F26</f>
         <v>2268</v>
@@ -9270,9 +9268,7 @@
       <c r="B27" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C27" s="2">
-        <v>29575268</v>
-      </c>
+      <c r="C27" s="2"/>
       <c r="D27" s="213">
         <f t="shared" ref="D27" si="9">283.5*F27</f>
         <v>1417.5</v>
@@ -9296,6 +9292,39 @@
       <c r="L27" s="215">
         <f t="shared" ref="L27" si="10">D27*(G27-H27)*1.3228</f>
         <v>-20438.252099999958</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="213">
+        <f t="shared" ref="D28" si="11">283.5*F28</f>
+        <v>1417.5</v>
+      </c>
+      <c r="E28" s="213"/>
+      <c r="F28" s="155">
+        <v>5</v>
+      </c>
+      <c r="G28" s="155">
+        <v>263</v>
+      </c>
+      <c r="H28" s="155">
+        <f>futuros!B13</f>
+        <v>261.89999999999998</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="162">
+        <v>46710</v>
+      </c>
+      <c r="K28" s="162"/>
+      <c r="L28" s="215">
+        <f t="shared" ref="L28" si="12">D28*(G28-H28)*1.3228</f>
+        <v>2062.5759000000426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualização contrato 070/25 e hedge
</commit_message>
<xml_diff>
--- a/vendas_cafe_em_reais.xlsx
+++ b/vendas_cafe_em_reais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotocastro/PycharmProjects/Vendas Cafe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2D4A16-BED4-6447-A560-755CC4CD77C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A51E11C-0BB0-3644-BBE6-979C70BD724F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="940" windowWidth="24960" windowHeight="16540" activeTab="3" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <sheet name="CashFlow_Edson_Luiz" sheetId="3" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Q$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Q$70</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'VENDA CAFÉ 220125'!$A$3:$Z$61</definedName>
     <definedName name="LITRAGEM" localSheetId="7">#REF!</definedName>
     <definedName name="LITRAGEM" localSheetId="5">#REF!</definedName>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="353">
   <si>
     <t>026/24</t>
   </si>
@@ -1126,6 +1126,9 @@
   </si>
   <si>
     <t>Naves Comércio de Café</t>
+  </si>
+  <si>
+    <t>070/25</t>
   </si>
 </sst>
 </file>
@@ -2627,26 +2630,26 @@
       </c>
       <c r="L6" s="177">
         <f>futuros!B3</f>
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="M6" s="177">
         <f>(L6+H6)*1.3228</f>
-        <v>446.77569999999997</v>
+        <v>479.38271999999995</v>
       </c>
       <c r="N6" s="167">
         <f>(E6*(M6+H6))</f>
-        <v>152568.22399999999</v>
+        <v>163002.47039999999</v>
       </c>
       <c r="O6" s="178">
         <v>5.7</v>
       </c>
       <c r="P6" s="167">
         <f t="shared" ref="P6:P16" si="1">M6*O6</f>
-        <v>2546.62149</v>
+        <v>2732.4815039999999</v>
       </c>
       <c r="Q6" s="167">
         <f t="shared" ref="Q6:Q16" si="2">P6*E6</f>
-        <v>814918.87679999997</v>
+        <v>874394.08127999993</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
@@ -2683,26 +2686,26 @@
       </c>
       <c r="L7" s="177">
         <f>L6</f>
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="M7" s="177">
         <f>(L7+H7)*1.3228</f>
-        <v>446.77569999999997</v>
+        <v>479.38271999999995</v>
       </c>
       <c r="N7" s="167">
         <f>(E7*(M7+H7))</f>
-        <v>152568.22399999999</v>
+        <v>163002.47039999999</v>
       </c>
       <c r="O7" s="178">
         <v>5.7</v>
       </c>
       <c r="P7" s="167">
         <f t="shared" si="1"/>
-        <v>2546.62149</v>
+        <v>2732.4815039999999</v>
       </c>
       <c r="Q7" s="167">
         <f t="shared" si="2"/>
-        <v>814918.87679999997</v>
+        <v>874394.08127999993</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
@@ -2739,26 +2742,26 @@
       </c>
       <c r="L8" s="177">
         <f>L7</f>
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="M8" s="177">
         <f>(L8+H8)*1.3228</f>
-        <v>446.77569999999997</v>
+        <v>479.38271999999995</v>
       </c>
       <c r="N8" s="167">
         <f>(E8*(M8+H8))</f>
-        <v>152568.22399999999</v>
+        <v>163002.47039999999</v>
       </c>
       <c r="O8" s="178">
         <v>5.7</v>
       </c>
       <c r="P8" s="167">
         <f t="shared" si="1"/>
-        <v>2546.62149</v>
+        <v>2732.4815039999999</v>
       </c>
       <c r="Q8" s="167">
         <f t="shared" si="2"/>
-        <v>814918.87679999997</v>
+        <v>874394.08127999993</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
@@ -2795,26 +2798,26 @@
       </c>
       <c r="L9" s="177">
         <f>futuros!B3</f>
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="M9" s="177">
         <f>(L9+H9)*1.3228</f>
-        <v>446.77569999999997</v>
+        <v>479.38271999999995</v>
       </c>
       <c r="N9" s="167">
         <f>(E9*(M9+H9))</f>
-        <v>152568.22399999999</v>
+        <v>163002.47039999999</v>
       </c>
       <c r="O9" s="178">
         <v>5.7</v>
       </c>
       <c r="P9" s="167">
         <f t="shared" si="1"/>
-        <v>2546.62149</v>
+        <v>2732.4815039999999</v>
       </c>
       <c r="Q9" s="167">
         <f t="shared" si="2"/>
-        <v>814918.87679999997</v>
+        <v>874394.08127999993</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
@@ -2851,26 +2854,26 @@
       </c>
       <c r="L10" s="177">
         <f>futuros!B4</f>
-        <v>298.55</v>
+        <v>321.25</v>
       </c>
       <c r="M10" s="177">
         <f>(L10+H10)*1.3228</f>
-        <v>434.60594000000003</v>
+        <v>464.63349999999997</v>
       </c>
       <c r="N10" s="167">
         <f>(E10*(M10+H10))</f>
-        <v>148673.9008</v>
+        <v>158282.72</v>
       </c>
       <c r="O10" s="178">
         <v>5.7</v>
       </c>
       <c r="P10" s="167">
         <f t="shared" si="1"/>
-        <v>2477.253858</v>
+        <v>2648.41095</v>
       </c>
       <c r="Q10" s="167">
         <f t="shared" si="2"/>
-        <v>792721.23456000001</v>
+        <v>847491.50399999996</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
@@ -2907,26 +2910,26 @@
       </c>
       <c r="L11" s="177">
         <f>futuros!B3</f>
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="M11" s="177">
         <f t="shared" ref="M11:M16" si="4">(L11+H11)*1.3228</f>
-        <v>444.13009999999997</v>
+        <v>476.73711999999995</v>
       </c>
       <c r="N11" s="167">
         <f t="shared" ref="N11:N16" si="5">(E11*(M11+H11))</f>
-        <v>151081.63199999998</v>
+        <v>161515.87839999999</v>
       </c>
       <c r="O11" s="178">
         <v>5.7</v>
       </c>
       <c r="P11" s="167">
         <f t="shared" si="1"/>
-        <v>2531.5415699999999</v>
+        <v>2717.4015839999997</v>
       </c>
       <c r="Q11" s="167">
         <f t="shared" si="2"/>
-        <v>810093.30239999993</v>
+        <v>869568.50687999988</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
@@ -2963,26 +2966,26 @@
       </c>
       <c r="L12" s="177">
         <f>futuros!B3</f>
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="M12" s="177">
         <f t="shared" si="4"/>
-        <v>444.13009999999997</v>
+        <v>476.73711999999995</v>
       </c>
       <c r="N12" s="167">
         <f t="shared" si="5"/>
-        <v>151081.63199999998</v>
+        <v>161515.87839999999</v>
       </c>
       <c r="O12" s="178">
         <v>5.7</v>
       </c>
       <c r="P12" s="167">
         <f t="shared" si="1"/>
-        <v>2531.5415699999999</v>
+        <v>2717.4015839999997</v>
       </c>
       <c r="Q12" s="167">
         <f t="shared" si="2"/>
-        <v>810093.30239999993</v>
+        <v>869568.50687999988</v>
       </c>
     </row>
     <row r="13" spans="2:20" s="166" customFormat="1" x14ac:dyDescent="0.25">
@@ -3019,26 +3022,26 @@
       </c>
       <c r="L13" s="177">
         <f>futuros!B4</f>
-        <v>298.55</v>
+        <v>321.25</v>
       </c>
       <c r="M13" s="177">
         <f t="shared" si="4"/>
-        <v>431.96034000000003</v>
+        <v>461.98789999999997</v>
       </c>
       <c r="N13" s="167">
         <f t="shared" si="5"/>
-        <v>147187.3088</v>
+        <v>156796.128</v>
       </c>
       <c r="O13" s="178">
         <v>5.7</v>
       </c>
       <c r="P13" s="167">
         <f t="shared" si="1"/>
-        <v>2462.1739380000004</v>
+        <v>2633.3310299999998</v>
       </c>
       <c r="Q13" s="167">
         <f t="shared" si="2"/>
-        <v>787895.66016000009</v>
+        <v>842665.92959999992</v>
       </c>
       <c r="R13" s="163"/>
       <c r="S13" s="163"/>
@@ -3078,26 +3081,26 @@
       </c>
       <c r="L14" s="177">
         <f>futuros!B5</f>
-        <v>293.10000000000002</v>
+        <v>312.95</v>
       </c>
       <c r="M14" s="177">
         <f t="shared" si="4"/>
-        <v>424.75108</v>
+        <v>451.00865999999996</v>
       </c>
       <c r="N14" s="167">
         <f t="shared" si="5"/>
-        <v>144880.3456</v>
+        <v>153282.77119999999</v>
       </c>
       <c r="O14" s="178">
         <v>5.7</v>
       </c>
       <c r="P14" s="167">
         <f t="shared" si="1"/>
-        <v>2421.0811560000002</v>
+        <v>2570.749362</v>
       </c>
       <c r="Q14" s="167">
         <f t="shared" si="2"/>
-        <v>774745.96992000006</v>
+        <v>822639.79584000004</v>
       </c>
       <c r="R14" s="163"/>
       <c r="S14" s="163"/>
@@ -3137,26 +3140,26 @@
       </c>
       <c r="L15" s="177">
         <f>futuros!B4</f>
-        <v>298.55</v>
+        <v>321.25</v>
       </c>
       <c r="M15" s="177">
         <f t="shared" si="4"/>
-        <v>365.82033999999999</v>
+        <v>395.84789999999998</v>
       </c>
       <c r="N15" s="167">
         <f t="shared" si="5"/>
-        <v>110022.5088</v>
+        <v>119631.32799999999</v>
       </c>
       <c r="O15" s="178">
         <v>5.7</v>
       </c>
       <c r="P15" s="167">
         <f t="shared" si="1"/>
-        <v>2085.1759379999999</v>
+        <v>2256.3330299999998</v>
       </c>
       <c r="Q15" s="167">
         <f t="shared" si="2"/>
-        <v>667256.30015999998</v>
+        <v>722026.56959999993</v>
       </c>
       <c r="R15" s="163"/>
       <c r="S15" s="163"/>
@@ -3196,26 +3199,26 @@
       </c>
       <c r="L16" s="177">
         <f>futuros!B3</f>
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="M16" s="177">
         <f t="shared" si="4"/>
-        <v>477.20009999999996</v>
+        <v>509.80711999999994</v>
       </c>
       <c r="N16" s="167">
         <f t="shared" si="5"/>
-        <v>169664.03200000001</v>
+        <v>180098.27839999998</v>
       </c>
       <c r="O16" s="178">
         <v>5.7</v>
       </c>
       <c r="P16" s="167">
         <f t="shared" si="1"/>
-        <v>2720.0405699999997</v>
+        <v>2905.9005839999995</v>
       </c>
       <c r="Q16" s="167">
         <f t="shared" si="2"/>
-        <v>870412.98239999986</v>
+        <v>929888.18687999982</v>
       </c>
       <c r="R16" s="163"/>
       <c r="S16" s="163"/>
@@ -3342,20 +3345,20 @@
       <c r="L19" s="179"/>
       <c r="M19" s="182">
         <f>N19/E19</f>
-        <v>471.12148571428571</v>
+        <v>495.73501428571427</v>
       </c>
       <c r="N19" s="183">
         <f>SUM(N5:N18)</f>
-        <v>2110624.2560000001</v>
+        <v>2220892.8640000001</v>
       </c>
       <c r="O19" s="184"/>
       <c r="P19" s="185">
         <f>Q19/E19</f>
-        <v>2566.0996114285713</v>
+        <v>2706.3967242857143</v>
       </c>
       <c r="Q19" s="183">
         <f>SUM(Q5:Q18)</f>
-        <v>11496126.259199999</v>
+        <v>12124657.3248</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
@@ -3478,7 +3481,7 @@
       </c>
       <c r="I25" s="177">
         <f>futuros!B3</f>
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="K25" s="163"/>
       <c r="L25" s="197">
@@ -3487,7 +3490,7 @@
       <c r="M25" s="163"/>
       <c r="N25" s="198">
         <f>(H25-I25)*1.3228*D25</f>
-        <v>-854609.57347499987</v>
+        <v>-1018229.9694839998</v>
       </c>
       <c r="O25" s="178">
         <f>O5</f>
@@ -3495,7 +3498,7 @@
       </c>
       <c r="Q25" s="198">
         <f>N25*O25</f>
-        <v>-4871274.5688074995</v>
+        <v>-5803910.8260587985</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
@@ -3520,7 +3523,7 @@
       </c>
       <c r="I26" s="177">
         <f>I25</f>
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="K26" s="163"/>
       <c r="L26" s="197">
@@ -3529,7 +3532,7 @@
       <c r="M26" s="163"/>
       <c r="N26" s="198">
         <f>(H26-I26)*1.3228*D26</f>
-        <v>-293092.03538999998</v>
+        <v>-357800.66657999996</v>
       </c>
       <c r="O26" s="178">
         <f>O6</f>
@@ -3537,7 +3540,7 @@
       </c>
       <c r="Q26" s="198">
         <f t="shared" ref="Q26:Q27" si="6">N26*O26</f>
-        <v>-1670624.6017229999</v>
+        <v>-2039463.7995059998</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
@@ -3561,7 +3564,7 @@
       </c>
       <c r="I27" s="200">
         <f>I26</f>
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="K27" s="163"/>
       <c r="L27" s="197">
@@ -3570,7 +3573,7 @@
       <c r="M27" s="163"/>
       <c r="N27" s="198">
         <f>(H27-I27)*1.3228*D27</f>
-        <v>-340073.76425400004</v>
+        <v>-438061.1200559999</v>
       </c>
       <c r="O27" s="178">
         <f>O7</f>
@@ -3578,7 +3581,7 @@
       </c>
       <c r="Q27" s="198">
         <f t="shared" si="6"/>
-        <v>-1938420.4562478003</v>
+        <v>-2496948.3843191997</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
@@ -3601,13 +3604,13 @@
       <c r="M28" s="202"/>
       <c r="N28" s="202">
         <f>SUM(N25:N27)</f>
-        <v>-1487775.3731189999</v>
+        <v>-1814091.7561199996</v>
       </c>
       <c r="O28" s="201"/>
       <c r="P28" s="201"/>
       <c r="Q28" s="202">
         <f>SUM(Q25:Q27)</f>
-        <v>-8480319.6267783009</v>
+        <v>-10340323.009883998</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
@@ -4291,7 +4294,7 @@
       </c>
       <c r="I57" s="177">
         <f>futuros!B8</f>
-        <v>276</v>
+        <v>292.55</v>
       </c>
       <c r="K57" s="178">
         <f>O8</f>
@@ -4303,7 +4306,7 @@
       <c r="M57" s="198"/>
       <c r="N57" s="198">
         <f>(H57-I57)*1.3228*D57</f>
-        <v>83703.080160000027</v>
+        <v>27844.774649999999</v>
       </c>
       <c r="O57" s="166">
         <f>O25</f>
@@ -4311,7 +4314,7 @@
       </c>
       <c r="Q57" s="198">
         <f>N57*O57</f>
-        <v>477107.55691200017</v>
+        <v>158715.215505</v>
       </c>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.25">
@@ -4335,7 +4338,7 @@
       </c>
       <c r="I58" s="177">
         <f>I57</f>
-        <v>276</v>
+        <v>292.55</v>
       </c>
       <c r="K58" s="178">
         <f>O9</f>
@@ -4347,7 +4350,7 @@
       <c r="M58" s="198"/>
       <c r="N58" s="198">
         <f>(H58-I58)*1.3228*D58</f>
-        <v>139205.12255999993</v>
+        <v>89553.2954399999</v>
       </c>
       <c r="O58" s="166">
         <f>O26</f>
@@ -4355,7 +4358,7 @@
       </c>
       <c r="Q58" s="198">
         <f>N58*O58</f>
-        <v>793469.19859199959</v>
+        <v>510453.78400799946</v>
       </c>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.25">
@@ -4378,13 +4381,13 @@
       <c r="M59" s="201"/>
       <c r="N59" s="202">
         <f>SUM(N56:N58)</f>
-        <v>222908.20271999994</v>
+        <v>117398.07008999991</v>
       </c>
       <c r="O59" s="201"/>
       <c r="P59" s="201"/>
       <c r="Q59" s="202">
         <f>SUM(Q56:Q58)</f>
-        <v>1270576.7555039998</v>
+        <v>669168.99951299943</v>
       </c>
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.25">
@@ -4522,10 +4525,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T69"/>
+  <dimension ref="A1:T70"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
@@ -7776,41 +7779,45 @@
       <c r="A66" s="2">
         <v>2025</v>
       </c>
+      <c r="B66" s="2" t="s">
+        <v>352</v>
+      </c>
       <c r="C66" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D66" s="159" t="s">
-        <v>331</v>
+        <v>257</v>
       </c>
       <c r="E66" s="2">
-        <v>4000</v>
+        <v>10</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="H66" s="2">
         <v>0</v>
       </c>
       <c r="I66" s="158">
-        <v>45992</v>
+        <v>45887</v>
       </c>
       <c r="J66" s="2">
         <v>4</v>
       </c>
       <c r="K66" s="158">
-        <v>45992</v>
-      </c>
-      <c r="L66" s="158"/>
+        <v>45880</v>
+      </c>
+      <c r="L66" s="155"/>
+      <c r="M66" s="155"/>
       <c r="N66" s="3"/>
       <c r="P66" s="3">
-        <v>1600</v>
+        <v>2250</v>
       </c>
       <c r="Q66" s="3">
         <f>E66*P66</f>
-        <v>6400000</v>
+        <v>22500</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
@@ -7818,13 +7825,14 @@
         <v>2025</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D67" s="159" t="s">
         <v>331</v>
       </c>
       <c r="E67" s="2">
-        <v>2500</v>
+        <f>3000-E66-E65</f>
+        <v>2978</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>32</v>
@@ -7844,16 +7852,14 @@
       <c r="K67" s="158">
         <v>45992</v>
       </c>
-      <c r="L67" s="155">
-        <v>325</v>
-      </c>
-      <c r="M67" s="155">
-        <f>(L67+H67)*1.3228</f>
-        <v>429.90999999999997</v>
-      </c>
-      <c r="N67" s="3">
-        <f>M67*E67</f>
-        <v>1074775</v>
+      <c r="L67" s="158"/>
+      <c r="N67" s="3"/>
+      <c r="P67" s="3">
+        <v>1600</v>
+      </c>
+      <c r="Q67" s="3">
+        <f>E67*P67</f>
+        <v>4764800</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
@@ -7867,7 +7873,8 @@
         <v>331</v>
       </c>
       <c r="E68" s="2">
-        <v>64.5</v>
+        <f>7000-4800-E69-E70</f>
+        <v>1686.5</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>32</v>
@@ -7882,21 +7889,21 @@
         <v>45992</v>
       </c>
       <c r="J68" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K68" s="158">
         <v>45992</v>
       </c>
       <c r="L68" s="155">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="M68" s="155">
         <f>(L68+H68)*1.3228</f>
-        <v>436.524</v>
+        <v>429.90999999999997</v>
       </c>
       <c r="N68" s="3">
         <f>M68*E68</f>
-        <v>28155.797999999999</v>
+        <v>725043.21499999997</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
@@ -7910,7 +7917,7 @@
         <v>331</v>
       </c>
       <c r="E69" s="2">
-        <v>449</v>
+        <v>64.5</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>32</v>
@@ -7922,30 +7929,73 @@
         <v>0</v>
       </c>
       <c r="I69" s="158">
-        <v>46082</v>
+        <v>45992</v>
       </c>
       <c r="J69" s="2">
         <v>1</v>
       </c>
       <c r="K69" s="158">
-        <v>46082</v>
+        <v>45992</v>
       </c>
       <c r="L69" s="155">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="M69" s="155">
         <f>(L69+H69)*1.3228</f>
-        <v>429.90999999999997</v>
+        <v>436.524</v>
       </c>
       <c r="N69" s="3">
         <f>M69*E69</f>
+        <v>28155.797999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A70" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D70" s="159" t="s">
+        <v>331</v>
+      </c>
+      <c r="E70" s="2">
+        <v>449</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H70" s="2">
+        <v>0</v>
+      </c>
+      <c r="I70" s="158">
+        <v>46082</v>
+      </c>
+      <c r="J70" s="2">
+        <v>1</v>
+      </c>
+      <c r="K70" s="158">
+        <v>46082</v>
+      </c>
+      <c r="L70" s="155">
+        <v>325</v>
+      </c>
+      <c r="M70" s="155">
+        <f>(L70+H70)*1.3228</f>
+        <v>429.90999999999997</v>
+      </c>
+      <c r="N70" s="3">
+        <f>M70*E70</f>
         <v>193029.59</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q69" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q69">
-      <sortCondition ref="B1:B69"/>
+  <autoFilter ref="A1:Q70" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q70">
+      <sortCondition ref="B1:B70"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -7982,7 +8032,7 @@
         <v>270</v>
       </c>
       <c r="D1" s="162">
-        <v>45880</v>
+        <v>45887</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7990,11 +8040,11 @@
         <v>45930</v>
       </c>
       <c r="B2" s="155">
-        <v>315</v>
+        <v>340</v>
       </c>
       <c r="C2" s="155">
         <f t="shared" ref="C2:C12" si="0">B2*1.3228</f>
-        <v>416.68200000000002</v>
+        <v>449.75200000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8002,11 +8052,11 @@
         <v>46021</v>
       </c>
       <c r="B3" s="155">
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="C3" s="155">
         <f t="shared" si="0"/>
-        <v>407.0917</v>
+        <v>439.69871999999998</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -8014,11 +8064,11 @@
         <v>46112</v>
       </c>
       <c r="B4" s="155">
-        <v>298.55</v>
+        <v>321.25</v>
       </c>
       <c r="C4" s="155">
         <f t="shared" si="0"/>
-        <v>394.92194000000001</v>
+        <v>424.9495</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -8026,11 +8076,11 @@
         <v>46173</v>
       </c>
       <c r="B5" s="155">
-        <v>293.10000000000002</v>
+        <v>312.95</v>
       </c>
       <c r="C5" s="155">
         <f t="shared" si="0"/>
-        <v>387.71268000000003</v>
+        <v>413.97026</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -8038,11 +8088,11 @@
         <v>46231</v>
       </c>
       <c r="B6" s="155">
-        <v>287.05</v>
+        <v>305.45</v>
       </c>
       <c r="C6" s="155">
         <f t="shared" si="0"/>
-        <v>379.70974000000001</v>
+        <v>404.04926</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -8050,11 +8100,11 @@
         <v>46295</v>
       </c>
       <c r="B7" s="155">
-        <v>280.39999999999998</v>
+        <v>297.39999999999998</v>
       </c>
       <c r="C7" s="155">
         <f t="shared" si="0"/>
-        <v>370.91311999999994</v>
+        <v>393.40071999999998</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -8062,11 +8112,11 @@
         <v>46386</v>
       </c>
       <c r="B8" s="155">
-        <v>276</v>
+        <v>292.55</v>
       </c>
       <c r="C8" s="155">
         <f t="shared" si="0"/>
-        <v>365.09280000000001</v>
+        <v>386.98514</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8074,11 +8124,11 @@
         <v>46477</v>
       </c>
       <c r="B9" s="155">
-        <v>274.2</v>
+        <v>289.5</v>
       </c>
       <c r="C9" s="155">
         <f t="shared" si="0"/>
-        <v>362.71175999999997</v>
+        <v>382.95060000000001</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -8086,11 +8136,11 @@
         <v>46538</v>
       </c>
       <c r="B10" s="155">
-        <v>265.89999999999998</v>
+        <v>286.35000000000002</v>
       </c>
       <c r="C10" s="155">
         <f t="shared" si="0"/>
-        <v>351.73251999999997</v>
+        <v>378.78378000000004</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -8098,11 +8148,11 @@
         <v>46596</v>
       </c>
       <c r="B11" s="155">
-        <v>265.8</v>
+        <v>282.89999999999998</v>
       </c>
       <c r="C11" s="155">
         <f t="shared" si="0"/>
-        <v>351.60023999999999</v>
+        <v>374.22011999999995</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -8110,11 +8160,11 @@
         <v>46660</v>
       </c>
       <c r="B12" s="155">
-        <v>263.8</v>
+        <v>279.10000000000002</v>
       </c>
       <c r="C12" s="155">
         <f t="shared" si="0"/>
-        <v>348.95463999999998</v>
+        <v>369.19348000000002</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -8122,11 +8172,11 @@
         <v>46751</v>
       </c>
       <c r="B13" s="155">
-        <v>261.89999999999998</v>
+        <v>275.75</v>
       </c>
       <c r="C13" s="155">
         <f>B13*1.3228</f>
-        <v>346.44131999999996</v>
+        <v>364.76209999999998</v>
       </c>
     </row>
   </sheetData>
@@ -8140,7 +8190,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8868,7 +8918,7 @@
       </c>
       <c r="H16" s="155">
         <f>futuros!B3</f>
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="162">
@@ -8877,7 +8927,7 @@
       <c r="K16" s="162"/>
       <c r="L16" s="215">
         <f t="shared" si="2"/>
-        <v>-854609.57347499998</v>
+        <v>-1018229.9694839999</v>
       </c>
       <c r="M16" s="160"/>
       <c r="N16" s="215"/>
@@ -8906,7 +8956,7 @@
       </c>
       <c r="H17" s="155">
         <f>futuros!B3</f>
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="162">
@@ -8915,7 +8965,7 @@
       <c r="K17" s="162"/>
       <c r="L17" s="215">
         <f t="shared" si="2"/>
-        <v>-293092.03539000003</v>
+        <v>-357800.66657999996</v>
       </c>
       <c r="M17" s="160"/>
       <c r="N17" s="215"/>
@@ -8946,7 +8996,7 @@
       </c>
       <c r="H18" s="155">
         <f>futuros!B3</f>
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="162">
@@ -8955,7 +9005,7 @@
       <c r="K18" s="162"/>
       <c r="L18" s="215">
         <f t="shared" si="2"/>
-        <v>58408.39935</v>
+        <v>-6300.2318399999403</v>
       </c>
       <c r="M18" s="160"/>
       <c r="N18" s="215"/>
@@ -8984,7 +9034,7 @@
       </c>
       <c r="H19" s="217">
         <f>futuros!B3</f>
-        <v>307.75</v>
+        <v>332.4</v>
       </c>
       <c r="I19" s="208"/>
       <c r="J19" s="219">
@@ -8993,7 +9043,7 @@
       <c r="K19" s="219"/>
       <c r="L19" s="220">
         <f t="shared" si="2"/>
-        <v>-179661.61130400002</v>
+        <v>-231428.51625599994</v>
       </c>
       <c r="M19" s="218"/>
       <c r="N19" s="220"/>
@@ -9024,7 +9074,7 @@
       </c>
       <c r="H20" s="155">
         <f>futuros!B4</f>
-        <v>298.55</v>
+        <v>321.25</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="162">
@@ -9033,7 +9083,7 @@
       <c r="K20" s="162"/>
       <c r="L20" s="215">
         <f t="shared" si="2"/>
-        <v>69433.805069999973</v>
+        <v>9844.1122500000001</v>
       </c>
       <c r="M20" s="160"/>
       <c r="N20" s="215"/>
@@ -9062,7 +9112,7 @@
       </c>
       <c r="H21" s="155">
         <f>futuros!B8</f>
-        <v>276</v>
+        <v>292.55</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="162">
@@ -9071,7 +9121,7 @@
       <c r="K21" s="162"/>
       <c r="L21" s="215">
         <f t="shared" si="2"/>
-        <v>83703.080160000027</v>
+        <v>27844.774649999999</v>
       </c>
       <c r="M21" s="160"/>
       <c r="N21" s="215"/>
@@ -9099,7 +9149,7 @@
       </c>
       <c r="H22" s="155">
         <f>futuros!B8</f>
-        <v>276</v>
+        <v>292.55</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="162">
@@ -9108,7 +9158,7 @@
       <c r="K22" s="162"/>
       <c r="L22" s="215">
         <f t="shared" si="2"/>
-        <v>139205.12255999993</v>
+        <v>89553.295439999885</v>
       </c>
       <c r="M22" s="160"/>
       <c r="N22" s="215"/>
@@ -9136,7 +9186,7 @@
       </c>
       <c r="H23" s="155">
         <f>futuros!B8</f>
-        <v>276</v>
+        <v>292.55</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="162">
@@ -9145,7 +9195,7 @@
       <c r="K23" s="162"/>
       <c r="L23" s="215">
         <f t="shared" si="2"/>
-        <v>93603.444479999962</v>
+        <v>43951.617359999931</v>
       </c>
       <c r="M23" s="160"/>
       <c r="N23" s="215"/>
@@ -9174,7 +9224,7 @@
       </c>
       <c r="H24" s="217">
         <f>futuros!B8</f>
-        <v>276</v>
+        <v>292.55</v>
       </c>
       <c r="I24" s="208"/>
       <c r="J24" s="219">
@@ -9183,7 +9233,7 @@
       <c r="K24" s="219"/>
       <c r="L24" s="220">
         <f t="shared" si="2"/>
-        <v>126004.63679999999</v>
+        <v>-47776.758120000115</v>
       </c>
       <c r="M24" s="218"/>
       <c r="N24" s="220"/>
@@ -9212,7 +9262,7 @@
       </c>
       <c r="H25" s="155">
         <f>futuros!B13</f>
-        <v>261.89999999999998</v>
+        <v>275.75</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="162">
@@ -9221,7 +9271,7 @@
       <c r="K25" s="162"/>
       <c r="L25" s="215">
         <f t="shared" si="2"/>
-        <v>-53214.458219999906</v>
+        <v>-110347.81065</v>
       </c>
       <c r="M25" s="160"/>
       <c r="N25" s="215"/>
@@ -9247,7 +9297,7 @@
       </c>
       <c r="H26" s="155">
         <f>futuros!B13</f>
-        <v>261.89999999999998</v>
+        <v>275.75</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="162">
@@ -9256,7 +9306,7 @@
       <c r="K26" s="162"/>
       <c r="L26" s="215">
         <f t="shared" ref="L26" si="8">D26*(G26-H26)*1.3228</f>
-        <v>-80702.969759999934</v>
+        <v>-122254.4988</v>
       </c>
       <c r="M26" s="160"/>
       <c r="N26" s="215"/>
@@ -9282,7 +9332,7 @@
       </c>
       <c r="H27" s="155">
         <f>futuros!B13</f>
-        <v>261.89999999999998</v>
+        <v>275.75</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="162">
@@ -9291,7 +9341,7 @@
       <c r="K27" s="162"/>
       <c r="L27" s="215">
         <f t="shared" ref="L27" si="10">D27*(G27-H27)*1.3228</f>
-        <v>-20438.252099999958</v>
+        <v>-46407.957750000001</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -9315,7 +9365,7 @@
       </c>
       <c r="H28" s="155">
         <f>futuros!B13</f>
-        <v>261.89999999999998</v>
+        <v>275.75</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="162">
@@ -9324,7 +9374,7 @@
       <c r="K28" s="162"/>
       <c r="L28" s="215">
         <f t="shared" ref="L28" si="12">D28*(G28-H28)*1.3228</f>
-        <v>2062.5759000000426</v>
+        <v>-23907.12975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste do Estoque Exportação de 7.000 sacas para 5.600 sacas
</commit_message>
<xml_diff>
--- a/vendas_cafe_em_reais.xlsx
+++ b/vendas_cafe_em_reais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotocastro/PycharmProjects/Vendas Cafe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6745CE-9AC1-564C-8456-6280606F25EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83F93CE-704F-974E-A6CA-60BE15191B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="940" windowWidth="24960" windowHeight="16700" activeTab="1" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
   </bookViews>
@@ -4528,8 +4528,8 @@
   <dimension ref="A1:T70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E65" sqref="E65:E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -7873,8 +7873,8 @@
         <v>331</v>
       </c>
       <c r="E68" s="2">
-        <f>7000-4800-E69-E70</f>
-        <v>1686.5</v>
+        <f>5600-4800-E69-E70</f>
+        <v>286.5</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>32</v>
@@ -7903,7 +7903,7 @@
       </c>
       <c r="N68" s="3">
         <f>M68*E68</f>
-        <v>725043.21499999997</v>
+        <v>123169.215</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Ajuste estoque do mercado interno para totalizar 30% de 8000 sacas
</commit_message>
<xml_diff>
--- a/vendas_cafe_em_reais.xlsx
+++ b/vendas_cafe_em_reais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotocastro/PycharmProjects/Vendas Cafe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83F93CE-704F-974E-A6CA-60BE15191B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54081BE0-CFD2-C545-9BB8-E56EA28ADED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="940" windowWidth="24960" windowHeight="16700" activeTab="1" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
   </bookViews>
@@ -4529,7 +4529,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E65" sqref="E65:E67"/>
+      <selection pane="bottomLeft" activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -7831,8 +7831,8 @@
         <v>331</v>
       </c>
       <c r="E67" s="2">
-        <f>3000-E66-E65</f>
-        <v>2968</v>
+        <f>2400-E66-E65</f>
+        <v>2368</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>32</v>
@@ -7859,7 +7859,7 @@
       </c>
       <c r="Q67" s="3">
         <f>E67*P67</f>
-        <v>4748800</v>
+        <v>3788800</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
@@ -7873,7 +7873,7 @@
         <v>331</v>
       </c>
       <c r="E68" s="2">
-        <f>5600-4800-E69-E70</f>
+        <f>0.7*8000-4800-E69-E70</f>
         <v>286.5</v>
       </c>
       <c r="F68" s="2" t="s">
@@ -8190,8 +8190,8 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L16" sqref="L16:L28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L16" sqref="L16:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
atualização 15/09 + contrato novo da Emporia
</commit_message>
<xml_diff>
--- a/vendas_cafe_em_reais.xlsx
+++ b/vendas_cafe_em_reais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotocastro/PycharmProjects/Vendas Cafe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C8DACC-49DD-4C4F-B7DF-F8F729991E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7DFB30-69F2-2344-8BFC-B889B5BBBB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="1960" windowWidth="24060" windowHeight="14420" activeTab="3" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
+    <workbookView xWindow="5340" yWindow="1960" windowWidth="24060" windowHeight="14420" activeTab="1" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2 (2)" sheetId="16" state="hidden" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="CashFlow_Edson_Luiz" sheetId="3" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Q$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Q$72</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'VENDA CAFÉ 220125'!$A$3:$Z$61</definedName>
     <definedName name="LITRAGEM" localSheetId="7">#REF!</definedName>
     <definedName name="LITRAGEM" localSheetId="5">#REF!</definedName>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="355">
   <si>
     <t>026/24</t>
   </si>
@@ -1132,6 +1132,9 @@
   </si>
   <si>
     <t>071/25</t>
+  </si>
+  <si>
+    <t>072/25</t>
   </si>
 </sst>
 </file>
@@ -4528,10 +4531,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T71"/>
+  <dimension ref="A1:T72"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
@@ -7872,57 +7875,53 @@
       <c r="A68" s="2">
         <v>2025</v>
       </c>
+      <c r="B68" s="2" t="s">
+        <v>354</v>
+      </c>
       <c r="C68" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="D68" s="159" t="s">
-        <v>331</v>
+        <v>46</v>
       </c>
       <c r="E68" s="2">
-        <f>2400-E66-E65-E67</f>
-        <v>2365</v>
+        <v>320</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>32</v>
+        <v>289</v>
       </c>
       <c r="H68" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I68" s="158">
-        <v>45992</v>
+        <v>45901</v>
       </c>
       <c r="J68" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K68" s="158">
-        <v>45992</v>
-      </c>
-      <c r="L68" s="158"/>
+        <v>45684</v>
+      </c>
+      <c r="L68" s="155"/>
+      <c r="M68" s="155"/>
       <c r="N68" s="3"/>
-      <c r="P68" s="3">
-        <v>1600</v>
-      </c>
-      <c r="Q68" s="3">
-        <f>E68*P68</f>
-        <v>3784000</v>
-      </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>2025</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D69" s="159" t="s">
         <v>331</v>
       </c>
       <c r="E69" s="2">
-        <f>0.7*8000-4800-E70-E71</f>
-        <v>286.5</v>
+        <f>2400-E66-E65-E67</f>
+        <v>2365</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>32</v>
@@ -7942,16 +7941,14 @@
       <c r="K69" s="158">
         <v>45992</v>
       </c>
-      <c r="L69" s="155">
-        <v>325</v>
-      </c>
-      <c r="M69" s="155">
-        <f>(L69+H69)*1.3228</f>
-        <v>429.90999999999997</v>
-      </c>
-      <c r="N69" s="3">
-        <f>M69*E69</f>
-        <v>123169.215</v>
+      <c r="L69" s="158"/>
+      <c r="N69" s="3"/>
+      <c r="P69" s="3">
+        <v>1600</v>
+      </c>
+      <c r="Q69" s="3">
+        <f>E69*P69</f>
+        <v>3784000</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
@@ -7965,7 +7962,8 @@
         <v>331</v>
       </c>
       <c r="E70" s="2">
-        <v>64.5</v>
+        <f>0.7*8000-4800-E71-E72</f>
+        <v>606.5</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>32</v>
@@ -7980,21 +7978,21 @@
         <v>45992</v>
       </c>
       <c r="J70" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K70" s="158">
         <v>45992</v>
       </c>
       <c r="L70" s="155">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="M70" s="155">
         <f>(L70+H70)*1.3228</f>
-        <v>436.524</v>
+        <v>429.90999999999997</v>
       </c>
       <c r="N70" s="3">
         <f>M70*E70</f>
-        <v>28155.797999999999</v>
+        <v>260740.41499999998</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
@@ -8008,7 +8006,7 @@
         <v>331</v>
       </c>
       <c r="E71" s="2">
-        <v>449</v>
+        <v>64.5</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>32</v>
@@ -8020,30 +8018,74 @@
         <v>0</v>
       </c>
       <c r="I71" s="158">
-        <v>46082</v>
+        <v>45992</v>
       </c>
       <c r="J71" s="2">
         <v>1</v>
       </c>
       <c r="K71" s="158">
-        <v>46082</v>
+        <v>45992</v>
       </c>
       <c r="L71" s="155">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="M71" s="155">
         <f>(L71+H71)*1.3228</f>
-        <v>429.90999999999997</v>
+        <v>436.524</v>
       </c>
       <c r="N71" s="3">
         <f>M71*E71</f>
-        <v>193029.59</v>
+        <v>28155.797999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" s="159" t="s">
+        <v>331</v>
+      </c>
+      <c r="E72" s="2">
+        <f>449-E68</f>
+        <v>129</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H72" s="2">
+        <v>0</v>
+      </c>
+      <c r="I72" s="158">
+        <v>46082</v>
+      </c>
+      <c r="J72" s="2">
+        <v>1</v>
+      </c>
+      <c r="K72" s="158">
+        <v>46082</v>
+      </c>
+      <c r="L72" s="155">
+        <v>325</v>
+      </c>
+      <c r="M72" s="155">
+        <f>(L72+H72)*1.3228</f>
+        <v>429.90999999999997</v>
+      </c>
+      <c r="N72" s="3">
+        <f>M72*E72</f>
+        <v>55458.39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q71" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q71">
-      <sortCondition ref="B1:B71"/>
+  <autoFilter ref="A1:Q72" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q72">
+      <sortCondition ref="B1:B72"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -8237,9 +8279,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435A83C4-FEBA-7F44-BF8C-E9ADE9845E60}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L16" sqref="L16:L28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
atualização 15/09 + contrato Emporia
</commit_message>
<xml_diff>
--- a/vendas_cafe_em_reais.xlsx
+++ b/vendas_cafe_em_reais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotocastro/PycharmProjects/Vendas Cafe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7DFB30-69F2-2344-8BFC-B889B5BBBB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6005F70F-2E6C-CE48-8BF1-A0C2BB381C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5340" yWindow="1960" windowWidth="24060" windowHeight="14420" activeTab="1" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
   </bookViews>
@@ -4535,7 +4535,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
+      <selection pane="bottomLeft" activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
atualização contratos 073 e 074, e hedge
</commit_message>
<xml_diff>
--- a/vendas_cafe_em_reais.xlsx
+++ b/vendas_cafe_em_reais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotocastro/PycharmProjects/Vendas Cafe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F275FD-7D55-984B-9CBB-8FFB3D6F06A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC861D1-1A8A-E64A-8CD2-5702AE86FCBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5340" yWindow="1960" windowWidth="24060" windowHeight="14420" activeTab="1" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <sheet name="CashFlow_Edson_Luiz" sheetId="3" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Q$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Q$74</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'VENDA CAFÉ 220125'!$A$3:$Z$61</definedName>
     <definedName name="LITRAGEM" localSheetId="7">#REF!</definedName>
     <definedName name="LITRAGEM" localSheetId="5">#REF!</definedName>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="357">
   <si>
     <t>026/24</t>
   </si>
@@ -1135,6 +1135,12 @@
   </si>
   <si>
     <t>072/25</t>
+  </si>
+  <si>
+    <t>073/25</t>
+  </si>
+  <si>
+    <t>074/25</t>
   </si>
 </sst>
 </file>
@@ -2635,27 +2641,27 @@
         <v>45961</v>
       </c>
       <c r="L6" s="177">
-        <f>futuros!B3</f>
-        <v>416.65</v>
+        <f>futuros!B2</f>
+        <v>365.65</v>
       </c>
       <c r="M6" s="177">
         <f>(L6+H6)*1.3228</f>
-        <v>590.82862</v>
+        <v>523.36581999999999</v>
       </c>
       <c r="N6" s="167">
         <f>(E6*(M6+H6))</f>
-        <v>198665.15840000001</v>
+        <v>177077.0624</v>
       </c>
       <c r="O6" s="178">
         <v>5.7</v>
       </c>
       <c r="P6" s="167">
         <f t="shared" ref="P6:P16" si="1">M6*O6</f>
-        <v>3367.7231340000003</v>
+        <v>2983.1851740000002</v>
       </c>
       <c r="Q6" s="167">
         <f t="shared" ref="Q6:Q16" si="2">P6*E6</f>
-        <v>1077671.4028800002</v>
+        <v>954619.25568000006</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
@@ -2692,26 +2698,26 @@
       </c>
       <c r="L7" s="177">
         <f>L6</f>
-        <v>416.65</v>
+        <v>365.65</v>
       </c>
       <c r="M7" s="177">
         <f>(L7+H7)*1.3228</f>
-        <v>590.82862</v>
+        <v>523.36581999999999</v>
       </c>
       <c r="N7" s="167">
         <f>(E7*(M7+H7))</f>
-        <v>198665.15840000001</v>
+        <v>177077.0624</v>
       </c>
       <c r="O7" s="178">
         <v>5.7</v>
       </c>
       <c r="P7" s="167">
         <f t="shared" si="1"/>
-        <v>3367.7231340000003</v>
+        <v>2983.1851740000002</v>
       </c>
       <c r="Q7" s="167">
         <f t="shared" si="2"/>
-        <v>1077671.4028800002</v>
+        <v>954619.25568000006</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
@@ -2748,26 +2754,26 @@
       </c>
       <c r="L8" s="177">
         <f>L7</f>
-        <v>416.65</v>
+        <v>365.65</v>
       </c>
       <c r="M8" s="177">
         <f>(L8+H8)*1.3228</f>
-        <v>590.82862</v>
+        <v>523.36581999999999</v>
       </c>
       <c r="N8" s="167">
         <f>(E8*(M8+H8))</f>
-        <v>198665.15840000001</v>
+        <v>177077.0624</v>
       </c>
       <c r="O8" s="178">
         <v>5.7</v>
       </c>
       <c r="P8" s="167">
         <f t="shared" si="1"/>
-        <v>3367.7231340000003</v>
+        <v>2983.1851740000002</v>
       </c>
       <c r="Q8" s="167">
         <f t="shared" si="2"/>
-        <v>1077671.4028800002</v>
+        <v>954619.25568000006</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
@@ -2803,27 +2809,27 @@
         <v>46052</v>
       </c>
       <c r="L9" s="177">
-        <f>futuros!B3</f>
-        <v>416.65</v>
+        <f>futuros!B2</f>
+        <v>365.65</v>
       </c>
       <c r="M9" s="177">
         <f>(L9+H9)*1.3228</f>
-        <v>590.82862</v>
+        <v>523.36581999999999</v>
       </c>
       <c r="N9" s="167">
         <f>(E9*(M9+H9))</f>
-        <v>198665.15840000001</v>
+        <v>177077.0624</v>
       </c>
       <c r="O9" s="178">
         <v>5.7</v>
       </c>
       <c r="P9" s="167">
         <f t="shared" si="1"/>
-        <v>3367.7231340000003</v>
+        <v>2983.1851740000002</v>
       </c>
       <c r="Q9" s="167">
         <f t="shared" si="2"/>
-        <v>1077671.4028800002</v>
+        <v>954619.25568000006</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
@@ -2859,27 +2865,27 @@
         <v>46114</v>
       </c>
       <c r="L10" s="177">
-        <f>futuros!B4</f>
-        <v>399.6</v>
+        <f>futuros!B3</f>
+        <v>346.15</v>
       </c>
       <c r="M10" s="177">
         <f>(L10+H10)*1.3228</f>
-        <v>568.27488000000005</v>
+        <v>497.57121999999998</v>
       </c>
       <c r="N10" s="167">
         <f>(E10*(M10+H10))</f>
-        <v>191447.96160000001</v>
+        <v>168822.7904</v>
       </c>
       <c r="O10" s="178">
         <v>5.7</v>
       </c>
       <c r="P10" s="167">
         <f t="shared" si="1"/>
-        <v>3239.1668160000004</v>
+        <v>2836.1559539999998</v>
       </c>
       <c r="Q10" s="167">
         <f t="shared" si="2"/>
-        <v>1036533.3811200002</v>
+        <v>907569.90527999995</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
@@ -2915,27 +2921,27 @@
         <v>45961</v>
       </c>
       <c r="L11" s="177">
-        <f>futuros!B3</f>
-        <v>416.65</v>
+        <f>futuros!B2</f>
+        <v>365.65</v>
       </c>
       <c r="M11" s="177">
         <f t="shared" ref="M11:M16" si="4">(L11+H11)*1.3228</f>
-        <v>588.18301999999994</v>
+        <v>520.72021999999993</v>
       </c>
       <c r="N11" s="167">
         <f t="shared" ref="N11:N16" si="5">(E11*(M11+H11))</f>
-        <v>197178.56639999998</v>
+        <v>175590.47039999999</v>
       </c>
       <c r="O11" s="178">
         <v>5.7</v>
       </c>
       <c r="P11" s="167">
         <f t="shared" si="1"/>
-        <v>3352.6432139999997</v>
+        <v>2968.1052539999996</v>
       </c>
       <c r="Q11" s="167">
         <f t="shared" si="2"/>
-        <v>1072845.8284799999</v>
+        <v>949793.6812799999</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
@@ -2971,27 +2977,27 @@
         <v>46022</v>
       </c>
       <c r="L12" s="177">
-        <f>futuros!B3</f>
-        <v>416.65</v>
+        <f>futuros!B2</f>
+        <v>365.65</v>
       </c>
       <c r="M12" s="177">
         <f t="shared" si="4"/>
-        <v>588.18301999999994</v>
+        <v>520.72021999999993</v>
       </c>
       <c r="N12" s="167">
         <f t="shared" si="5"/>
-        <v>197178.56639999998</v>
+        <v>175590.47039999999</v>
       </c>
       <c r="O12" s="178">
         <v>5.7</v>
       </c>
       <c r="P12" s="167">
         <f t="shared" si="1"/>
-        <v>3352.6432139999997</v>
+        <v>2968.1052539999996</v>
       </c>
       <c r="Q12" s="167">
         <f t="shared" si="2"/>
-        <v>1072845.8284799999</v>
+        <v>949793.6812799999</v>
       </c>
     </row>
     <row r="13" spans="2:20" s="166" customFormat="1" x14ac:dyDescent="0.25">
@@ -3027,27 +3033,27 @@
         <v>46083</v>
       </c>
       <c r="L13" s="177">
-        <f>futuros!B4</f>
-        <v>399.6</v>
+        <f>futuros!B3</f>
+        <v>346.15</v>
       </c>
       <c r="M13" s="177">
         <f t="shared" si="4"/>
-        <v>565.62927999999999</v>
+        <v>494.92561999999998</v>
       </c>
       <c r="N13" s="167">
         <f t="shared" si="5"/>
-        <v>189961.36960000001</v>
+        <v>167336.19839999999</v>
       </c>
       <c r="O13" s="178">
         <v>5.7</v>
       </c>
       <c r="P13" s="167">
         <f t="shared" si="1"/>
-        <v>3224.0868960000003</v>
+        <v>2821.0760340000002</v>
       </c>
       <c r="Q13" s="167">
         <f t="shared" si="2"/>
-        <v>1031707.8067200001</v>
+        <v>902744.33088000002</v>
       </c>
       <c r="R13" s="163"/>
       <c r="S13" s="163"/>
@@ -3086,27 +3092,27 @@
         <v>46142</v>
       </c>
       <c r="L14" s="177">
-        <f>futuros!B5</f>
-        <v>386.15</v>
+        <f>futuros!B4</f>
+        <v>332.15</v>
       </c>
       <c r="M14" s="177">
         <f t="shared" si="4"/>
-        <v>547.83762000000002</v>
+        <v>476.40641999999997</v>
       </c>
       <c r="N14" s="167">
         <f t="shared" si="5"/>
-        <v>184268.03840000002</v>
+        <v>161410.05439999999</v>
       </c>
       <c r="O14" s="178">
         <v>5.7</v>
       </c>
       <c r="P14" s="167">
         <f t="shared" si="1"/>
-        <v>3122.674434</v>
+        <v>2715.5165939999997</v>
       </c>
       <c r="Q14" s="167">
         <f t="shared" si="2"/>
-        <v>999255.81888000004</v>
+        <v>868965.31007999997</v>
       </c>
       <c r="R14" s="163"/>
       <c r="S14" s="163"/>
@@ -3145,27 +3151,27 @@
         <v>46052</v>
       </c>
       <c r="L15" s="177">
-        <f>futuros!B4</f>
-        <v>399.6</v>
+        <f>futuros!B3</f>
+        <v>346.15</v>
       </c>
       <c r="M15" s="177">
         <f t="shared" si="4"/>
-        <v>499.48928000000001</v>
+        <v>428.78561999999994</v>
       </c>
       <c r="N15" s="167">
         <f t="shared" si="5"/>
-        <v>152796.56959999999</v>
+        <v>130171.39839999998</v>
       </c>
       <c r="O15" s="178">
         <v>5.7</v>
       </c>
       <c r="P15" s="167">
         <f t="shared" si="1"/>
-        <v>2847.0888960000002</v>
+        <v>2444.0780339999997</v>
       </c>
       <c r="Q15" s="167">
         <f t="shared" si="2"/>
-        <v>911068.44672000012</v>
+        <v>782104.97087999992</v>
       </c>
       <c r="R15" s="163"/>
       <c r="S15" s="163"/>
@@ -3204,27 +3210,27 @@
         <v>45991</v>
       </c>
       <c r="L16" s="177">
-        <f>futuros!B3</f>
-        <v>416.65</v>
+        <f>futuros!B2</f>
+        <v>365.65</v>
       </c>
       <c r="M16" s="177">
         <f t="shared" si="4"/>
-        <v>621.25301999999999</v>
+        <v>553.79021999999998</v>
       </c>
       <c r="N16" s="167">
         <f t="shared" si="5"/>
-        <v>215760.9664</v>
+        <v>194172.87039999999</v>
       </c>
       <c r="O16" s="178">
         <v>5.7</v>
       </c>
       <c r="P16" s="167">
         <f t="shared" si="1"/>
-        <v>3541.142214</v>
+        <v>3156.6042539999999</v>
       </c>
       <c r="Q16" s="167">
         <f t="shared" si="2"/>
-        <v>1133165.5084800001</v>
+        <v>1010113.36128</v>
       </c>
       <c r="R16" s="163"/>
       <c r="S16" s="163"/>
@@ -3351,20 +3357,20 @@
       <c r="L19" s="179"/>
       <c r="M19" s="182">
         <f>N19/E19</f>
-        <v>580.58318571428572</v>
+        <v>526.59877285714288</v>
       </c>
       <c r="N19" s="183">
         <f>SUM(N5:N18)</f>
-        <v>2601012.6719999998</v>
+        <v>2359162.5024000001</v>
       </c>
       <c r="O19" s="184"/>
       <c r="P19" s="185">
         <f>Q19/E19</f>
-        <v>3190.0313014285712</v>
+        <v>2882.3201481428569</v>
       </c>
       <c r="Q19" s="183">
         <f>SUM(Q5:Q18)</f>
-        <v>14291340.2304</v>
+        <v>12912794.263679998</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
@@ -3486,8 +3492,8 @@
         <v>179</v>
       </c>
       <c r="I25" s="177">
-        <f>futuros!B3</f>
-        <v>416.65</v>
+        <f>futuros!B2</f>
+        <v>365.65</v>
       </c>
       <c r="K25" s="163"/>
       <c r="L25" s="197">
@@ -3496,7 +3502,7 @@
       <c r="M25" s="163"/>
       <c r="N25" s="198">
         <f>(H25-I25)*1.3228*D25</f>
-        <v>-1577459.9233889997</v>
+        <v>-1238934.9661289998</v>
       </c>
       <c r="O25" s="178">
         <f>O5</f>
@@ -3504,7 +3510,7 @@
       </c>
       <c r="Q25" s="198">
         <f>N25*O25</f>
-        <v>-8991521.5633172989</v>
+        <v>-7061929.3069352992</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
@@ -3529,7 +3535,7 @@
       </c>
       <c r="I26" s="177">
         <f>I25</f>
-        <v>416.65</v>
+        <v>365.65</v>
       </c>
       <c r="K26" s="163"/>
       <c r="L26" s="197">
@@ -3538,7 +3544,7 @@
       <c r="M26" s="163"/>
       <c r="N26" s="198">
         <f>(H26-I26)*1.3228*D26</f>
-        <v>-578965.05512999999</v>
+        <v>-445085.12852999999</v>
       </c>
       <c r="O26" s="178">
         <f>O6</f>
@@ -3546,7 +3552,7 @@
       </c>
       <c r="Q26" s="198">
         <f t="shared" ref="Q26:Q27" si="6">N26*O26</f>
-        <v>-3300100.814241</v>
+        <v>-2536985.2326210001</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
@@ -3570,7 +3576,7 @@
       </c>
       <c r="I27" s="200">
         <f>I26</f>
-        <v>416.65</v>
+        <v>365.65</v>
       </c>
       <c r="K27" s="163"/>
       <c r="L27" s="197">
@@ -3579,7 +3585,7 @@
       <c r="M27" s="163"/>
       <c r="N27" s="198">
         <f>(H27-I27)*1.3228*D27</f>
-        <v>-772967.19414599997</v>
+        <v>-570234.73386599997</v>
       </c>
       <c r="O27" s="178">
         <f>O7</f>
@@ -3587,7 +3593,7 @@
       </c>
       <c r="Q27" s="198">
         <f t="shared" si="6"/>
-        <v>-4405913.0066321995</v>
+        <v>-3250337.9830362001</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
@@ -3610,13 +3616,13 @@
       <c r="M28" s="202"/>
       <c r="N28" s="202">
         <f>SUM(N25:N27)</f>
-        <v>-2929392.1726649995</v>
+        <v>-2254254.8285249998</v>
       </c>
       <c r="O28" s="201"/>
       <c r="P28" s="201"/>
       <c r="Q28" s="202">
         <f>SUM(Q25:Q27)</f>
-        <v>-16697535.384190498</v>
+        <v>-12849252.522592498</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
@@ -4299,8 +4305,8 @@
         <v>300.8</v>
       </c>
       <c r="I57" s="177">
-        <f>futuros!B8</f>
-        <v>342.7</v>
+        <f>futuros!B7</f>
+        <v>299.14999999999998</v>
       </c>
       <c r="K57" s="178">
         <f>O8</f>
@@ -4312,7 +4318,7 @@
       <c r="M57" s="198"/>
       <c r="N57" s="198">
         <f>(H57-I57)*1.3228*D57</f>
-        <v>-141417.70397999993</v>
+        <v>5568.9549300001145</v>
       </c>
       <c r="O57" s="166">
         <f>O25</f>
@@ -4320,7 +4326,7 @@
       </c>
       <c r="Q57" s="198">
         <f>N57*O57</f>
-        <v>-806080.91268599965</v>
+        <v>31743.043101000654</v>
       </c>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.25">
@@ -4344,7 +4350,7 @@
       </c>
       <c r="I58" s="177">
         <f>I57</f>
-        <v>342.7</v>
+        <v>299.14999999999998</v>
       </c>
       <c r="K58" s="178">
         <f>O9</f>
@@ -4356,7 +4362,7 @@
       <c r="M58" s="198"/>
       <c r="N58" s="198">
         <f>(H58-I58)*1.3228*D58</f>
-        <v>-60902.241120000035</v>
+        <v>69752.566800000001</v>
       </c>
       <c r="O58" s="166">
         <f>O26</f>
@@ -4364,7 +4370,7 @@
       </c>
       <c r="Q58" s="198">
         <f>N58*O58</f>
-        <v>-347142.77438400022</v>
+        <v>397589.63076000003</v>
       </c>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.25">
@@ -4387,13 +4393,13 @@
       <c r="M59" s="201"/>
       <c r="N59" s="202">
         <f>SUM(N56:N58)</f>
-        <v>-202319.94509999995</v>
+        <v>75321.52173000011</v>
       </c>
       <c r="O59" s="201"/>
       <c r="P59" s="201"/>
       <c r="Q59" s="202">
         <f>SUM(Q56:Q58)</f>
-        <v>-1153223.68707</v>
+        <v>429332.67386100069</v>
       </c>
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.25">
@@ -4531,7 +4537,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T72"/>
+  <dimension ref="A1:T74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
@@ -7884,8 +7890,9 @@
       <c r="D68" s="159" t="s">
         <v>46</v>
       </c>
-      <c r="E68" s="2">
-        <v>320</v>
+      <c r="E68" s="213">
+        <f>20000/60</f>
+        <v>333.33333333333331</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>27</v>
@@ -7913,86 +7920,92 @@
       <c r="A69" s="2">
         <v>2025</v>
       </c>
+      <c r="B69" s="2" t="s">
+        <v>355</v>
+      </c>
       <c r="C69" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D69" s="159" t="s">
-        <v>331</v>
-      </c>
-      <c r="E69" s="2">
-        <f>2400-E66-E65-E67</f>
-        <v>2365</v>
+        <v>24</v>
+      </c>
+      <c r="E69" s="213">
+        <v>5</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="H69" s="2">
         <v>0</v>
       </c>
       <c r="I69" s="158">
-        <v>45992</v>
+        <v>45923</v>
       </c>
       <c r="J69" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K69" s="158">
-        <v>45992</v>
-      </c>
-      <c r="L69" s="158"/>
+        <f>I69+20</f>
+        <v>45943</v>
+      </c>
+      <c r="L69" s="155"/>
+      <c r="M69" s="155"/>
       <c r="N69" s="3"/>
       <c r="P69" s="3">
-        <v>1600</v>
+        <v>2750</v>
       </c>
       <c r="Q69" s="3">
         <f>E69*P69</f>
-        <v>3784000</v>
+        <v>13750</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>2025</v>
       </c>
+      <c r="B70" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="C70" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D70" s="159" t="s">
-        <v>331</v>
-      </c>
-      <c r="E70" s="2">
-        <f>0.7*8000-4800-E71-E72-E68</f>
-        <v>286.5</v>
+        <v>351</v>
+      </c>
+      <c r="E70" s="213">
+        <v>10</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>32</v>
+        <v>290</v>
       </c>
       <c r="H70" s="2">
         <v>0</v>
       </c>
       <c r="I70" s="158">
-        <v>45992</v>
+        <v>45923</v>
       </c>
       <c r="J70" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K70" s="158">
-        <v>45992</v>
-      </c>
-      <c r="L70" s="155">
-        <v>325</v>
-      </c>
-      <c r="M70" s="155">
-        <f>(L70+H70)*1.3228</f>
-        <v>429.90999999999997</v>
-      </c>
-      <c r="N70" s="3">
-        <f>M70*E70</f>
-        <v>123169.215</v>
+        <f>I70+20</f>
+        <v>45943</v>
+      </c>
+      <c r="L70" s="155"/>
+      <c r="M70" s="155"/>
+      <c r="N70" s="3"/>
+      <c r="P70" s="3">
+        <v>3200</v>
+      </c>
+      <c r="Q70" s="3">
+        <f>E70*P70</f>
+        <v>32000</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
@@ -8000,13 +8013,14 @@
         <v>2025</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D71" s="159" t="s">
         <v>331</v>
       </c>
-      <c r="E71" s="2">
-        <v>64.5</v>
+      <c r="E71" s="213">
+        <f>2400-E66-E65-E67-E69-E70</f>
+        <v>2350</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>32</v>
@@ -8021,21 +8035,19 @@
         <v>45992</v>
       </c>
       <c r="J71" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K71" s="158">
         <v>45992</v>
       </c>
-      <c r="L71" s="155">
-        <v>330</v>
-      </c>
-      <c r="M71" s="155">
-        <f>(L71+H71)*1.3228</f>
-        <v>436.524</v>
-      </c>
-      <c r="N71" s="3">
-        <f>M71*E71</f>
-        <v>28155.797999999999</v>
+      <c r="L71" s="158"/>
+      <c r="N71" s="3"/>
+      <c r="P71" s="3">
+        <v>1600</v>
+      </c>
+      <c r="Q71" s="3">
+        <f>E71*P71</f>
+        <v>3760000</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
@@ -8049,8 +8061,8 @@
         <v>331</v>
       </c>
       <c r="E72" s="2">
-        <f>449-E68</f>
-        <v>129</v>
+        <f>0.7*8000-4800-E73-E74-E68</f>
+        <v>286.49999999999994</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>32</v>
@@ -8062,13 +8074,13 @@
         <v>0</v>
       </c>
       <c r="I72" s="158">
-        <v>46082</v>
+        <v>45992</v>
       </c>
       <c r="J72" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K72" s="158">
-        <v>46082</v>
+        <v>45992</v>
       </c>
       <c r="L72" s="155">
         <v>325</v>
@@ -8079,13 +8091,100 @@
       </c>
       <c r="N72" s="3">
         <f>M72*E72</f>
-        <v>55458.39</v>
+        <v>123169.21499999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A73" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D73" s="159" t="s">
+        <v>331</v>
+      </c>
+      <c r="E73" s="2">
+        <v>64.5</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H73" s="2">
+        <v>0</v>
+      </c>
+      <c r="I73" s="158">
+        <v>45992</v>
+      </c>
+      <c r="J73" s="2">
+        <v>1</v>
+      </c>
+      <c r="K73" s="158">
+        <v>45992</v>
+      </c>
+      <c r="L73" s="155">
+        <v>330</v>
+      </c>
+      <c r="M73" s="155">
+        <f>(L73+H73)*1.3228</f>
+        <v>436.524</v>
+      </c>
+      <c r="N73" s="3">
+        <f>M73*E73</f>
+        <v>28155.797999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A74" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74" s="159" t="s">
+        <v>331</v>
+      </c>
+      <c r="E74" s="213">
+        <f>449-E68</f>
+        <v>115.66666666666669</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H74" s="2">
+        <v>0</v>
+      </c>
+      <c r="I74" s="158">
+        <v>46082</v>
+      </c>
+      <c r="J74" s="2">
+        <v>1</v>
+      </c>
+      <c r="K74" s="158">
+        <v>46082</v>
+      </c>
+      <c r="L74" s="155">
+        <v>325</v>
+      </c>
+      <c r="M74" s="155">
+        <f>(L74+H74)*1.3228</f>
+        <v>429.90999999999997</v>
+      </c>
+      <c r="N74" s="3">
+        <f>M74*E74</f>
+        <v>49726.256666666668</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q72" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q72">
-      <sortCondition ref="B1:B72"/>
+  <autoFilter ref="A1:Q74" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q74">
+      <sortCondition ref="B1:B74"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -8096,10 +8195,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62549E7F-C2F6-E740-8F49-EDB7C93FB4DD}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -8122,151 +8221,139 @@
         <v>270</v>
       </c>
       <c r="D1" s="162">
-        <v>45915</v>
+        <v>45922</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="158">
-        <v>45930</v>
+        <v>46021</v>
       </c>
       <c r="B2" s="155">
-        <v>425.15</v>
+        <v>365.65</v>
       </c>
       <c r="C2" s="155">
-        <f t="shared" ref="C2:C12" si="0">B2*1.3228</f>
-        <v>562.38842</v>
+        <f t="shared" ref="C2:C11" si="0">B2*1.3228</f>
+        <v>483.68181999999996</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="158">
-        <v>46021</v>
+        <v>46112</v>
       </c>
       <c r="B3" s="155">
-        <v>416.65</v>
+        <v>346.15</v>
       </c>
       <c r="C3" s="155">
         <f t="shared" si="0"/>
-        <v>551.14461999999992</v>
+        <v>457.88721999999996</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="158">
-        <v>46112</v>
+        <v>46173</v>
       </c>
       <c r="B4" s="155">
-        <v>399.6</v>
+        <v>332.15</v>
       </c>
       <c r="C4" s="155">
         <f t="shared" si="0"/>
-        <v>528.59087999999997</v>
+        <v>439.36801999999994</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="158">
-        <v>46173</v>
+        <v>46231</v>
       </c>
       <c r="B5" s="155">
-        <v>386.15</v>
+        <v>318.75</v>
       </c>
       <c r="C5" s="155">
         <f t="shared" si="0"/>
-        <v>510.79921999999993</v>
+        <v>421.64249999999998</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="158">
-        <v>46231</v>
+        <v>46295</v>
       </c>
       <c r="B6" s="155">
-        <v>371.75</v>
+        <v>308.2</v>
       </c>
       <c r="C6" s="155">
         <f t="shared" si="0"/>
-        <v>491.7509</v>
+        <v>407.68696</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="158">
-        <v>46295</v>
+        <v>46386</v>
       </c>
       <c r="B7" s="155">
-        <v>356.05</v>
+        <v>299.14999999999998</v>
       </c>
       <c r="C7" s="155">
         <f t="shared" si="0"/>
-        <v>470.98293999999999</v>
+        <v>395.71561999999994</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="158">
-        <v>46386</v>
+        <v>46477</v>
       </c>
       <c r="B8" s="155">
-        <v>342.7</v>
+        <v>294</v>
       </c>
       <c r="C8" s="155">
         <f t="shared" si="0"/>
-        <v>453.32355999999999</v>
+        <v>388.90319999999997</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="158">
-        <v>46477</v>
+        <v>46538</v>
       </c>
       <c r="B9" s="155">
-        <v>332.8</v>
+        <v>286.5</v>
       </c>
       <c r="C9" s="155">
         <f t="shared" si="0"/>
-        <v>440.22784000000001</v>
+        <v>378.98219999999998</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="158">
-        <v>46538</v>
+        <v>46596</v>
       </c>
       <c r="B10" s="155">
-        <v>323.64999999999998</v>
+        <v>281</v>
       </c>
       <c r="C10" s="155">
         <f t="shared" si="0"/>
-        <v>428.12421999999998</v>
+        <v>371.70679999999999</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="158">
-        <v>46596</v>
+        <v>46660</v>
       </c>
       <c r="B11" s="155">
-        <v>315</v>
+        <v>274.89999999999998</v>
       </c>
       <c r="C11" s="155">
         <f t="shared" si="0"/>
-        <v>416.68200000000002</v>
+        <v>363.63771999999994</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="158">
-        <v>46660</v>
+        <v>46751</v>
       </c>
       <c r="B12" s="155">
-        <v>305.89999999999998</v>
+        <v>268.89999999999998</v>
       </c>
       <c r="C12" s="155">
-        <f t="shared" si="0"/>
-        <v>404.64451999999994</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="158">
-        <v>46751</v>
-      </c>
-      <c r="B13" s="155">
-        <v>298.14999999999998</v>
-      </c>
-      <c r="C13" s="155">
-        <f>B13*1.3228</f>
-        <v>394.39281999999997</v>
+        <f>B12*1.3228</f>
+        <v>355.70091999999994</v>
       </c>
     </row>
   </sheetData>
@@ -8280,8 +8367,8 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16:D19"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L16" sqref="L16:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9008,8 +9095,8 @@
         <v>179</v>
       </c>
       <c r="H16" s="155">
-        <f>futuros!B3</f>
-        <v>416.65</v>
+        <f>futuros!B2</f>
+        <v>365.65</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="162">
@@ -9018,7 +9105,7 @@
       <c r="K16" s="162"/>
       <c r="L16" s="215">
         <f t="shared" si="2"/>
-        <v>-1577459.9233889999</v>
+        <v>-1238934.9661289998</v>
       </c>
       <c r="M16" s="160"/>
       <c r="N16" s="215"/>
@@ -9046,8 +9133,8 @@
         <v>196.1</v>
       </c>
       <c r="H17" s="155">
-        <f>futuros!B3</f>
-        <v>416.65</v>
+        <f>futuros!B2</f>
+        <v>365.65</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="162">
@@ -9056,7 +9143,7 @@
       <c r="K17" s="162"/>
       <c r="L17" s="215">
         <f t="shared" si="2"/>
-        <v>-578965.05512999999</v>
+        <v>-445085.12852999999</v>
       </c>
       <c r="M17" s="160"/>
       <c r="N17" s="215"/>
@@ -9086,8 +9173,8 @@
         <v>330</v>
       </c>
       <c r="H18" s="155">
-        <f>futuros!B3</f>
-        <v>416.65</v>
+        <f>futuros!B2</f>
+        <v>365.65</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="162">
@@ -9096,7 +9183,7 @@
       <c r="K18" s="162"/>
       <c r="L18" s="215">
         <f t="shared" si="2"/>
-        <v>-227464.62038999994</v>
+        <v>-93584.693789999947</v>
       </c>
       <c r="M18" s="160"/>
       <c r="N18" s="215"/>
@@ -9124,8 +9211,8 @@
         <v>222.2</v>
       </c>
       <c r="H19" s="217">
-        <f>futuros!B3</f>
-        <v>416.65</v>
+        <f>futuros!B2</f>
+        <v>365.65</v>
       </c>
       <c r="I19" s="208"/>
       <c r="J19" s="219">
@@ -9134,7 +9221,7 @@
       <c r="K19" s="219"/>
       <c r="L19" s="220">
         <f t="shared" si="2"/>
-        <v>-408360.02709599992</v>
+        <v>-301256.08581599995</v>
       </c>
       <c r="M19" s="218"/>
       <c r="N19" s="220"/>
@@ -9164,8 +9251,8 @@
         <v>325</v>
       </c>
       <c r="H20" s="155">
-        <f>futuros!B4</f>
-        <v>399.6</v>
+        <f>futuros!B3</f>
+        <v>346.15</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="162">
@@ -9174,7 +9261,7 @@
       <c r="K20" s="162"/>
       <c r="L20" s="215">
         <f t="shared" si="2"/>
-        <v>-195832.20636000004</v>
+        <v>-55520.793089999934</v>
       </c>
       <c r="M20" s="160"/>
       <c r="N20" s="215"/>
@@ -9202,8 +9289,8 @@
         <v>300.8</v>
       </c>
       <c r="H21" s="155">
-        <f>futuros!B8</f>
-        <v>342.7</v>
+        <f>futuros!B7</f>
+        <v>299.14999999999998</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="162">
@@ -9212,7 +9299,7 @@
       <c r="K21" s="162"/>
       <c r="L21" s="215">
         <f t="shared" si="2"/>
-        <v>-141417.70397999993</v>
+        <v>5568.9549300001145</v>
       </c>
       <c r="M21" s="160"/>
       <c r="N21" s="215"/>
@@ -9239,8 +9326,8 @@
         <v>322.39999999999998</v>
       </c>
       <c r="H22" s="155">
-        <f>futuros!B8</f>
-        <v>342.7</v>
+        <f>futuros!B7</f>
+        <v>299.14999999999998</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="162">
@@ -9249,7 +9336,7 @@
       <c r="K22" s="162"/>
       <c r="L22" s="215">
         <f t="shared" si="2"/>
-        <v>-60902.241120000028</v>
+        <v>69752.566800000001</v>
       </c>
       <c r="M22" s="160"/>
       <c r="N22" s="215"/>
@@ -9276,8 +9363,8 @@
         <v>307.2</v>
       </c>
       <c r="H23" s="155">
-        <f>futuros!B8</f>
-        <v>342.7</v>
+        <f>futuros!B7</f>
+        <v>299.14999999999998</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="162">
@@ -9286,7 +9373,7 @@
       <c r="K23" s="162"/>
       <c r="L23" s="215">
         <f t="shared" si="2"/>
-        <v>-106503.9192</v>
+        <v>24150.888720000035</v>
       </c>
       <c r="M23" s="160"/>
       <c r="N23" s="215"/>
@@ -9314,8 +9401,8 @@
         <v>288</v>
       </c>
       <c r="H24" s="217">
-        <f>futuros!B8</f>
-        <v>342.7</v>
+        <f>futuros!B7</f>
+        <v>299.14999999999998</v>
       </c>
       <c r="I24" s="208"/>
       <c r="J24" s="219">
@@ -9324,7 +9411,7 @@
       <c r="K24" s="219"/>
       <c r="L24" s="220">
         <f t="shared" si="2"/>
-        <v>-574371.13607999985</v>
+        <v>-117079.30835999976</v>
       </c>
       <c r="M24" s="218"/>
       <c r="N24" s="220"/>
@@ -9352,8 +9439,8 @@
         <v>249</v>
       </c>
       <c r="H25" s="155">
-        <f>futuros!B13</f>
-        <v>298.14999999999998</v>
+        <f>futuros!B12</f>
+        <v>268.89999999999998</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="162">
@@ -9362,7 +9449,7 @@
       <c r="K25" s="162"/>
       <c r="L25" s="215">
         <f t="shared" si="2"/>
-        <v>-202751.2109699999</v>
+        <v>-82090.520819999903</v>
       </c>
       <c r="M25" s="160"/>
       <c r="N25" s="215"/>
@@ -9387,8 +9474,8 @@
         <v>235</v>
       </c>
       <c r="H26" s="155">
-        <f>futuros!B13</f>
-        <v>298.14999999999998</v>
+        <f>futuros!B12</f>
+        <v>268.89999999999998</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="162">
@@ -9397,7 +9484,7 @@
       <c r="K26" s="162"/>
       <c r="L26" s="215">
         <f t="shared" ref="L26" si="8">D26*(G26-H26)*1.3228</f>
-        <v>-189456.97175999993</v>
+        <v>-101703.74255999994</v>
       </c>
       <c r="M26" s="160"/>
       <c r="N26" s="215"/>
@@ -9422,8 +9509,8 @@
         <v>251</v>
       </c>
       <c r="H27" s="155">
-        <f>futuros!B13</f>
-        <v>298.14999999999998</v>
+        <f>futuros!B12</f>
+        <v>268.89999999999998</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="162">
@@ -9432,7 +9519,7 @@
       <c r="K27" s="162"/>
       <c r="L27" s="215">
         <f t="shared" ref="L27" si="10">D27*(G27-H27)*1.3228</f>
-        <v>-88409.503349999955</v>
+        <v>-33563.735099999954</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -9455,8 +9542,8 @@
         <v>263</v>
       </c>
       <c r="H28" s="155">
-        <f>futuros!B13</f>
-        <v>298.14999999999998</v>
+        <f>futuros!B12</f>
+        <v>268.89999999999998</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="162">
@@ -9465,7 +9552,7 @@
       <c r="K28" s="162"/>
       <c r="L28" s="215">
         <f t="shared" ref="L28" si="12">D28*(G28-H28)*1.3228</f>
-        <v>-65908.675349999961</v>
+        <v>-11062.907099999957</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualização preços 25/09 e contrato 039 emporia
</commit_message>
<xml_diff>
--- a/vendas_cafe_em_reais.xlsx
+++ b/vendas_cafe_em_reais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotocastro/PycharmProjects/Vendas Cafe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC861D1-1A8A-E64A-8CD2-5702AE86FCBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012FEF55-87C4-8444-B308-83C6A4CB2966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="1960" windowWidth="24060" windowHeight="14420" activeTab="1" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
+    <workbookView xWindow="5340" yWindow="1960" windowWidth="24060" windowHeight="14420" activeTab="3" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2 (2)" sheetId="16" state="hidden" r:id="rId1"/>
@@ -2642,26 +2642,26 @@
       </c>
       <c r="L6" s="177">
         <f>futuros!B2</f>
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="M6" s="177">
         <f>(L6+H6)*1.3228</f>
-        <v>523.36581999999999</v>
+        <v>527.26808000000005</v>
       </c>
       <c r="N6" s="167">
         <f>(E6*(M6+H6))</f>
-        <v>177077.0624</v>
+        <v>178325.7856</v>
       </c>
       <c r="O6" s="178">
         <v>5.7</v>
       </c>
       <c r="P6" s="167">
         <f t="shared" ref="P6:P16" si="1">M6*O6</f>
-        <v>2983.1851740000002</v>
+        <v>3005.4280560000002</v>
       </c>
       <c r="Q6" s="167">
         <f t="shared" ref="Q6:Q16" si="2">P6*E6</f>
-        <v>954619.25568000006</v>
+        <v>961736.97792000009</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
@@ -2698,26 +2698,26 @@
       </c>
       <c r="L7" s="177">
         <f>L6</f>
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="M7" s="177">
         <f>(L7+H7)*1.3228</f>
-        <v>523.36581999999999</v>
+        <v>527.26808000000005</v>
       </c>
       <c r="N7" s="167">
         <f>(E7*(M7+H7))</f>
-        <v>177077.0624</v>
+        <v>178325.7856</v>
       </c>
       <c r="O7" s="178">
         <v>5.7</v>
       </c>
       <c r="P7" s="167">
         <f t="shared" si="1"/>
-        <v>2983.1851740000002</v>
+        <v>3005.4280560000002</v>
       </c>
       <c r="Q7" s="167">
         <f t="shared" si="2"/>
-        <v>954619.25568000006</v>
+        <v>961736.97792000009</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
@@ -2754,26 +2754,26 @@
       </c>
       <c r="L8" s="177">
         <f>L7</f>
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="M8" s="177">
         <f>(L8+H8)*1.3228</f>
-        <v>523.36581999999999</v>
+        <v>527.26808000000005</v>
       </c>
       <c r="N8" s="167">
         <f>(E8*(M8+H8))</f>
-        <v>177077.0624</v>
+        <v>178325.7856</v>
       </c>
       <c r="O8" s="178">
         <v>5.7</v>
       </c>
       <c r="P8" s="167">
         <f t="shared" si="1"/>
-        <v>2983.1851740000002</v>
+        <v>3005.4280560000002</v>
       </c>
       <c r="Q8" s="167">
         <f t="shared" si="2"/>
-        <v>954619.25568000006</v>
+        <v>961736.97792000009</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
@@ -2810,26 +2810,26 @@
       </c>
       <c r="L9" s="177">
         <f>futuros!B2</f>
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="M9" s="177">
         <f>(L9+H9)*1.3228</f>
-        <v>523.36581999999999</v>
+        <v>527.26808000000005</v>
       </c>
       <c r="N9" s="167">
         <f>(E9*(M9+H9))</f>
-        <v>177077.0624</v>
+        <v>178325.7856</v>
       </c>
       <c r="O9" s="178">
         <v>5.7</v>
       </c>
       <c r="P9" s="167">
         <f t="shared" si="1"/>
-        <v>2983.1851740000002</v>
+        <v>3005.4280560000002</v>
       </c>
       <c r="Q9" s="167">
         <f t="shared" si="2"/>
-        <v>954619.25568000006</v>
+        <v>961736.97792000009</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
@@ -2866,26 +2866,26 @@
       </c>
       <c r="L10" s="177">
         <f>futuros!B3</f>
-        <v>346.15</v>
+        <v>349.1</v>
       </c>
       <c r="M10" s="177">
         <f>(L10+H10)*1.3228</f>
-        <v>497.57121999999998</v>
+        <v>501.47348</v>
       </c>
       <c r="N10" s="167">
         <f>(E10*(M10+H10))</f>
-        <v>168822.7904</v>
+        <v>170071.51360000001</v>
       </c>
       <c r="O10" s="178">
         <v>5.7</v>
       </c>
       <c r="P10" s="167">
         <f t="shared" si="1"/>
-        <v>2836.1559539999998</v>
+        <v>2858.3988359999998</v>
       </c>
       <c r="Q10" s="167">
         <f t="shared" si="2"/>
-        <v>907569.90527999995</v>
+        <v>914687.62751999998</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
@@ -2922,26 +2922,26 @@
       </c>
       <c r="L11" s="177">
         <f>futuros!B2</f>
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="M11" s="177">
         <f t="shared" ref="M11:M16" si="4">(L11+H11)*1.3228</f>
-        <v>520.72021999999993</v>
+        <v>524.62248</v>
       </c>
       <c r="N11" s="167">
         <f t="shared" ref="N11:N16" si="5">(E11*(M11+H11))</f>
-        <v>175590.47039999999</v>
+        <v>176839.1936</v>
       </c>
       <c r="O11" s="178">
         <v>5.7</v>
       </c>
       <c r="P11" s="167">
         <f t="shared" si="1"/>
-        <v>2968.1052539999996</v>
+        <v>2990.3481360000001</v>
       </c>
       <c r="Q11" s="167">
         <f t="shared" si="2"/>
-        <v>949793.6812799999</v>
+        <v>956911.40352000005</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
@@ -2978,26 +2978,26 @@
       </c>
       <c r="L12" s="177">
         <f>futuros!B2</f>
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="M12" s="177">
         <f t="shared" si="4"/>
-        <v>520.72021999999993</v>
+        <v>524.62248</v>
       </c>
       <c r="N12" s="167">
         <f t="shared" si="5"/>
-        <v>175590.47039999999</v>
+        <v>176839.1936</v>
       </c>
       <c r="O12" s="178">
         <v>5.7</v>
       </c>
       <c r="P12" s="167">
         <f t="shared" si="1"/>
-        <v>2968.1052539999996</v>
+        <v>2990.3481360000001</v>
       </c>
       <c r="Q12" s="167">
         <f t="shared" si="2"/>
-        <v>949793.6812799999</v>
+        <v>956911.40352000005</v>
       </c>
     </row>
     <row r="13" spans="2:20" s="166" customFormat="1" x14ac:dyDescent="0.25">
@@ -3034,26 +3034,26 @@
       </c>
       <c r="L13" s="177">
         <f>futuros!B3</f>
-        <v>346.15</v>
+        <v>349.1</v>
       </c>
       <c r="M13" s="177">
         <f t="shared" si="4"/>
-        <v>494.92561999999998</v>
+        <v>498.82787999999999</v>
       </c>
       <c r="N13" s="167">
         <f t="shared" si="5"/>
-        <v>167336.19839999999</v>
+        <v>168584.9216</v>
       </c>
       <c r="O13" s="178">
         <v>5.7</v>
       </c>
       <c r="P13" s="167">
         <f t="shared" si="1"/>
-        <v>2821.0760340000002</v>
+        <v>2843.3189160000002</v>
       </c>
       <c r="Q13" s="167">
         <f t="shared" si="2"/>
-        <v>902744.33088000002</v>
+        <v>909862.05312000006</v>
       </c>
       <c r="R13" s="163"/>
       <c r="S13" s="163"/>
@@ -3093,26 +3093,26 @@
       </c>
       <c r="L14" s="177">
         <f>futuros!B4</f>
-        <v>332.15</v>
+        <v>335.85</v>
       </c>
       <c r="M14" s="177">
         <f t="shared" si="4"/>
-        <v>476.40641999999997</v>
+        <v>481.30078000000003</v>
       </c>
       <c r="N14" s="167">
         <f t="shared" si="5"/>
-        <v>161410.05439999999</v>
+        <v>162976.24960000001</v>
       </c>
       <c r="O14" s="178">
         <v>5.7</v>
       </c>
       <c r="P14" s="167">
         <f t="shared" si="1"/>
-        <v>2715.5165939999997</v>
+        <v>2743.4144460000002</v>
       </c>
       <c r="Q14" s="167">
         <f t="shared" si="2"/>
-        <v>868965.31007999997</v>
+        <v>877892.6227200001</v>
       </c>
       <c r="R14" s="163"/>
       <c r="S14" s="163"/>
@@ -3152,26 +3152,26 @@
       </c>
       <c r="L15" s="177">
         <f>futuros!B3</f>
-        <v>346.15</v>
+        <v>349.1</v>
       </c>
       <c r="M15" s="177">
         <f t="shared" si="4"/>
-        <v>428.78561999999994</v>
+        <v>432.68788000000001</v>
       </c>
       <c r="N15" s="167">
         <f t="shared" si="5"/>
-        <v>130171.39839999998</v>
+        <v>131420.12160000001</v>
       </c>
       <c r="O15" s="178">
         <v>5.7</v>
       </c>
       <c r="P15" s="167">
         <f t="shared" si="1"/>
-        <v>2444.0780339999997</v>
+        <v>2466.3209160000001</v>
       </c>
       <c r="Q15" s="167">
         <f t="shared" si="2"/>
-        <v>782104.97087999992</v>
+        <v>789222.69312000007</v>
       </c>
       <c r="R15" s="163"/>
       <c r="S15" s="163"/>
@@ -3211,26 +3211,26 @@
       </c>
       <c r="L16" s="177">
         <f>futuros!B2</f>
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="M16" s="177">
         <f t="shared" si="4"/>
-        <v>553.79021999999998</v>
+        <v>557.69248000000005</v>
       </c>
       <c r="N16" s="167">
         <f t="shared" si="5"/>
-        <v>194172.87039999999</v>
+        <v>195421.59360000002</v>
       </c>
       <c r="O16" s="178">
         <v>5.7</v>
       </c>
       <c r="P16" s="167">
         <f t="shared" si="1"/>
-        <v>3156.6042539999999</v>
+        <v>3178.8471360000003</v>
       </c>
       <c r="Q16" s="167">
         <f t="shared" si="2"/>
-        <v>1010113.36128</v>
+        <v>1017231.0835200001</v>
       </c>
       <c r="R16" s="163"/>
       <c r="S16" s="163"/>
@@ -3357,20 +3357,20 @@
       <c r="L19" s="179"/>
       <c r="M19" s="182">
         <f>N19/E19</f>
-        <v>526.59877285714288</v>
+        <v>529.73569857142843</v>
       </c>
       <c r="N19" s="183">
         <f>SUM(N5:N18)</f>
-        <v>2359162.5024000001</v>
+        <v>2373215.9295999995</v>
       </c>
       <c r="O19" s="184"/>
       <c r="P19" s="185">
         <f>Q19/E19</f>
-        <v>2882.3201481428569</v>
+        <v>2900.2006247142858</v>
       </c>
       <c r="Q19" s="183">
         <f>SUM(Q5:Q18)</f>
-        <v>12912794.263679998</v>
+        <v>12992898.79872</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="I25" s="177">
         <f>futuros!B2</f>
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="K25" s="163"/>
       <c r="L25" s="197">
@@ -3502,7 +3502,7 @@
       <c r="M25" s="163"/>
       <c r="N25" s="198">
         <f>(H25-I25)*1.3228*D25</f>
-        <v>-1238934.9661289998</v>
+        <v>-1258516.3116959999</v>
       </c>
       <c r="O25" s="178">
         <f>O5</f>
@@ -3510,7 +3510,7 @@
       </c>
       <c r="Q25" s="198">
         <f>N25*O25</f>
-        <v>-7061929.3069352992</v>
+        <v>-7173542.9766672002</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
@@ -3535,7 +3535,7 @@
       </c>
       <c r="I26" s="177">
         <f>I25</f>
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="K26" s="163"/>
       <c r="L26" s="197">
@@ -3544,7 +3544,7 @@
       <c r="M26" s="163"/>
       <c r="N26" s="198">
         <f>(H26-I26)*1.3228*D26</f>
-        <v>-445085.12852999999</v>
+        <v>-452829.16350000002</v>
       </c>
       <c r="O26" s="178">
         <f>O6</f>
@@ -3552,7 +3552,7 @@
       </c>
       <c r="Q26" s="198">
         <f t="shared" ref="Q26:Q27" si="6">N26*O26</f>
-        <v>-2536985.2326210001</v>
+        <v>-2581126.2319500004</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
@@ -3576,7 +3576,7 @@
       </c>
       <c r="I27" s="200">
         <f>I26</f>
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="K27" s="163"/>
       <c r="L27" s="197">
@@ -3585,7 +3585,7 @@
       <c r="M27" s="163"/>
       <c r="N27" s="198">
         <f>(H27-I27)*1.3228*D27</f>
-        <v>-570234.73386599997</v>
+        <v>-581961.41539200011</v>
       </c>
       <c r="O27" s="178">
         <f>O7</f>
@@ -3593,7 +3593,7 @@
       </c>
       <c r="Q27" s="198">
         <f t="shared" si="6"/>
-        <v>-3250337.9830362001</v>
+        <v>-3317180.0677344007</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
@@ -3616,13 +3616,13 @@
       <c r="M28" s="202"/>
       <c r="N28" s="202">
         <f>SUM(N25:N27)</f>
-        <v>-2254254.8285249998</v>
+        <v>-2293306.890588</v>
       </c>
       <c r="O28" s="201"/>
       <c r="P28" s="201"/>
       <c r="Q28" s="202">
         <f>SUM(Q25:Q27)</f>
-        <v>-12849252.522592498</v>
+        <v>-13071849.276351601</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
@@ -4306,7 +4306,7 @@
       </c>
       <c r="I57" s="177">
         <f>futuros!B7</f>
-        <v>299.14999999999998</v>
+        <v>301.5</v>
       </c>
       <c r="K57" s="178">
         <f>O8</f>
@@ -4318,7 +4318,7 @@
       <c r="M57" s="198"/>
       <c r="N57" s="198">
         <f>(H57-I57)*1.3228*D57</f>
-        <v>5568.9549300001145</v>
+        <v>-2362.5869399999615</v>
       </c>
       <c r="O57" s="166">
         <f>O25</f>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="Q57" s="198">
         <f>N57*O57</f>
-        <v>31743.043101000654</v>
+        <v>-13466.74555799978</v>
       </c>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.25">
@@ -4350,7 +4350,7 @@
       </c>
       <c r="I58" s="177">
         <f>I57</f>
-        <v>299.14999999999998</v>
+        <v>301.5</v>
       </c>
       <c r="K58" s="178">
         <f>O9</f>
@@ -4362,7 +4362,7 @@
       <c r="M58" s="198"/>
       <c r="N58" s="198">
         <f>(H58-I58)*1.3228*D58</f>
-        <v>69752.566800000001</v>
+        <v>62702.307359999933</v>
       </c>
       <c r="O58" s="166">
         <f>O26</f>
@@ -4370,7 +4370,7 @@
       </c>
       <c r="Q58" s="198">
         <f>N58*O58</f>
-        <v>397589.63076000003</v>
+        <v>357403.15195199964</v>
       </c>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.25">
@@ -4393,13 +4393,13 @@
       <c r="M59" s="201"/>
       <c r="N59" s="202">
         <f>SUM(N56:N58)</f>
-        <v>75321.52173000011</v>
+        <v>60339.720419999969</v>
       </c>
       <c r="O59" s="201"/>
       <c r="P59" s="201"/>
       <c r="Q59" s="202">
         <f>SUM(Q56:Q58)</f>
-        <v>429332.67386100069</v>
+        <v>343936.40639399987</v>
       </c>
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.25">
@@ -4539,9 +4539,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+      <selection pane="bottomLeft" activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -6472,7 +6472,17 @@
         <f>M36*E36</f>
         <v>132160</v>
       </c>
-      <c r="O36" s="160"/>
+      <c r="O36" s="160">
+        <v>5.3368000000000002</v>
+      </c>
+      <c r="P36" s="3">
+        <f>M36*O36</f>
+        <v>2204.0984000000003</v>
+      </c>
+      <c r="Q36" s="3">
+        <f>P36*E36</f>
+        <v>705311.48800000013</v>
+      </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
@@ -8190,6 +8200,9 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="Q32" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -8221,7 +8234,7 @@
         <v>270</v>
       </c>
       <c r="D1" s="162">
-        <v>45922</v>
+        <v>45925</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8229,11 +8242,11 @@
         <v>46021</v>
       </c>
       <c r="B2" s="155">
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="C2" s="155">
         <f t="shared" ref="C2:C11" si="0">B2*1.3228</f>
-        <v>483.68181999999996</v>
+        <v>487.58408000000003</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8241,11 +8254,11 @@
         <v>46112</v>
       </c>
       <c r="B3" s="155">
-        <v>346.15</v>
+        <v>349.1</v>
       </c>
       <c r="C3" s="155">
         <f t="shared" si="0"/>
-        <v>457.88721999999996</v>
+        <v>461.78948000000003</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -8253,11 +8266,11 @@
         <v>46173</v>
       </c>
       <c r="B4" s="155">
-        <v>332.15</v>
+        <v>335.85</v>
       </c>
       <c r="C4" s="155">
         <f t="shared" si="0"/>
-        <v>439.36801999999994</v>
+        <v>444.26238000000001</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -8265,11 +8278,11 @@
         <v>46231</v>
       </c>
       <c r="B5" s="155">
-        <v>318.75</v>
+        <v>322.7</v>
       </c>
       <c r="C5" s="155">
         <f t="shared" si="0"/>
-        <v>421.64249999999998</v>
+        <v>426.86755999999997</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -8277,11 +8290,11 @@
         <v>46295</v>
       </c>
       <c r="B6" s="155">
-        <v>308.2</v>
+        <v>310.25</v>
       </c>
       <c r="C6" s="155">
         <f t="shared" si="0"/>
-        <v>407.68696</v>
+        <v>410.39870000000002</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -8289,11 +8302,11 @@
         <v>46386</v>
       </c>
       <c r="B7" s="155">
-        <v>299.14999999999998</v>
+        <v>301.5</v>
       </c>
       <c r="C7" s="155">
         <f t="shared" si="0"/>
-        <v>395.71561999999994</v>
+        <v>398.82420000000002</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -8301,11 +8314,11 @@
         <v>46477</v>
       </c>
       <c r="B8" s="155">
-        <v>294</v>
+        <v>298.8</v>
       </c>
       <c r="C8" s="155">
         <f t="shared" si="0"/>
-        <v>388.90319999999997</v>
+        <v>395.25263999999999</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8313,11 +8326,11 @@
         <v>46538</v>
       </c>
       <c r="B9" s="155">
-        <v>286.5</v>
+        <v>292.39999999999998</v>
       </c>
       <c r="C9" s="155">
         <f t="shared" si="0"/>
-        <v>378.98219999999998</v>
+        <v>386.78671999999995</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -8325,11 +8338,11 @@
         <v>46596</v>
       </c>
       <c r="B10" s="155">
-        <v>281</v>
+        <v>287.3</v>
       </c>
       <c r="C10" s="155">
         <f t="shared" si="0"/>
-        <v>371.70679999999999</v>
+        <v>380.04043999999999</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -8337,11 +8350,11 @@
         <v>46660</v>
       </c>
       <c r="B11" s="155">
-        <v>274.89999999999998</v>
+        <v>281.60000000000002</v>
       </c>
       <c r="C11" s="155">
         <f t="shared" si="0"/>
-        <v>363.63771999999994</v>
+        <v>372.50048000000004</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -8349,11 +8362,11 @@
         <v>46751</v>
       </c>
       <c r="B12" s="155">
-        <v>268.89999999999998</v>
+        <v>276.25</v>
       </c>
       <c r="C12" s="155">
         <f>B12*1.3228</f>
-        <v>355.70091999999994</v>
+        <v>365.42349999999999</v>
       </c>
     </row>
   </sheetData>
@@ -8366,8 +8379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435A83C4-FEBA-7F44-BF8C-E9ADE9845E60}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L16" sqref="L16:L28"/>
     </sheetView>
   </sheetViews>
@@ -9096,7 +9109,7 @@
       </c>
       <c r="H16" s="155">
         <f>futuros!B2</f>
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="162">
@@ -9105,7 +9118,7 @@
       <c r="K16" s="162"/>
       <c r="L16" s="215">
         <f t="shared" si="2"/>
-        <v>-1238934.9661289998</v>
+        <v>-1258516.3116960002</v>
       </c>
       <c r="M16" s="160"/>
       <c r="N16" s="215"/>
@@ -9134,7 +9147,7 @@
       </c>
       <c r="H17" s="155">
         <f>futuros!B2</f>
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="162">
@@ -9143,7 +9156,7 @@
       <c r="K17" s="162"/>
       <c r="L17" s="215">
         <f t="shared" si="2"/>
-        <v>-445085.12852999999</v>
+        <v>-452829.16350000008</v>
       </c>
       <c r="M17" s="160"/>
       <c r="N17" s="215"/>
@@ -9174,7 +9187,7 @@
       </c>
       <c r="H18" s="155">
         <f>futuros!B2</f>
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="162">
@@ -9183,7 +9196,7 @@
       <c r="K18" s="162"/>
       <c r="L18" s="215">
         <f t="shared" si="2"/>
-        <v>-93584.693789999947</v>
+        <v>-101328.72876000006</v>
       </c>
       <c r="M18" s="160"/>
       <c r="N18" s="215"/>
@@ -9212,7 +9225,7 @@
       </c>
       <c r="H19" s="217">
         <f>futuros!B2</f>
-        <v>365.65</v>
+        <v>368.6</v>
       </c>
       <c r="I19" s="208"/>
       <c r="J19" s="219">
@@ -9221,7 +9234,7 @@
       <c r="K19" s="219"/>
       <c r="L19" s="220">
         <f t="shared" si="2"/>
-        <v>-301256.08581599995</v>
+        <v>-307451.31379200006</v>
       </c>
       <c r="M19" s="218"/>
       <c r="N19" s="220"/>
@@ -9252,7 +9265,7 @@
       </c>
       <c r="H20" s="155">
         <f>futuros!B3</f>
-        <v>346.15</v>
+        <v>349.1</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="162">
@@ -9261,7 +9274,7 @@
       <c r="K20" s="162"/>
       <c r="L20" s="215">
         <f t="shared" si="2"/>
-        <v>-55520.793089999934</v>
+        <v>-63264.828060000065</v>
       </c>
       <c r="M20" s="160"/>
       <c r="N20" s="215"/>
@@ -9290,7 +9303,7 @@
       </c>
       <c r="H21" s="155">
         <f>futuros!B7</f>
-        <v>299.14999999999998</v>
+        <v>301.5</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="162">
@@ -9299,7 +9312,7 @@
       <c r="K21" s="162"/>
       <c r="L21" s="215">
         <f t="shared" si="2"/>
-        <v>5568.9549300001145</v>
+        <v>-2362.5869399999615</v>
       </c>
       <c r="M21" s="160"/>
       <c r="N21" s="215"/>
@@ -9327,7 +9340,7 @@
       </c>
       <c r="H22" s="155">
         <f>futuros!B7</f>
-        <v>299.14999999999998</v>
+        <v>301.5</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="162">
@@ -9336,7 +9349,7 @@
       <c r="K22" s="162"/>
       <c r="L22" s="215">
         <f t="shared" si="2"/>
-        <v>69752.566800000001</v>
+        <v>62702.307359999926</v>
       </c>
       <c r="M22" s="160"/>
       <c r="N22" s="215"/>
@@ -9364,7 +9377,7 @@
       </c>
       <c r="H23" s="155">
         <f>futuros!B7</f>
-        <v>299.14999999999998</v>
+        <v>301.5</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="162">
@@ -9373,7 +9386,7 @@
       <c r="K23" s="162"/>
       <c r="L23" s="215">
         <f t="shared" si="2"/>
-        <v>24150.888720000035</v>
+        <v>17100.629279999968</v>
       </c>
       <c r="M23" s="160"/>
       <c r="N23" s="215"/>
@@ -9402,7 +9415,7 @@
       </c>
       <c r="H24" s="217">
         <f>futuros!B7</f>
-        <v>299.14999999999998</v>
+        <v>301.5</v>
       </c>
       <c r="I24" s="208"/>
       <c r="J24" s="219">
@@ -9411,7 +9424,7 @@
       <c r="K24" s="219"/>
       <c r="L24" s="220">
         <f t="shared" si="2"/>
-        <v>-117079.30835999976</v>
+        <v>-141755.2164</v>
       </c>
       <c r="M24" s="218"/>
       <c r="N24" s="220"/>
@@ -9440,7 +9453,7 @@
       </c>
       <c r="H25" s="155">
         <f>futuros!B12</f>
-        <v>268.89999999999998</v>
+        <v>276.25</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="162">
@@ -9449,7 +9462,7 @@
       <c r="K25" s="162"/>
       <c r="L25" s="215">
         <f t="shared" si="2"/>
-        <v>-82090.520819999903</v>
+        <v>-112410.38655</v>
       </c>
       <c r="M25" s="160"/>
       <c r="N25" s="215"/>
@@ -9475,7 +9488,7 @@
       </c>
       <c r="H26" s="155">
         <f>futuros!B12</f>
-        <v>268.89999999999998</v>
+        <v>276.25</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="162">
@@ -9484,7 +9497,7 @@
       <c r="K26" s="162"/>
       <c r="L26" s="215">
         <f t="shared" ref="L26" si="8">D26*(G26-H26)*1.3228</f>
-        <v>-101703.74255999994</v>
+        <v>-123754.554</v>
       </c>
       <c r="M26" s="160"/>
       <c r="N26" s="215"/>
@@ -9510,7 +9523,7 @@
       </c>
       <c r="H27" s="155">
         <f>futuros!B12</f>
-        <v>268.89999999999998</v>
+        <v>276.25</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="162">
@@ -9519,7 +9532,7 @@
       <c r="K27" s="162"/>
       <c r="L27" s="215">
         <f t="shared" ref="L27" si="10">D27*(G27-H27)*1.3228</f>
-        <v>-33563.735099999954</v>
+        <v>-47345.492249999996</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -9543,7 +9556,7 @@
       </c>
       <c r="H28" s="155">
         <f>futuros!B12</f>
-        <v>268.89999999999998</v>
+        <v>276.25</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="162">
@@ -9552,7 +9565,7 @@
       <c r="K28" s="162"/>
       <c r="L28" s="215">
         <f t="shared" ref="L28" si="12">D28*(G28-H28)*1.3228</f>
-        <v>-11062.907099999957</v>
+        <v>-24844.664249999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização dos preços 13/10
</commit_message>
<xml_diff>
--- a/vendas_cafe_em_reais.xlsx
+++ b/vendas_cafe_em_reais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotocastro/PycharmProjects/Vendas Cafe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295E0BDA-1F64-2048-98EF-BE7635F7CBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EC92A2-929A-A142-9A49-02B0535AE982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="680" windowWidth="24980" windowHeight="18440" activeTab="3" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
+    <workbookView xWindow="4420" yWindow="680" windowWidth="24980" windowHeight="18440" activeTab="1" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2 (2)" sheetId="16" state="hidden" r:id="rId1"/>
@@ -2642,26 +2642,26 @@
       </c>
       <c r="L6" s="177">
         <f>futuros!B2</f>
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="M6" s="177">
         <f>(L6+H6)*1.3228</f>
-        <v>550.68164000000002</v>
+        <v>545.91955999999993</v>
       </c>
       <c r="N6" s="167">
         <f>(E6*(M6+H6))</f>
-        <v>185818.12479999999</v>
+        <v>184294.25919999997</v>
       </c>
       <c r="O6" s="178">
         <v>5.7</v>
       </c>
       <c r="P6" s="167">
         <f t="shared" ref="P6:P16" si="1">M6*O6</f>
-        <v>3138.8853480000002</v>
+        <v>3111.7414919999997</v>
       </c>
       <c r="Q6" s="167">
         <f t="shared" ref="Q6:Q16" si="2">P6*E6</f>
-        <v>1004443.3113600001</v>
+        <v>995757.27743999986</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
@@ -2698,26 +2698,26 @@
       </c>
       <c r="L7" s="177">
         <f>L6</f>
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="M7" s="177">
         <f>(L7+H7)*1.3228</f>
-        <v>550.68164000000002</v>
+        <v>545.91955999999993</v>
       </c>
       <c r="N7" s="167">
         <f>(E7*(M7+H7))</f>
-        <v>185818.12479999999</v>
+        <v>184294.25919999997</v>
       </c>
       <c r="O7" s="178">
         <v>5.7</v>
       </c>
       <c r="P7" s="167">
         <f t="shared" si="1"/>
-        <v>3138.8853480000002</v>
+        <v>3111.7414919999997</v>
       </c>
       <c r="Q7" s="167">
         <f t="shared" si="2"/>
-        <v>1004443.3113600001</v>
+        <v>995757.27743999986</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
@@ -2754,26 +2754,26 @@
       </c>
       <c r="L8" s="177">
         <f>L7</f>
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="M8" s="177">
         <f>(L8+H8)*1.3228</f>
-        <v>550.68164000000002</v>
+        <v>545.91955999999993</v>
       </c>
       <c r="N8" s="167">
         <f>(E8*(M8+H8))</f>
-        <v>185818.12479999999</v>
+        <v>184294.25919999997</v>
       </c>
       <c r="O8" s="178">
         <v>5.7</v>
       </c>
       <c r="P8" s="167">
         <f t="shared" si="1"/>
-        <v>3138.8853480000002</v>
+        <v>3111.7414919999997</v>
       </c>
       <c r="Q8" s="167">
         <f t="shared" si="2"/>
-        <v>1004443.3113600001</v>
+        <v>995757.27743999986</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
@@ -2810,26 +2810,26 @@
       </c>
       <c r="L9" s="177">
         <f>futuros!B2</f>
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="M9" s="177">
         <f>(L9+H9)*1.3228</f>
-        <v>550.68164000000002</v>
+        <v>545.91955999999993</v>
       </c>
       <c r="N9" s="167">
         <f>(E9*(M9+H9))</f>
-        <v>185818.12479999999</v>
+        <v>184294.25919999997</v>
       </c>
       <c r="O9" s="178">
         <v>5.7</v>
       </c>
       <c r="P9" s="167">
         <f t="shared" si="1"/>
-        <v>3138.8853480000002</v>
+        <v>3111.7414919999997</v>
       </c>
       <c r="Q9" s="167">
         <f t="shared" si="2"/>
-        <v>1004443.3113600001</v>
+        <v>995757.27743999986</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
@@ -2866,26 +2866,26 @@
       </c>
       <c r="L10" s="177">
         <f>futuros!B3</f>
-        <v>369.85</v>
+        <v>364.55</v>
       </c>
       <c r="M10" s="177">
         <f>(L10+H10)*1.3228</f>
-        <v>528.92158000000006</v>
+        <v>521.91074000000003</v>
       </c>
       <c r="N10" s="167">
         <f>(E10*(M10+H10))</f>
-        <v>178854.90560000003</v>
+        <v>176611.43680000002</v>
       </c>
       <c r="O10" s="178">
         <v>5.7</v>
       </c>
       <c r="P10" s="167">
         <f t="shared" si="1"/>
-        <v>3014.8530060000003</v>
+        <v>2974.8912180000002</v>
       </c>
       <c r="Q10" s="167">
         <f t="shared" si="2"/>
-        <v>964752.96192000015</v>
+        <v>951965.1897600001</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
@@ -2922,26 +2922,26 @@
       </c>
       <c r="L11" s="177">
         <f>futuros!B2</f>
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="M11" s="177">
         <f t="shared" ref="M11:M16" si="4">(L11+H11)*1.3228</f>
-        <v>548.03603999999996</v>
+        <v>543.27395999999999</v>
       </c>
       <c r="N11" s="167">
         <f t="shared" ref="N11:N16" si="5">(E11*(M11+H11))</f>
-        <v>184331.53279999999</v>
+        <v>182807.6672</v>
       </c>
       <c r="O11" s="178">
         <v>5.7</v>
       </c>
       <c r="P11" s="167">
         <f t="shared" si="1"/>
-        <v>3123.8054279999997</v>
+        <v>3096.661572</v>
       </c>
       <c r="Q11" s="167">
         <f t="shared" si="2"/>
-        <v>999617.73695999989</v>
+        <v>990931.70304000005</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
@@ -2978,26 +2978,26 @@
       </c>
       <c r="L12" s="177">
         <f>futuros!B2</f>
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="M12" s="177">
         <f t="shared" si="4"/>
-        <v>548.03603999999996</v>
+        <v>543.27395999999999</v>
       </c>
       <c r="N12" s="167">
         <f t="shared" si="5"/>
-        <v>184331.53279999999</v>
+        <v>182807.6672</v>
       </c>
       <c r="O12" s="178">
         <v>5.7</v>
       </c>
       <c r="P12" s="167">
         <f t="shared" si="1"/>
-        <v>3123.8054279999997</v>
+        <v>3096.661572</v>
       </c>
       <c r="Q12" s="167">
         <f t="shared" si="2"/>
-        <v>999617.73695999989</v>
+        <v>990931.70304000005</v>
       </c>
     </row>
     <row r="13" spans="2:20" s="166" customFormat="1" x14ac:dyDescent="0.25">
@@ -3034,26 +3034,26 @@
       </c>
       <c r="L13" s="177">
         <f>futuros!B3</f>
-        <v>369.85</v>
+        <v>364.55</v>
       </c>
       <c r="M13" s="177">
         <f t="shared" si="4"/>
-        <v>526.27598</v>
+        <v>519.26513999999997</v>
       </c>
       <c r="N13" s="167">
         <f t="shared" si="5"/>
-        <v>177368.31359999999</v>
+        <v>175124.84479999999</v>
       </c>
       <c r="O13" s="178">
         <v>5.7</v>
       </c>
       <c r="P13" s="167">
         <f t="shared" si="1"/>
-        <v>2999.7730860000001</v>
+        <v>2959.8112980000001</v>
       </c>
       <c r="Q13" s="167">
         <f t="shared" si="2"/>
-        <v>959927.38752000011</v>
+        <v>947139.61536000005</v>
       </c>
       <c r="R13" s="163"/>
       <c r="S13" s="163"/>
@@ -3093,26 +3093,26 @@
       </c>
       <c r="L14" s="177">
         <f>futuros!B4</f>
-        <v>358.2</v>
+        <v>351.3</v>
       </c>
       <c r="M14" s="177">
         <f t="shared" si="4"/>
-        <v>510.86535999999995</v>
+        <v>501.73804000000001</v>
       </c>
       <c r="N14" s="167">
         <f t="shared" si="5"/>
-        <v>172436.91519999999</v>
+        <v>169516.1728</v>
       </c>
       <c r="O14" s="178">
         <v>5.7</v>
       </c>
       <c r="P14" s="167">
         <f t="shared" si="1"/>
-        <v>2911.9325519999998</v>
+        <v>2859.9068280000001</v>
       </c>
       <c r="Q14" s="167">
         <f t="shared" si="2"/>
-        <v>931818.41663999995</v>
+        <v>915170.18495999998</v>
       </c>
       <c r="R14" s="163"/>
       <c r="S14" s="163"/>
@@ -3152,26 +3152,26 @@
       </c>
       <c r="L15" s="177">
         <f>futuros!B3</f>
-        <v>369.85</v>
+        <v>364.55</v>
       </c>
       <c r="M15" s="177">
         <f t="shared" si="4"/>
-        <v>460.13598000000002</v>
+        <v>453.12513999999999</v>
       </c>
       <c r="N15" s="167">
         <f t="shared" si="5"/>
-        <v>140203.51360000001</v>
+        <v>137960.0448</v>
       </c>
       <c r="O15" s="178">
         <v>5.7</v>
       </c>
       <c r="P15" s="167">
         <f t="shared" si="1"/>
-        <v>2622.7750860000001</v>
+        <v>2582.813298</v>
       </c>
       <c r="Q15" s="167">
         <f t="shared" si="2"/>
-        <v>839288.02752</v>
+        <v>826500.25536000007</v>
       </c>
       <c r="R15" s="163"/>
       <c r="S15" s="163"/>
@@ -3211,26 +3211,26 @@
       </c>
       <c r="L16" s="177">
         <f>futuros!B2</f>
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="M16" s="177">
         <f t="shared" si="4"/>
-        <v>581.10604000000001</v>
+        <v>576.34395999999992</v>
       </c>
       <c r="N16" s="167">
         <f t="shared" si="5"/>
-        <v>202913.93280000001</v>
+        <v>201390.06719999999</v>
       </c>
       <c r="O16" s="178">
         <v>5.7</v>
       </c>
       <c r="P16" s="167">
         <f t="shared" si="1"/>
-        <v>3312.3044280000004</v>
+        <v>3285.1605719999998</v>
       </c>
       <c r="Q16" s="167">
         <f t="shared" si="2"/>
-        <v>1059937.4169600001</v>
+        <v>1051251.38304</v>
       </c>
       <c r="R16" s="163"/>
       <c r="S16" s="163"/>
@@ -3357,20 +3357,20 @@
       <c r="L19" s="179"/>
       <c r="M19" s="182">
         <f>N19/E19</f>
-        <v>549.43596999999988</v>
+        <v>544.90065571428579</v>
       </c>
       <c r="N19" s="183">
         <f>SUM(N5:N18)</f>
-        <v>2461473.1455999995</v>
+        <v>2441154.9376000003</v>
       </c>
       <c r="O19" s="184"/>
       <c r="P19" s="185">
         <f>Q19/E19</f>
-        <v>3012.4921718571436</v>
+        <v>2986.6408804285716</v>
       </c>
       <c r="Q19" s="183">
         <f>SUM(Q5:Q18)</f>
-        <v>13495964.929920003</v>
+        <v>13380151.14432</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="I25" s="177">
         <f>futuros!B2</f>
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="K25" s="163"/>
       <c r="L25" s="197">
@@ -3502,7 +3502,7 @@
       <c r="M25" s="163"/>
       <c r="N25" s="198">
         <f>(H25-I25)*1.3228*D25</f>
-        <v>-1376004.3850980001</v>
+        <v>-1352108.5057620001</v>
       </c>
       <c r="O25" s="178">
         <f>O5</f>
@@ -3510,7 +3510,7 @@
       </c>
       <c r="Q25" s="198">
         <f>N25*O25</f>
-        <v>-7843224.9950586008</v>
+        <v>-7707018.4828434009</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
@@ -3535,7 +3535,7 @@
       </c>
       <c r="I26" s="177">
         <f>I25</f>
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="K26" s="163"/>
       <c r="L26" s="197">
@@ -3544,7 +3544,7 @@
       <c r="M26" s="163"/>
       <c r="N26" s="198">
         <f>(H26-I26)*1.3228*D26</f>
-        <v>-499293.37332000001</v>
+        <v>-489843.02555999998</v>
       </c>
       <c r="O26" s="178">
         <f>O6</f>
@@ -3552,7 +3552,7 @@
       </c>
       <c r="Q26" s="198">
         <f t="shared" ref="Q26:Q27" si="6">N26*O26</f>
-        <v>-2845972.227924</v>
+        <v>-2792105.2456919998</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
@@ -3576,7 +3576,7 @@
       </c>
       <c r="I27" s="200">
         <f>I26</f>
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="K27" s="163"/>
       <c r="L27" s="197">
@@ -3585,7 +3585,7 @@
       <c r="M27" s="163"/>
       <c r="N27" s="198">
         <f>(H27-I27)*1.3228*D27</f>
-        <v>-652321.50454800006</v>
+        <v>-638010.9779399999</v>
       </c>
       <c r="O27" s="178">
         <f>O7</f>
@@ -3593,7 +3593,7 @@
       </c>
       <c r="Q27" s="198">
         <f t="shared" si="6"/>
-        <v>-3718232.5759236002</v>
+        <v>-3636662.5742579997</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
@@ -3616,13 +3616,13 @@
       <c r="M28" s="202"/>
       <c r="N28" s="202">
         <f>SUM(N25:N27)</f>
-        <v>-2527619.262966</v>
+        <v>-2479962.5092620002</v>
       </c>
       <c r="O28" s="201"/>
       <c r="P28" s="201"/>
       <c r="Q28" s="202">
         <f>SUM(Q25:Q27)</f>
-        <v>-14407429.7989062</v>
+        <v>-14135786.3027934</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
@@ -4306,7 +4306,7 @@
       </c>
       <c r="I57" s="177">
         <f>futuros!B7</f>
-        <v>325.14999999999998</v>
+        <v>320.35000000000002</v>
       </c>
       <c r="K57" s="178">
         <f>O8</f>
@@ -4318,7 +4318,7 @@
       <c r="M57" s="198"/>
       <c r="N57" s="198">
         <f>(H57-I57)*1.3228*D57</f>
-        <v>-82184.274269999878</v>
+        <v>-65983.678110000037</v>
       </c>
       <c r="O57" s="166">
         <f>O25</f>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="Q57" s="198">
         <f>N57*O57</f>
-        <v>-468450.36333899933</v>
+        <v>-376106.96522700024</v>
       </c>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.25">
@@ -4350,7 +4350,7 @@
       </c>
       <c r="I58" s="177">
         <f>I57</f>
-        <v>325.14999999999998</v>
+        <v>320.35000000000002</v>
       </c>
       <c r="K58" s="178">
         <f>O9</f>
@@ -4362,7 +4362,7 @@
       <c r="M58" s="198"/>
       <c r="N58" s="198">
         <f>(H58-I58)*1.3228*D58</f>
-        <v>-8250.3035999999993</v>
+        <v>6150.2263199998633</v>
       </c>
       <c r="O58" s="166">
         <f>O26</f>
@@ -4370,7 +4370,7 @@
       </c>
       <c r="Q58" s="198">
         <f>N58*O58</f>
-        <v>-47026.730519999997</v>
+        <v>35056.290023999223</v>
       </c>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.25">
@@ -4393,13 +4393,13 @@
       <c r="M59" s="201"/>
       <c r="N59" s="202">
         <f>SUM(N56:N58)</f>
-        <v>-90434.577869999877</v>
+        <v>-59833.451790000174</v>
       </c>
       <c r="O59" s="201"/>
       <c r="P59" s="201"/>
       <c r="Q59" s="202">
         <f>SUM(Q56:Q58)</f>
-        <v>-515477.09385899932</v>
+        <v>-341050.67520300101</v>
       </c>
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.25">
@@ -4539,7 +4539,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P32" sqref="P32"/>
     </sheetView>
@@ -8234,7 +8234,7 @@
         <v>270</v>
       </c>
       <c r="D1" s="162">
-        <v>45936</v>
+        <v>45943</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8242,11 +8242,11 @@
         <v>46021</v>
       </c>
       <c r="B2" s="155">
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="C2" s="155">
         <f t="shared" ref="C2:C11" si="0">B2*1.3228</f>
-        <v>510.99763999999999</v>
+        <v>506.23555999999996</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8254,11 +8254,11 @@
         <v>46112</v>
       </c>
       <c r="B3" s="155">
-        <v>369.85</v>
+        <v>364.55</v>
       </c>
       <c r="C3" s="155">
         <f t="shared" si="0"/>
-        <v>489.23758000000004</v>
+        <v>482.22674000000001</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -8266,11 +8266,11 @@
         <v>46173</v>
       </c>
       <c r="B4" s="155">
-        <v>358.2</v>
+        <v>351.3</v>
       </c>
       <c r="C4" s="155">
         <f t="shared" si="0"/>
-        <v>473.82695999999999</v>
+        <v>464.69963999999999</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -8278,11 +8278,11 @@
         <v>46231</v>
       </c>
       <c r="B5" s="155">
-        <v>347.2</v>
+        <v>340</v>
       </c>
       <c r="C5" s="155">
         <f t="shared" si="0"/>
-        <v>459.27616</v>
+        <v>449.75200000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -8290,11 +8290,11 @@
         <v>46295</v>
       </c>
       <c r="B6" s="155">
-        <v>333.85</v>
+        <v>328.6</v>
       </c>
       <c r="C6" s="155">
         <f t="shared" si="0"/>
-        <v>441.61678000000001</v>
+        <v>434.67207999999999</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -8302,11 +8302,11 @@
         <v>46386</v>
       </c>
       <c r="B7" s="155">
-        <v>325.14999999999998</v>
+        <v>320.35000000000002</v>
       </c>
       <c r="C7" s="155">
         <f t="shared" si="0"/>
-        <v>430.10841999999997</v>
+        <v>423.75898000000001</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -8314,11 +8314,11 @@
         <v>46477</v>
       </c>
       <c r="B8" s="155">
-        <v>318.89999999999998</v>
+        <v>309.5</v>
       </c>
       <c r="C8" s="155">
         <f t="shared" si="0"/>
-        <v>421.84091999999998</v>
+        <v>409.40659999999997</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8326,11 +8326,11 @@
         <v>46538</v>
       </c>
       <c r="B9" s="155">
-        <v>320.7</v>
+        <v>302.3</v>
       </c>
       <c r="C9" s="155">
         <f t="shared" si="0"/>
-        <v>424.22195999999997</v>
+        <v>399.88244000000003</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -8338,11 +8338,11 @@
         <v>46596</v>
       </c>
       <c r="B10" s="155">
-        <v>315.60000000000002</v>
+        <v>297.2</v>
       </c>
       <c r="C10" s="155">
         <f t="shared" si="0"/>
-        <v>417.47568000000001</v>
+        <v>393.13615999999996</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -8350,11 +8350,11 @@
         <v>46660</v>
       </c>
       <c r="B11" s="155">
-        <v>310.14999999999998</v>
+        <v>291.5</v>
       </c>
       <c r="C11" s="155">
         <f t="shared" si="0"/>
-        <v>410.26641999999998</v>
+        <v>385.59620000000001</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -8362,11 +8362,11 @@
         <v>46751</v>
       </c>
       <c r="B12" s="155">
-        <v>304.75</v>
+        <v>285.5</v>
       </c>
       <c r="C12" s="155">
         <f>B12*1.3228</f>
-        <v>403.12329999999997</v>
+        <v>377.65940000000001</v>
       </c>
     </row>
   </sheetData>
@@ -8379,8 +8379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435A83C4-FEBA-7F44-BF8C-E9ADE9845E60}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L16" sqref="L16:L28"/>
     </sheetView>
   </sheetViews>
@@ -9109,7 +9109,7 @@
       </c>
       <c r="H16" s="155">
         <f>futuros!B2</f>
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="162">
@@ -9118,7 +9118,7 @@
       <c r="K16" s="162"/>
       <c r="L16" s="215">
         <f t="shared" si="2"/>
-        <v>-1376004.3850980001</v>
+        <v>-1352108.5057619999</v>
       </c>
       <c r="M16" s="160"/>
       <c r="N16" s="215"/>
@@ -9147,7 +9147,7 @@
       </c>
       <c r="H17" s="155">
         <f>futuros!B2</f>
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="162">
@@ -9156,7 +9156,7 @@
       <c r="K17" s="162"/>
       <c r="L17" s="215">
         <f t="shared" si="2"/>
-        <v>-499293.37332000001</v>
+        <v>-489843.02555999998</v>
       </c>
       <c r="M17" s="160"/>
       <c r="N17" s="215"/>
@@ -9187,7 +9187,7 @@
       </c>
       <c r="H18" s="155">
         <f>futuros!B2</f>
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="162">
@@ -9196,7 +9196,7 @@
       <c r="K18" s="162"/>
       <c r="L18" s="215">
         <f t="shared" si="2"/>
-        <v>-147792.93858000002</v>
+        <v>-138342.59081999998</v>
       </c>
       <c r="M18" s="160"/>
       <c r="N18" s="215"/>
@@ -9225,7 +9225,7 @@
       </c>
       <c r="H19" s="217">
         <f>futuros!B2</f>
-        <v>386.3</v>
+        <v>382.7</v>
       </c>
       <c r="I19" s="208"/>
       <c r="J19" s="219">
@@ -9234,7 +9234,7 @@
       <c r="K19" s="219"/>
       <c r="L19" s="220">
         <f t="shared" si="2"/>
-        <v>-344622.68164800003</v>
+        <v>-337062.40343999997</v>
       </c>
       <c r="M19" s="218"/>
       <c r="N19" s="220"/>
@@ -9265,7 +9265,7 @@
       </c>
       <c r="H20" s="155">
         <f>futuros!B3</f>
-        <v>369.85</v>
+        <v>364.55</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="162">
@@ -9274,7 +9274,7 @@
       <c r="K20" s="162"/>
       <c r="L20" s="215">
         <f t="shared" si="2"/>
-        <v>-117735.58251000005</v>
+        <v>-103822.57053000003</v>
       </c>
       <c r="M20" s="160"/>
       <c r="N20" s="215"/>
@@ -9303,7 +9303,7 @@
       </c>
       <c r="H21" s="155">
         <f>futuros!B7</f>
-        <v>325.14999999999998</v>
+        <v>320.35000000000002</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="162">
@@ -9312,7 +9312,7 @@
       <c r="K21" s="162"/>
       <c r="L21" s="215">
         <f t="shared" si="2"/>
-        <v>-82184.274269999878</v>
+        <v>-65983.678110000037</v>
       </c>
       <c r="M21" s="160"/>
       <c r="N21" s="215"/>
@@ -9340,7 +9340,7 @@
       </c>
       <c r="H22" s="155">
         <f>futuros!B7</f>
-        <v>325.14999999999998</v>
+        <v>320.35000000000002</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="162">
@@ -9349,7 +9349,7 @@
       <c r="K22" s="162"/>
       <c r="L22" s="215">
         <f t="shared" si="2"/>
-        <v>-8250.3035999999993</v>
+        <v>6150.2263199998633</v>
       </c>
       <c r="M22" s="160"/>
       <c r="N22" s="215"/>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="H23" s="155">
         <f>futuros!B7</f>
-        <v>325.14999999999998</v>
+        <v>320.35000000000002</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="162">
@@ -9386,7 +9386,7 @@
       <c r="K23" s="162"/>
       <c r="L23" s="215">
         <f t="shared" si="2"/>
-        <v>-53851.981679999968</v>
+        <v>-39451.451760000098</v>
       </c>
       <c r="M23" s="160"/>
       <c r="N23" s="215"/>
@@ -9415,7 +9415,7 @@
       </c>
       <c r="H24" s="217">
         <f>futuros!B7</f>
-        <v>325.14999999999998</v>
+        <v>320.35000000000002</v>
       </c>
       <c r="I24" s="208"/>
       <c r="J24" s="219">
@@ -9424,7 +9424,7 @@
       <c r="K24" s="219"/>
       <c r="L24" s="220">
         <f t="shared" si="2"/>
-        <v>-390089.35475999978</v>
+        <v>-339687.50004000025</v>
       </c>
       <c r="M24" s="218"/>
       <c r="N24" s="220"/>
@@ -9453,7 +9453,7 @@
       </c>
       <c r="H25" s="155">
         <f>futuros!B12</f>
-        <v>304.75</v>
+        <v>285.5</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="162">
@@ -9462,7 +9462,7 @@
       <c r="K25" s="162"/>
       <c r="L25" s="215">
         <f t="shared" si="2"/>
-        <v>-229977.21284999998</v>
+        <v>-150568.04069999998</v>
       </c>
       <c r="M25" s="160"/>
       <c r="N25" s="215"/>
@@ -9488,7 +9488,7 @@
       </c>
       <c r="H26" s="155">
         <f>futuros!B12</f>
-        <v>304.75</v>
+        <v>285.5</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="162">
@@ -9497,7 +9497,7 @@
       <c r="K26" s="162"/>
       <c r="L26" s="215">
         <f t="shared" ref="L26" si="8">D26*(G26-H26)*1.3228</f>
-        <v>-209257.7004</v>
+        <v>-151505.57519999999</v>
       </c>
       <c r="M26" s="160"/>
       <c r="N26" s="215"/>
@@ -9523,7 +9523,7 @@
       </c>
       <c r="H27" s="155">
         <f>futuros!B12</f>
-        <v>304.75</v>
+        <v>285.5</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="162">
@@ -9532,7 +9532,7 @@
       <c r="K27" s="162"/>
       <c r="L27" s="215">
         <f t="shared" ref="L27" si="10">D27*(G27-H27)*1.3228</f>
-        <v>-100784.95875000001</v>
+        <v>-64689.880499999999</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -9556,7 +9556,7 @@
       </c>
       <c r="H28" s="155">
         <f>futuros!B12</f>
-        <v>304.75</v>
+        <v>285.5</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="162">
@@ -9565,7 +9565,7 @@
       <c r="K28" s="162"/>
       <c r="L28" s="215">
         <f t="shared" ref="L28" si="12">D28*(G28-H28)*1.3228</f>
-        <v>-78284.130749999997</v>
+        <v>-42189.052499999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização 03/11 e contratos Southland
</commit_message>
<xml_diff>
--- a/vendas_cafe_em_reais.xlsx
+++ b/vendas_cafe_em_reais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotocastro/PycharmProjects/Vendas Cafe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8E01DC-3A49-3341-B94A-7199CBC8B54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B0A892-64A4-9848-B8B5-ACF6FA955D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="680" windowWidth="24980" windowHeight="18440" activeTab="3" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
+    <workbookView xWindow="4640" yWindow="680" windowWidth="24760" windowHeight="18440" activeTab="1" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2 (2)" sheetId="16" state="hidden" r:id="rId1"/>
@@ -1154,7 +1154,7 @@
     <numFmt numFmtId="167" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="168" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1290,6 +1290,13 @@
     <font>
       <sz val="10"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1519,11 +1526,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="226">
+  <cellXfs count="234">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2055,6 +2063,28 @@
     <xf numFmtId="168" fontId="20" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="20" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2069,9 +2099,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FBDE122D-F9BE-AE4A-91C0-5CA92DAE08C8}"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2642,26 +2673,26 @@
       </c>
       <c r="L6" s="177">
         <f>futuros!B2</f>
-        <v>408.3</v>
+        <v>400.05</v>
       </c>
       <c r="M6" s="177">
         <f>(L6+H6)*1.3228</f>
-        <v>579.78323999999998</v>
+        <v>568.87013999999999</v>
       </c>
       <c r="N6" s="167">
         <f>(E6*(M6+H6))</f>
-        <v>195130.63679999998</v>
+        <v>191638.4448</v>
       </c>
       <c r="O6" s="178">
         <v>5.7</v>
       </c>
       <c r="P6" s="167">
         <f t="shared" ref="P6:P16" si="1">M6*O6</f>
-        <v>3304.7644679999999</v>
+        <v>3242.5597980000002</v>
       </c>
       <c r="Q6" s="167">
         <f t="shared" ref="Q6:Q16" si="2">P6*E6</f>
-        <v>1057524.6297599999</v>
+        <v>1037619.1353600001</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
@@ -2698,26 +2729,26 @@
       </c>
       <c r="L7" s="177">
         <f>L6</f>
-        <v>408.3</v>
+        <v>400.05</v>
       </c>
       <c r="M7" s="177">
         <f>(L7+H7)*1.3228</f>
-        <v>579.78323999999998</v>
+        <v>568.87013999999999</v>
       </c>
       <c r="N7" s="167">
         <f>(E7*(M7+H7))</f>
-        <v>195130.63679999998</v>
+        <v>191638.4448</v>
       </c>
       <c r="O7" s="178">
         <v>5.7</v>
       </c>
       <c r="P7" s="167">
         <f t="shared" si="1"/>
-        <v>3304.7644679999999</v>
+        <v>3242.5597980000002</v>
       </c>
       <c r="Q7" s="167">
         <f t="shared" si="2"/>
-        <v>1057524.6297599999</v>
+        <v>1037619.1353600001</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
@@ -2754,26 +2785,26 @@
       </c>
       <c r="L8" s="177">
         <f>L7</f>
-        <v>408.3</v>
+        <v>400.05</v>
       </c>
       <c r="M8" s="177">
         <f>(L8+H8)*1.3228</f>
-        <v>579.78323999999998</v>
+        <v>568.87013999999999</v>
       </c>
       <c r="N8" s="167">
         <f>(E8*(M8+H8))</f>
-        <v>195130.63679999998</v>
+        <v>191638.4448</v>
       </c>
       <c r="O8" s="178">
         <v>5.7</v>
       </c>
       <c r="P8" s="167">
         <f t="shared" si="1"/>
-        <v>3304.7644679999999</v>
+        <v>3242.5597980000002</v>
       </c>
       <c r="Q8" s="167">
         <f t="shared" si="2"/>
-        <v>1057524.6297599999</v>
+        <v>1037619.1353600001</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
@@ -2810,26 +2841,26 @@
       </c>
       <c r="L9" s="177">
         <f>futuros!B2</f>
-        <v>408.3</v>
+        <v>400.05</v>
       </c>
       <c r="M9" s="177">
         <f>(L9+H9)*1.3228</f>
-        <v>579.78323999999998</v>
+        <v>568.87013999999999</v>
       </c>
       <c r="N9" s="167">
         <f>(E9*(M9+H9))</f>
-        <v>195130.63679999998</v>
+        <v>191638.4448</v>
       </c>
       <c r="O9" s="178">
         <v>5.7</v>
       </c>
       <c r="P9" s="167">
         <f t="shared" si="1"/>
-        <v>3304.7644679999999</v>
+        <v>3242.5597980000002</v>
       </c>
       <c r="Q9" s="167">
         <f t="shared" si="2"/>
-        <v>1057524.6297599999</v>
+        <v>1037619.1353600001</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
@@ -2866,26 +2897,26 @@
       </c>
       <c r="L10" s="177">
         <f>futuros!B3</f>
-        <v>384.95</v>
+        <v>378.75</v>
       </c>
       <c r="M10" s="177">
         <f>(L10+H10)*1.3228</f>
-        <v>548.89585999999997</v>
+        <v>540.69449999999995</v>
       </c>
       <c r="N10" s="167">
         <f>(E10*(M10+H10))</f>
-        <v>185246.6752</v>
+        <v>182622.24</v>
       </c>
       <c r="O10" s="178">
         <v>5.7</v>
       </c>
       <c r="P10" s="167">
         <f t="shared" si="1"/>
-        <v>3128.7064019999998</v>
+        <v>3081.9586499999996</v>
       </c>
       <c r="Q10" s="167">
         <f t="shared" si="2"/>
-        <v>1001186.0486399999</v>
+        <v>986226.76799999992</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
@@ -2922,26 +2953,26 @@
       </c>
       <c r="L11" s="177">
         <f>futuros!B2</f>
-        <v>408.3</v>
+        <v>400.05</v>
       </c>
       <c r="M11" s="177">
         <f t="shared" ref="M11:M16" si="4">(L11+H11)*1.3228</f>
-        <v>577.13764000000003</v>
+        <v>566.22454000000005</v>
       </c>
       <c r="N11" s="167">
         <f t="shared" ref="N11:N16" si="5">(E11*(M11+H11))</f>
-        <v>193644.0448</v>
+        <v>190151.85280000002</v>
       </c>
       <c r="O11" s="178">
         <v>5.7</v>
       </c>
       <c r="P11" s="167">
         <f t="shared" si="1"/>
-        <v>3289.6845480000002</v>
+        <v>3227.4798780000006</v>
       </c>
       <c r="Q11" s="167">
         <f t="shared" si="2"/>
-        <v>1052699.0553600001</v>
+        <v>1032793.5609600001</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
@@ -2978,26 +3009,26 @@
       </c>
       <c r="L12" s="177">
         <f>futuros!B2</f>
-        <v>408.3</v>
+        <v>400.05</v>
       </c>
       <c r="M12" s="177">
         <f t="shared" si="4"/>
-        <v>577.13764000000003</v>
+        <v>566.22454000000005</v>
       </c>
       <c r="N12" s="167">
         <f t="shared" si="5"/>
-        <v>193644.0448</v>
+        <v>190151.85280000002</v>
       </c>
       <c r="O12" s="178">
         <v>5.7</v>
       </c>
       <c r="P12" s="167">
         <f t="shared" si="1"/>
-        <v>3289.6845480000002</v>
+        <v>3227.4798780000006</v>
       </c>
       <c r="Q12" s="167">
         <f t="shared" si="2"/>
-        <v>1052699.0553600001</v>
+        <v>1032793.5609600001</v>
       </c>
     </row>
     <row r="13" spans="2:20" s="166" customFormat="1" x14ac:dyDescent="0.25">
@@ -3034,26 +3065,26 @@
       </c>
       <c r="L13" s="177">
         <f>futuros!B3</f>
-        <v>384.95</v>
+        <v>378.75</v>
       </c>
       <c r="M13" s="177">
         <f t="shared" si="4"/>
-        <v>546.25026000000003</v>
+        <v>538.0489</v>
       </c>
       <c r="N13" s="167">
         <f t="shared" si="5"/>
-        <v>183760.08319999999</v>
+        <v>181135.64799999999</v>
       </c>
       <c r="O13" s="178">
         <v>5.7</v>
       </c>
       <c r="P13" s="167">
         <f t="shared" si="1"/>
-        <v>3113.6264820000001</v>
+        <v>3066.8787299999999</v>
       </c>
       <c r="Q13" s="167">
         <f t="shared" si="2"/>
-        <v>996360.47424000001</v>
+        <v>981401.1936</v>
       </c>
       <c r="R13" s="163"/>
       <c r="S13" s="163"/>
@@ -3093,26 +3124,26 @@
       </c>
       <c r="L14" s="177">
         <f>futuros!B4</f>
-        <v>369.05</v>
+        <v>363.15</v>
       </c>
       <c r="M14" s="177">
         <f t="shared" si="4"/>
-        <v>525.21774000000005</v>
+        <v>517.41321999999991</v>
       </c>
       <c r="N14" s="167">
         <f t="shared" si="5"/>
-        <v>177029.67680000002</v>
+        <v>174532.23039999997</v>
       </c>
       <c r="O14" s="178">
         <v>5.7</v>
       </c>
       <c r="P14" s="167">
         <f t="shared" si="1"/>
-        <v>2993.7411180000004</v>
+        <v>2949.2553539999994</v>
       </c>
       <c r="Q14" s="167">
         <f t="shared" si="2"/>
-        <v>957997.15776000009</v>
+        <v>943761.71327999979</v>
       </c>
       <c r="R14" s="163"/>
       <c r="S14" s="163"/>
@@ -3152,26 +3183,26 @@
       </c>
       <c r="L15" s="177">
         <f>futuros!B3</f>
-        <v>384.95</v>
+        <v>378.75</v>
       </c>
       <c r="M15" s="177">
         <f t="shared" si="4"/>
-        <v>480.11025999999998</v>
+        <v>471.90890000000002</v>
       </c>
       <c r="N15" s="167">
         <f t="shared" si="5"/>
-        <v>146595.28320000001</v>
+        <v>143970.848</v>
       </c>
       <c r="O15" s="178">
         <v>5.7</v>
       </c>
       <c r="P15" s="167">
         <f t="shared" si="1"/>
-        <v>2736.6284820000001</v>
+        <v>2689.8807300000003</v>
       </c>
       <c r="Q15" s="167">
         <f t="shared" si="2"/>
-        <v>875721.11424000002</v>
+        <v>860761.83360000013</v>
       </c>
       <c r="R15" s="163"/>
       <c r="S15" s="163"/>
@@ -3211,26 +3242,26 @@
       </c>
       <c r="L16" s="177">
         <f>futuros!B2</f>
-        <v>408.3</v>
+        <v>400.05</v>
       </c>
       <c r="M16" s="177">
         <f t="shared" si="4"/>
-        <v>610.20763999999997</v>
+        <v>599.29453999999998</v>
       </c>
       <c r="N16" s="167">
         <f t="shared" si="5"/>
-        <v>212226.4448</v>
+        <v>208734.25279999999</v>
       </c>
       <c r="O16" s="178">
         <v>5.7</v>
       </c>
       <c r="P16" s="167">
         <f t="shared" si="1"/>
-        <v>3478.183548</v>
+        <v>3415.9788779999999</v>
       </c>
       <c r="Q16" s="167">
         <f t="shared" si="2"/>
-        <v>1113018.73536</v>
+        <v>1093113.2409600001</v>
       </c>
       <c r="R16" s="163"/>
       <c r="S16" s="163"/>
@@ -3357,20 +3388,20 @@
       <c r="L19" s="179"/>
       <c r="M19" s="182">
         <f>N19/E19</f>
-        <v>569.29214285714284</v>
+        <v>561.52069285714288</v>
       </c>
       <c r="N19" s="183">
         <f>SUM(N5:N18)</f>
-        <v>2550428.7999999998</v>
+        <v>2515612.7039999999</v>
       </c>
       <c r="O19" s="184"/>
       <c r="P19" s="185">
         <f>Q19/E19</f>
-        <v>3125.672357142857</v>
+        <v>3081.3750921428573</v>
       </c>
       <c r="Q19" s="183">
         <f>SUM(Q5:Q18)</f>
-        <v>14003012.16</v>
+        <v>13804560.412800001</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
@@ -3493,7 +3524,7 @@
       </c>
       <c r="I25" s="177">
         <f>futuros!B2</f>
-        <v>408.3</v>
+        <v>400.05</v>
       </c>
       <c r="K25" s="163"/>
       <c r="L25" s="197">
@@ -3502,7 +3533,7 @@
       <c r="M25" s="163"/>
       <c r="N25" s="198">
         <f>(H25-I25)*1.3228*D25</f>
-        <v>-1522034.7588179999</v>
+        <v>-1467273.368673</v>
       </c>
       <c r="O25" s="178">
         <f>O5</f>
@@ -3510,7 +3541,7 @@
       </c>
       <c r="Q25" s="198">
         <f>N25*O25</f>
-        <v>-8675598.1252625994</v>
+        <v>-8363458.2014361005</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
@@ -3535,7 +3566,7 @@
       </c>
       <c r="I26" s="177">
         <f>I25</f>
-        <v>408.3</v>
+        <v>400.05</v>
       </c>
       <c r="K26" s="163"/>
       <c r="L26" s="197">
@@ -3544,7 +3575,7 @@
       <c r="M26" s="163"/>
       <c r="N26" s="198">
         <f>(H26-I26)*1.3228*D26</f>
-        <v>-557045.49852000002</v>
+        <v>-535388.45157000003</v>
       </c>
       <c r="O26" s="178">
         <f>O6</f>
@@ -3552,7 +3583,7 @@
       </c>
       <c r="Q26" s="198">
         <f t="shared" ref="Q26:Q27" si="6">N26*O26</f>
-        <v>-3175159.3415640001</v>
+        <v>-3051714.1739490004</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
@@ -3576,7 +3607,7 @@
       </c>
       <c r="I27" s="200">
         <f>I26</f>
-        <v>408.3</v>
+        <v>400.05</v>
       </c>
       <c r="K27" s="163"/>
       <c r="L27" s="197">
@@ -3585,7 +3616,7 @@
       <c r="M27" s="163"/>
       <c r="N27" s="198">
         <f>(H27-I27)*1.3228*D27</f>
-        <v>-739774.7227080001</v>
+        <v>-706979.76589799998</v>
       </c>
       <c r="O27" s="178">
         <f>O7</f>
@@ -3593,7 +3624,7 @@
       </c>
       <c r="Q27" s="198">
         <f t="shared" si="6"/>
-        <v>-4216715.9194356008</v>
+        <v>-4029784.6656185999</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
@@ -3616,13 +3647,13 @@
       <c r="M28" s="202"/>
       <c r="N28" s="202">
         <f>SUM(N25:N27)</f>
-        <v>-2818854.9800460003</v>
+        <v>-2709641.586141</v>
       </c>
       <c r="O28" s="201"/>
       <c r="P28" s="201"/>
       <c r="Q28" s="202">
         <f>SUM(Q25:Q27)</f>
-        <v>-16067473.386262201</v>
+        <v>-15444957.041003702</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
@@ -4306,7 +4337,7 @@
       </c>
       <c r="I57" s="177">
         <f>futuros!B7</f>
-        <v>330.15</v>
+        <v>322.5</v>
       </c>
       <c r="K57" s="178">
         <f>O8</f>
@@ -4318,7 +4349,7 @@
       <c r="M57" s="198"/>
       <c r="N57" s="198">
         <f>(H57-I57)*1.3228*D57</f>
-        <v>-99059.895269999892</v>
+        <v>-73240.195139999967</v>
       </c>
       <c r="O57" s="166">
         <f>O25</f>
@@ -4326,7 +4357,7 @@
       </c>
       <c r="Q57" s="198">
         <f>N57*O57</f>
-        <v>-564641.40303899942</v>
+        <v>-417469.11229799985</v>
       </c>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.25">
@@ -4350,7 +4381,7 @@
       </c>
       <c r="I58" s="177">
         <f>I57</f>
-        <v>330.15</v>
+        <v>322.5</v>
       </c>
       <c r="K58" s="178">
         <f>O9</f>
@@ -4362,7 +4393,7 @@
       <c r="M58" s="198"/>
       <c r="N58" s="198">
         <f>(H58-I58)*1.3228*D58</f>
-        <v>-23250.855599999999</v>
+        <v>-300.01104000006819</v>
       </c>
       <c r="O58" s="166">
         <f>O26</f>
@@ -4370,7 +4401,7 @@
       </c>
       <c r="Q58" s="198">
         <f>N58*O58</f>
-        <v>-132529.87692000001</v>
+        <v>-1710.0629280003886</v>
       </c>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.25">
@@ -4393,13 +4424,13 @@
       <c r="M59" s="201"/>
       <c r="N59" s="202">
         <f>SUM(N56:N58)</f>
-        <v>-122310.75086999989</v>
+        <v>-73540.206180000037</v>
       </c>
       <c r="O59" s="201"/>
       <c r="P59" s="201"/>
       <c r="Q59" s="202">
         <f>SUM(Q56:Q58)</f>
-        <v>-697171.27995899948</v>
+        <v>-419179.17522600025</v>
       </c>
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.25">
@@ -4539,9 +4570,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P32" sqref="P32"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -7226,7 +7257,7 @@
         <v>19</v>
       </c>
       <c r="E53" s="2">
-        <v>320</v>
+        <v>240</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>27</v>
@@ -7251,7 +7282,7 @@
       </c>
       <c r="N53" s="3">
         <f t="shared" si="4"/>
-        <v>156160</v>
+        <v>117120</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
@@ -7268,13 +7299,13 @@
         <v>19</v>
       </c>
       <c r="E54" s="2">
-        <v>320</v>
+        <v>80</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>289</v>
+        <v>35</v>
       </c>
       <c r="H54" s="2">
         <v>0</v>
@@ -7293,7 +7324,7 @@
       </c>
       <c r="N54" s="3">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
@@ -8234,7 +8265,7 @@
         <v>270</v>
       </c>
       <c r="D1" s="162">
-        <v>45950</v>
+        <v>45964</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8242,11 +8273,11 @@
         <v>46021</v>
       </c>
       <c r="B2" s="155">
-        <v>408.3</v>
+        <v>400.05</v>
       </c>
       <c r="C2" s="155">
         <f t="shared" ref="C2:C11" si="0">B2*1.3228</f>
-        <v>540.09924000000001</v>
+        <v>529.18614000000002</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8254,11 +8285,11 @@
         <v>46112</v>
       </c>
       <c r="B3" s="155">
-        <v>384.95</v>
+        <v>378.75</v>
       </c>
       <c r="C3" s="155">
         <f t="shared" si="0"/>
-        <v>509.21186</v>
+        <v>501.01049999999998</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -8266,11 +8297,11 @@
         <v>46173</v>
       </c>
       <c r="B4" s="155">
-        <v>369.05</v>
+        <v>363.15</v>
       </c>
       <c r="C4" s="155">
         <f t="shared" si="0"/>
-        <v>488.17934000000002</v>
+        <v>480.37481999999994</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -8278,11 +8309,11 @@
         <v>46231</v>
       </c>
       <c r="B5" s="155">
-        <v>354.05</v>
+        <v>348.25</v>
       </c>
       <c r="C5" s="155">
         <f t="shared" si="0"/>
-        <v>468.33733999999998</v>
+        <v>460.6651</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -8290,11 +8321,11 @@
         <v>46295</v>
       </c>
       <c r="B6" s="155">
-        <v>340.05</v>
+        <v>334</v>
       </c>
       <c r="C6" s="155">
         <f t="shared" si="0"/>
-        <v>449.81814000000003</v>
+        <v>441.8152</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -8302,11 +8333,11 @@
         <v>46386</v>
       </c>
       <c r="B7" s="155">
-        <v>330.15</v>
+        <v>322.5</v>
       </c>
       <c r="C7" s="155">
         <f t="shared" si="0"/>
-        <v>436.72241999999994</v>
+        <v>426.60300000000001</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -8314,11 +8345,11 @@
         <v>46477</v>
       </c>
       <c r="B8" s="155">
-        <v>321.39999999999998</v>
+        <v>311.8</v>
       </c>
       <c r="C8" s="155">
         <f t="shared" si="0"/>
-        <v>425.14791999999994</v>
+        <v>412.44904000000002</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8326,11 +8357,11 @@
         <v>46538</v>
       </c>
       <c r="B9" s="155">
-        <v>310.39999999999998</v>
+        <v>306.5</v>
       </c>
       <c r="C9" s="155">
         <f t="shared" si="0"/>
-        <v>410.59711999999996</v>
+        <v>405.43819999999999</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -8338,11 +8369,11 @@
         <v>46596</v>
       </c>
       <c r="B10" s="155">
-        <v>304.64999999999998</v>
+        <v>301.35000000000002</v>
       </c>
       <c r="C10" s="155">
         <f t="shared" si="0"/>
-        <v>402.99101999999993</v>
+        <v>398.62578000000002</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -8350,11 +8381,11 @@
         <v>46660</v>
       </c>
       <c r="B11" s="155">
-        <v>298.5</v>
+        <v>295.95</v>
       </c>
       <c r="C11" s="155">
         <f t="shared" si="0"/>
-        <v>394.85579999999999</v>
+        <v>391.48265999999995</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -8362,11 +8393,11 @@
         <v>46751</v>
       </c>
       <c r="B12" s="155">
-        <v>292.39999999999998</v>
+        <v>290.35000000000002</v>
       </c>
       <c r="C12" s="155">
         <f>B12*1.3228</f>
-        <v>386.78671999999995</v>
+        <v>384.07498000000004</v>
       </c>
     </row>
   </sheetData>
@@ -8379,9 +8410,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435A83C4-FEBA-7F44-BF8C-E9ADE9845E60}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L16" sqref="L16:L19"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L18" sqref="L18:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9041,48 +9072,48 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="209" t="s">
+      <c r="A15" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B15" s="209" t="s">
+      <c r="B15" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C15" s="208">
-        <f>C19</f>
+      <c r="C15" s="2">
+        <f>C17</f>
         <v>47616</v>
       </c>
-      <c r="D15" s="216">
+      <c r="D15" s="213">
         <f t="shared" ref="D15" si="4">283.5*F15</f>
         <v>1417.5</v>
       </c>
-      <c r="E15" s="216"/>
-      <c r="F15" s="217">
+      <c r="E15" s="213"/>
+      <c r="F15" s="155">
         <v>5</v>
       </c>
-      <c r="G15" s="217">
-        <f>G19</f>
+      <c r="G15" s="155">
+        <f>G17</f>
         <v>222.2</v>
       </c>
-      <c r="H15" s="217">
+      <c r="H15" s="155">
         <v>280</v>
       </c>
-      <c r="I15" s="208"/>
-      <c r="J15" s="219">
+      <c r="I15" s="2"/>
+      <c r="J15" s="162">
         <v>45769</v>
       </c>
-      <c r="K15" s="219">
+      <c r="K15" s="162">
         <v>45840</v>
       </c>
-      <c r="L15" s="220">
+      <c r="L15" s="215">
         <f t="shared" ref="L15" si="5">D15*(G15-H15)*1.3228</f>
         <v>-108378.98820000002</v>
       </c>
-      <c r="M15" s="218">
+      <c r="M15" s="160">
         <f>5.4677</f>
         <v>5.4676999999999998</v>
       </c>
-      <c r="N15" s="220">
-        <f t="shared" ref="N15" si="6">IF(I15="",L15*M15,(D15*(G15*I15-H15*M15)*1.3328))</f>
+      <c r="N15" s="215">
+        <f t="shared" ref="N15:N16" si="6">IF(I15="",L15*M15,(D15*(G15*I15-H15*M15)*1.3328))</f>
         <v>-592583.79378114012</v>
       </c>
     </row>
@@ -9091,7 +9122,7 @@
         <v>295</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="C16" s="2">
         <v>25852</v>
@@ -9108,133 +9139,145 @@
         <v>179</v>
       </c>
       <c r="H16" s="155">
-        <f>futuros!B2</f>
-        <v>408.3</v>
-      </c>
-      <c r="I16" s="2"/>
+        <v>434</v>
+      </c>
+      <c r="I16" s="228"/>
       <c r="J16" s="162">
         <v>45973</v>
       </c>
-      <c r="K16" s="162"/>
+      <c r="K16" s="162">
+        <v>45953</v>
+      </c>
       <c r="L16" s="215">
         <f t="shared" si="2"/>
-        <v>-1522034.7588180001</v>
-      </c>
-      <c r="M16" s="160"/>
-      <c r="N16" s="215"/>
+        <v>-1692624.7863</v>
+      </c>
+      <c r="M16" s="160">
+        <v>5.3811</v>
+      </c>
+      <c r="N16" s="215">
+        <f t="shared" si="6"/>
+        <v>-9108183.2375589311</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="209" t="s">
+        <v>295</v>
+      </c>
+      <c r="B17" s="209" t="s">
+        <v>325</v>
+      </c>
+      <c r="C17" s="208">
+        <v>47616</v>
+      </c>
+      <c r="D17" s="216">
+        <f>283.5*F17</f>
+        <v>1587.6</v>
+      </c>
+      <c r="E17" s="216"/>
+      <c r="F17" s="217">
+        <f>10.6-5</f>
+        <v>5.6</v>
+      </c>
+      <c r="G17" s="217">
+        <v>222.2</v>
+      </c>
+      <c r="H17" s="217">
+        <v>434</v>
+      </c>
+      <c r="I17" s="228"/>
+      <c r="J17" s="219">
+        <v>45980</v>
+      </c>
+      <c r="K17" s="219">
+        <v>45953</v>
+      </c>
+      <c r="L17" s="220">
+        <f>D17*(G17-H17)*1.3228</f>
+        <v>-444796.36790399998</v>
+      </c>
+      <c r="M17" s="218">
+        <v>5.3811</v>
+      </c>
+      <c r="N17" s="220">
+        <f>IF(I17="",L17*M17,(D17*(G17*I17-H17*M17)*1.3328))</f>
+        <v>-2393493.7353282142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="221" t="s">
         <v>296</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="221" t="s">
         <v>330</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C18" s="222">
         <v>507931308</v>
       </c>
-      <c r="D17" s="213">
+      <c r="D18" s="223">
         <f t="shared" si="0"/>
         <v>1984.5</v>
       </c>
-      <c r="E17" s="213"/>
-      <c r="F17" s="155">
+      <c r="E18" s="223"/>
+      <c r="F18" s="224">
         <f>262500/37500</f>
         <v>7</v>
       </c>
-      <c r="G17" s="155">
+      <c r="G18" s="224">
         <v>196.1</v>
       </c>
-      <c r="H17" s="155">
+      <c r="H18" s="224">
         <f>futuros!B2</f>
-        <v>408.3</v>
-      </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="162">
+        <v>400.05</v>
+      </c>
+      <c r="I18" s="222"/>
+      <c r="J18" s="225">
         <v>45973</v>
       </c>
-      <c r="K17" s="162"/>
-      <c r="L17" s="215">
+      <c r="K18" s="225"/>
+      <c r="L18" s="226">
         <f t="shared" si="2"/>
-        <v>-557045.49852000002</v>
-      </c>
-      <c r="M17" s="160"/>
-      <c r="N17" s="215"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+        <v>-535388.45157000003</v>
+      </c>
+      <c r="M18" s="227"/>
+      <c r="N18" s="226"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="209" t="s">
         <v>296</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="209" t="s">
         <v>329</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C19" s="208">
         <v>29487615</v>
       </c>
-      <c r="D18" s="213">
+      <c r="D19" s="216">
         <f t="shared" si="0"/>
         <v>1984.5</v>
       </c>
-      <c r="E18" s="213" t="s">
+      <c r="E19" s="216" t="s">
         <v>344</v>
       </c>
-      <c r="F18" s="155">
+      <c r="F19" s="217">
         <f>262500/37500</f>
         <v>7</v>
       </c>
-      <c r="G18" s="155">
+      <c r="G19" s="217">
         <v>330</v>
-      </c>
-      <c r="H18" s="155">
-        <f>futuros!B2</f>
-        <v>408.3</v>
-      </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="162">
-        <v>45973</v>
-      </c>
-      <c r="K18" s="162"/>
-      <c r="L18" s="215">
-        <f t="shared" si="2"/>
-        <v>-205545.06378000005</v>
-      </c>
-      <c r="M18" s="160"/>
-      <c r="N18" s="215"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="209" t="s">
-        <v>295</v>
-      </c>
-      <c r="B19" s="209" t="s">
-        <v>330</v>
-      </c>
-      <c r="C19" s="208">
-        <v>47616</v>
-      </c>
-      <c r="D19" s="216">
-        <f t="shared" si="0"/>
-        <v>1587.6</v>
-      </c>
-      <c r="E19" s="216"/>
-      <c r="F19" s="217">
-        <f>10.6-5</f>
-        <v>5.6</v>
-      </c>
-      <c r="G19" s="217">
-        <v>222.2</v>
       </c>
       <c r="H19" s="217">
         <f>futuros!B2</f>
-        <v>408.3</v>
+        <v>400.05</v>
       </c>
       <c r="I19" s="208"/>
       <c r="J19" s="219">
-        <v>45980</v>
+        <v>45973</v>
       </c>
       <c r="K19" s="219"/>
       <c r="L19" s="220">
         <f t="shared" si="2"/>
-        <v>-390824.38180800003</v>
+        <v>-183888.01683000004</v>
       </c>
       <c r="M19" s="218"/>
       <c r="N19" s="220"/>
@@ -9265,7 +9308,7 @@
       </c>
       <c r="H20" s="155">
         <f>futuros!B3</f>
-        <v>384.95</v>
+        <v>378.75</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="162">
@@ -9274,7 +9317,7 @@
       <c r="K20" s="162"/>
       <c r="L20" s="215">
         <f t="shared" si="2"/>
-        <v>-157374.54116999998</v>
+        <v>-141098.94224999999</v>
       </c>
       <c r="M20" s="160"/>
       <c r="N20" s="215"/>
@@ -9303,7 +9346,7 @@
       </c>
       <c r="H21" s="155">
         <f>futuros!B7</f>
-        <v>330.15</v>
+        <v>322.5</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="162">
@@ -9312,7 +9355,7 @@
       <c r="K21" s="162"/>
       <c r="L21" s="215">
         <f t="shared" si="2"/>
-        <v>-99059.895269999877</v>
+        <v>-73240.195139999967</v>
       </c>
       <c r="M21" s="160"/>
       <c r="N21" s="215"/>
@@ -9340,7 +9383,7 @@
       </c>
       <c r="H22" s="155">
         <f>futuros!B7</f>
-        <v>330.15</v>
+        <v>322.5</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="162">
@@ -9349,7 +9392,7 @@
       <c r="K22" s="162"/>
       <c r="L22" s="215">
         <f t="shared" si="2"/>
-        <v>-23250.855599999999</v>
+        <v>-300.01104000006819</v>
       </c>
       <c r="M22" s="160"/>
       <c r="N22" s="215"/>
@@ -9377,7 +9420,7 @@
       </c>
       <c r="H23" s="155">
         <f>futuros!B7</f>
-        <v>330.15</v>
+        <v>322.5</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="162">
@@ -9386,7 +9429,7 @@
       <c r="K23" s="162"/>
       <c r="L23" s="215">
         <f t="shared" si="2"/>
-        <v>-68852.533679999964</v>
+        <v>-45901.689120000032</v>
       </c>
       <c r="M23" s="160"/>
       <c r="N23" s="215"/>
@@ -9415,7 +9458,7 @@
       </c>
       <c r="H24" s="217">
         <f>futuros!B7</f>
-        <v>330.15</v>
+        <v>322.5</v>
       </c>
       <c r="I24" s="208"/>
       <c r="J24" s="219">
@@ -9424,7 +9467,7 @@
       <c r="K24" s="219"/>
       <c r="L24" s="220">
         <f t="shared" si="2"/>
-        <v>-442591.28675999976</v>
+        <v>-362263.3308</v>
       </c>
       <c r="M24" s="218"/>
       <c r="N24" s="220"/>
@@ -9453,7 +9496,7 @@
       </c>
       <c r="H25" s="155">
         <f>futuros!B12</f>
-        <v>292.39999999999998</v>
+        <v>290.35000000000002</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="162">
@@ -9462,7 +9505,7 @@
       <c r="K25" s="162"/>
       <c r="L25" s="215">
         <f t="shared" si="2"/>
-        <v>-179031.58811999991</v>
+        <v>-170575.02693000008</v>
       </c>
       <c r="M25" s="160"/>
       <c r="N25" s="215"/>
@@ -9488,7 +9531,7 @@
       </c>
       <c r="H26" s="155">
         <f>futuros!B12</f>
-        <v>292.39999999999998</v>
+        <v>290.35000000000002</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="162">
@@ -9497,7 +9540,7 @@
       <c r="K26" s="162"/>
       <c r="L26" s="215">
         <f t="shared" ref="L26" si="8">D26*(G26-H26)*1.3228</f>
-        <v>-172206.33695999993</v>
+        <v>-166056.11064000006</v>
       </c>
       <c r="M26" s="160"/>
       <c r="N26" s="215"/>
@@ -9523,7 +9566,7 @@
       </c>
       <c r="H27" s="155">
         <f>futuros!B12</f>
-        <v>292.39999999999998</v>
+        <v>290.35000000000002</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="162">
@@ -9532,7 +9575,7 @@
       <c r="K27" s="162"/>
       <c r="L27" s="215">
         <f t="shared" ref="L27" si="10">D27*(G27-H27)*1.3228</f>
-        <v>-77627.856599999956</v>
+        <v>-73783.965150000033</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -9556,7 +9599,7 @@
       </c>
       <c r="H28" s="155">
         <f>futuros!B12</f>
-        <v>292.39999999999998</v>
+        <v>290.35000000000002</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="162">
@@ -9565,14 +9608,13 @@
       <c r="K28" s="162"/>
       <c r="L28" s="215">
         <f t="shared" ref="L28" si="12">D28*(G28-H28)*1.3228</f>
-        <v>-55127.028599999961</v>
+        <v>-51283.137150000039</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="E7:E13" numberStoredAsText="1"/>
-    <ignoredError sqref="F19" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -10297,10 +10339,10 @@
       <c r="M3" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="N3" s="221" t="s">
+      <c r="N3" s="229" t="s">
         <v>112</v>
       </c>
-      <c r="O3" s="221"/>
+      <c r="O3" s="229"/>
       <c r="P3" s="55" t="s">
         <v>113</v>
       </c>
@@ -13381,8 +13423,8 @@
       <c r="K74" s="83"/>
       <c r="L74" s="83"/>
       <c r="M74" s="83"/>
-      <c r="N74" s="222"/>
-      <c r="O74" s="222"/>
+      <c r="N74" s="230"/>
+      <c r="O74" s="230"/>
       <c r="P74" s="83"/>
       <c r="Q74" s="83"/>
       <c r="R74" s="83"/>
@@ -15739,8 +15781,8 @@
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="223"/>
-      <c r="C9" s="224"/>
+      <c r="B9" s="231"/>
+      <c r="C9" s="232"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
         <v>48</v>
@@ -16342,10 +16384,10 @@
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B43" s="41"/>
-      <c r="C43" s="225" t="s">
+      <c r="C43" s="233" t="s">
         <v>74</v>
       </c>
-      <c r="D43" s="225"/>
+      <c r="D43" s="233"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B44" s="42"/>
@@ -16355,10 +16397,10 @@
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B45" s="43"/>
-      <c r="C45" s="225" t="s">
+      <c r="C45" s="233" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="225"/>
+      <c r="D45" s="233"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B46" s="44"/>

</xml_diff>

<commit_message>
Atualizacao 01/12 + dois contratos para 3 Corações
</commit_message>
<xml_diff>
--- a/vendas_cafe_em_reais.xlsx
+++ b/vendas_cafe_em_reais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotocastro/PycharmProjects/Vendas Cafe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBC6320-6CF7-364B-AB8D-96878F59DA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7058749C-3638-3D47-B4C0-4DDB6BA75338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="680" windowWidth="21340" windowHeight="18440" activeTab="1" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
+    <workbookView xWindow="4420" yWindow="680" windowWidth="24980" windowHeight="18440" activeTab="1" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2 (2)" sheetId="16" state="hidden" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="CashFlow_Edson_Luiz" sheetId="3" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Q$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Q$80</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'VENDA CAFÉ 220125'!$A$3:$Z$61</definedName>
     <definedName name="LITRAGEM" localSheetId="7">#REF!</definedName>
     <definedName name="LITRAGEM" localSheetId="5">#REF!</definedName>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="365">
   <si>
     <t>026/24</t>
   </si>
@@ -1156,6 +1156,15 @@
   </si>
   <si>
     <t>WWTrading Worldwide</t>
+  </si>
+  <si>
+    <t>079/25</t>
+  </si>
+  <si>
+    <t>080/25</t>
+  </si>
+  <si>
+    <t>Café 3 Corações</t>
   </si>
 </sst>
 </file>
@@ -1557,7 +1566,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="235">
+  <cellXfs count="234">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2092,9 +2101,6 @@
     <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2702,26 +2708,26 @@
       </c>
       <c r="L6" s="177">
         <f>futuros!B2</f>
-        <v>399.9</v>
+        <v>407.1</v>
       </c>
       <c r="M6" s="177">
         <f>(L6+H6)*1.3228</f>
-        <v>568.67171999999994</v>
+        <v>578.19587999999999</v>
       </c>
       <c r="N6" s="167">
         <f>(E6*(M6+H6))</f>
-        <v>191574.95039999997</v>
+        <v>194622.68160000001</v>
       </c>
       <c r="O6" s="178">
         <v>5.7</v>
       </c>
       <c r="P6" s="167">
         <f t="shared" ref="P6:P16" si="1">M6*O6</f>
-        <v>3241.4288039999997</v>
+        <v>3295.716516</v>
       </c>
       <c r="Q6" s="167">
         <f t="shared" ref="Q6:Q16" si="2">P6*E6</f>
-        <v>1037257.2172799999</v>
+        <v>1054629.2851199999</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
@@ -2758,26 +2764,26 @@
       </c>
       <c r="L7" s="177">
         <f>L6</f>
-        <v>399.9</v>
+        <v>407.1</v>
       </c>
       <c r="M7" s="177">
         <f>(L7+H7)*1.3228</f>
-        <v>568.67171999999994</v>
+        <v>578.19587999999999</v>
       </c>
       <c r="N7" s="167">
         <f>(E7*(M7+H7))</f>
-        <v>191574.95039999997</v>
+        <v>194622.68160000001</v>
       </c>
       <c r="O7" s="178">
         <v>5.7</v>
       </c>
       <c r="P7" s="167">
         <f t="shared" si="1"/>
-        <v>3241.4288039999997</v>
+        <v>3295.716516</v>
       </c>
       <c r="Q7" s="167">
         <f t="shared" si="2"/>
-        <v>1037257.2172799999</v>
+        <v>1054629.2851199999</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
@@ -2814,26 +2820,26 @@
       </c>
       <c r="L8" s="177">
         <f>L7</f>
-        <v>399.9</v>
+        <v>407.1</v>
       </c>
       <c r="M8" s="177">
         <f>(L8+H8)*1.3228</f>
-        <v>568.67171999999994</v>
+        <v>578.19587999999999</v>
       </c>
       <c r="N8" s="167">
         <f>(E8*(M8+H8))</f>
-        <v>191574.95039999997</v>
+        <v>194622.68160000001</v>
       </c>
       <c r="O8" s="178">
         <v>5.7</v>
       </c>
       <c r="P8" s="167">
         <f t="shared" si="1"/>
-        <v>3241.4288039999997</v>
+        <v>3295.716516</v>
       </c>
       <c r="Q8" s="167">
         <f t="shared" si="2"/>
-        <v>1037257.2172799999</v>
+        <v>1054629.2851199999</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
@@ -2870,26 +2876,26 @@
       </c>
       <c r="L9" s="177">
         <f>futuros!B2</f>
-        <v>399.9</v>
+        <v>407.1</v>
       </c>
       <c r="M9" s="177">
         <f>(L9+H9)*1.3228</f>
-        <v>568.67171999999994</v>
+        <v>578.19587999999999</v>
       </c>
       <c r="N9" s="167">
         <f>(E9*(M9+H9))</f>
-        <v>191574.95039999997</v>
+        <v>194622.68160000001</v>
       </c>
       <c r="O9" s="178">
         <v>5.7</v>
       </c>
       <c r="P9" s="167">
         <f t="shared" si="1"/>
-        <v>3241.4288039999997</v>
+        <v>3295.716516</v>
       </c>
       <c r="Q9" s="167">
         <f t="shared" si="2"/>
-        <v>1037257.2172799999</v>
+        <v>1054629.2851199999</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
@@ -2926,26 +2932,26 @@
       </c>
       <c r="L10" s="177">
         <f>futuros!B3</f>
-        <v>369.4</v>
+        <v>375.6</v>
       </c>
       <c r="M10" s="177">
         <f>(L10+H10)*1.3228</f>
-        <v>528.32632000000001</v>
+        <v>536.52768000000003</v>
       </c>
       <c r="N10" s="167">
         <f>(E10*(M10+H10))</f>
-        <v>178664.42240000001</v>
+        <v>181288.85760000002</v>
       </c>
       <c r="O10" s="178">
         <v>5.7</v>
       </c>
       <c r="P10" s="167">
         <f t="shared" si="1"/>
-        <v>3011.460024</v>
+        <v>3058.2077760000002</v>
       </c>
       <c r="Q10" s="167">
         <f t="shared" si="2"/>
-        <v>963667.20767999999</v>
+        <v>978626.48832</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
@@ -2982,26 +2988,26 @@
       </c>
       <c r="L11" s="177">
         <f>futuros!B2</f>
-        <v>399.9</v>
+        <v>407.1</v>
       </c>
       <c r="M11" s="177">
         <f t="shared" ref="M11:M16" si="4">(L11+H11)*1.3228</f>
-        <v>566.02611999999999</v>
+        <v>575.55028000000004</v>
       </c>
       <c r="N11" s="167">
         <f t="shared" ref="N11:N16" si="5">(E11*(M11+H11))</f>
-        <v>190088.3584</v>
+        <v>193136.08960000001</v>
       </c>
       <c r="O11" s="178">
         <v>5.7</v>
       </c>
       <c r="P11" s="167">
         <f t="shared" si="1"/>
-        <v>3226.348884</v>
+        <v>3280.6365960000003</v>
       </c>
       <c r="Q11" s="167">
         <f t="shared" si="2"/>
-        <v>1032431.6428799999</v>
+        <v>1049803.7107200001</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
@@ -3038,26 +3044,26 @@
       </c>
       <c r="L12" s="177">
         <f>futuros!B2</f>
-        <v>399.9</v>
+        <v>407.1</v>
       </c>
       <c r="M12" s="177">
         <f t="shared" si="4"/>
-        <v>566.02611999999999</v>
+        <v>575.55028000000004</v>
       </c>
       <c r="N12" s="167">
         <f t="shared" si="5"/>
-        <v>190088.3584</v>
+        <v>193136.08960000001</v>
       </c>
       <c r="O12" s="178">
         <v>5.7</v>
       </c>
       <c r="P12" s="167">
         <f t="shared" si="1"/>
-        <v>3226.348884</v>
+        <v>3280.6365960000003</v>
       </c>
       <c r="Q12" s="167">
         <f t="shared" si="2"/>
-        <v>1032431.6428799999</v>
+        <v>1049803.7107200001</v>
       </c>
     </row>
     <row r="13" spans="2:20" s="166" customFormat="1" x14ac:dyDescent="0.25">
@@ -3094,26 +3100,26 @@
       </c>
       <c r="L13" s="177">
         <f>futuros!B3</f>
-        <v>369.4</v>
+        <v>375.6</v>
       </c>
       <c r="M13" s="177">
         <f t="shared" si="4"/>
-        <v>525.68071999999995</v>
+        <v>533.88207999999997</v>
       </c>
       <c r="N13" s="167">
         <f t="shared" si="5"/>
-        <v>177177.83039999998</v>
+        <v>179802.26559999998</v>
       </c>
       <c r="O13" s="178">
         <v>5.7</v>
       </c>
       <c r="P13" s="167">
         <f t="shared" si="1"/>
-        <v>2996.3801039999998</v>
+        <v>3043.1278560000001</v>
       </c>
       <c r="Q13" s="167">
         <f t="shared" si="2"/>
-        <v>958841.63327999995</v>
+        <v>973800.91391999996</v>
       </c>
       <c r="R13" s="163"/>
       <c r="S13" s="163"/>
@@ -3153,26 +3159,26 @@
       </c>
       <c r="L14" s="177">
         <f>futuros!B4</f>
-        <v>351.85</v>
+        <v>358.65</v>
       </c>
       <c r="M14" s="177">
         <f t="shared" si="4"/>
-        <v>502.46558000000005</v>
+        <v>511.46061999999995</v>
       </c>
       <c r="N14" s="167">
         <f t="shared" si="5"/>
-        <v>169748.98560000001</v>
+        <v>172627.39839999998</v>
       </c>
       <c r="O14" s="178">
         <v>5.7</v>
       </c>
       <c r="P14" s="167">
         <f t="shared" si="1"/>
-        <v>2864.0538060000003</v>
+        <v>2915.3255339999996</v>
       </c>
       <c r="Q14" s="167">
         <f t="shared" si="2"/>
-        <v>916497.21792000008</v>
+        <v>932904.17087999987</v>
       </c>
       <c r="R14" s="163"/>
       <c r="S14" s="163"/>
@@ -3212,26 +3218,26 @@
       </c>
       <c r="L15" s="177">
         <f>futuros!B3</f>
-        <v>369.4</v>
+        <v>375.6</v>
       </c>
       <c r="M15" s="177">
         <f t="shared" si="4"/>
-        <v>459.54071999999996</v>
+        <v>467.74208000000004</v>
       </c>
       <c r="N15" s="167">
         <f t="shared" si="5"/>
-        <v>140013.03039999999</v>
+        <v>142637.46560000003</v>
       </c>
       <c r="O15" s="178">
         <v>5.7</v>
       </c>
       <c r="P15" s="167">
         <f t="shared" si="1"/>
-        <v>2619.3821039999998</v>
+        <v>2666.1298560000005</v>
       </c>
       <c r="Q15" s="167">
         <f t="shared" si="2"/>
-        <v>838202.27327999996</v>
+        <v>853161.55392000009</v>
       </c>
       <c r="R15" s="163"/>
       <c r="S15" s="163"/>
@@ -3271,26 +3277,26 @@
       </c>
       <c r="L16" s="177">
         <f>futuros!B2</f>
-        <v>399.9</v>
+        <v>407.1</v>
       </c>
       <c r="M16" s="177">
         <f t="shared" si="4"/>
-        <v>599.09611999999993</v>
+        <v>608.62027999999998</v>
       </c>
       <c r="N16" s="167">
         <f t="shared" si="5"/>
-        <v>208670.75839999999</v>
+        <v>211718.4896</v>
       </c>
       <c r="O16" s="178">
         <v>5.7</v>
       </c>
       <c r="P16" s="167">
         <f t="shared" si="1"/>
-        <v>3414.8478839999998</v>
+        <v>3469.1355960000001</v>
       </c>
       <c r="Q16" s="167">
         <f t="shared" si="2"/>
-        <v>1092751.3228799999</v>
+        <v>1110123.39072</v>
       </c>
       <c r="R16" s="163"/>
       <c r="S16" s="163"/>
@@ -3417,20 +3423,20 @@
       <c r="L19" s="179"/>
       <c r="M19" s="182">
         <f>N19/E19</f>
-        <v>557.70346999999992</v>
+        <v>564.86548714285721</v>
       </c>
       <c r="N19" s="183">
         <f>SUM(N5:N18)</f>
-        <v>2498511.5455999998</v>
+        <v>2530597.3824000005</v>
       </c>
       <c r="O19" s="184"/>
       <c r="P19" s="185">
         <f>Q19/E19</f>
-        <v>3059.6169218571426</v>
+        <v>3100.4404195714283</v>
       </c>
       <c r="Q19" s="183">
         <f>SUM(Q5:Q18)</f>
-        <v>13707083.80992</v>
+        <v>13889973.07968</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
@@ -3553,7 +3559,7 @@
       </c>
       <c r="I25" s="177">
         <f>futuros!B2</f>
-        <v>399.9</v>
+        <v>407.1</v>
       </c>
       <c r="K25" s="163"/>
       <c r="L25" s="197">
@@ -3562,7 +3568,7 @@
       <c r="M25" s="163"/>
       <c r="N25" s="198">
         <f>(H25-I25)*1.3228*D25</f>
-        <v>-1466277.7070339997</v>
+        <v>-1514069.4657059999</v>
       </c>
       <c r="O25" s="178">
         <f>O5</f>
@@ -3570,7 +3576,7 @@
       </c>
       <c r="Q25" s="198">
         <f>N25*O25</f>
-        <v>-8357782.9300937988</v>
+        <v>-8630195.9545242004</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
@@ -3595,7 +3601,7 @@
       </c>
       <c r="I26" s="177">
         <f>I25</f>
-        <v>399.9</v>
+        <v>407.1</v>
       </c>
       <c r="K26" s="163"/>
       <c r="L26" s="197">
@@ -3604,7 +3610,7 @@
       <c r="M26" s="163"/>
       <c r="N26" s="198">
         <f>(H26-I26)*1.3228*D26</f>
-        <v>-534994.68707999995</v>
+        <v>-553895.38260000013</v>
       </c>
       <c r="O26" s="178">
         <f>O6</f>
@@ -3612,7 +3618,7 @@
       </c>
       <c r="Q26" s="198">
         <f t="shared" ref="Q26:Q27" si="6">N26*O26</f>
-        <v>-3049469.7163559999</v>
+        <v>-3157203.6808200008</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
@@ -3636,7 +3642,7 @@
       </c>
       <c r="I27" s="200">
         <f>I26</f>
-        <v>399.9</v>
+        <v>407.1</v>
       </c>
       <c r="K27" s="163"/>
       <c r="L27" s="197">
@@ -3645,7 +3651,7 @@
       <c r="M27" s="163"/>
       <c r="N27" s="198">
         <f>(H27-I27)*1.3228*D27</f>
-        <v>-706383.49395599996</v>
+        <v>-735004.54717200005</v>
       </c>
       <c r="O27" s="178">
         <f>O7</f>
@@ -3653,7 +3659,7 @@
       </c>
       <c r="Q27" s="198">
         <f t="shared" si="6"/>
-        <v>-4026385.9155492</v>
+        <v>-4189525.9188804002</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
@@ -3676,13 +3682,13 @@
       <c r="M28" s="202"/>
       <c r="N28" s="202">
         <f>SUM(N25:N27)</f>
-        <v>-2707655.8880699999</v>
+        <v>-2802969.3954779999</v>
       </c>
       <c r="O28" s="201"/>
       <c r="P28" s="201"/>
       <c r="Q28" s="202">
         <f>SUM(Q25:Q27)</f>
-        <v>-15433638.561998999</v>
+        <v>-15976925.554224603</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
@@ -4366,7 +4372,7 @@
       </c>
       <c r="I57" s="177">
         <f>futuros!B7</f>
-        <v>319.5</v>
+        <v>324.8</v>
       </c>
       <c r="K57" s="178">
         <f>O8</f>
@@ -4378,7 +4384,7 @@
       <c r="M57" s="198"/>
       <c r="N57" s="198">
         <f>(H57-I57)*1.3228*D57</f>
-        <v>-63114.822539999957</v>
+        <v>-81002.980800000005</v>
       </c>
       <c r="O57" s="166">
         <f>O25</f>
@@ -4386,7 +4392,7 @@
       </c>
       <c r="Q57" s="198">
         <f>N57*O57</f>
-        <v>-359754.48847799975</v>
+        <v>-461716.99056000006</v>
       </c>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.25">
@@ -4410,7 +4416,7 @@
       </c>
       <c r="I58" s="177">
         <f>I57</f>
-        <v>319.5</v>
+        <v>324.8</v>
       </c>
       <c r="K58" s="178">
         <f>O9</f>
@@ -4422,7 +4428,7 @@
       <c r="M58" s="198"/>
       <c r="N58" s="198">
         <f>(H58-I58)*1.3228*D58</f>
-        <v>8700.320159999932</v>
+        <v>-7200.2649600001023</v>
       </c>
       <c r="O58" s="166">
         <f>O26</f>
@@ -4430,7 +4436,7 @@
       </c>
       <c r="Q58" s="198">
         <f>N58*O58</f>
-        <v>49591.824911999611</v>
+        <v>-41041.510272000582</v>
       </c>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.25">
@@ -4453,13 +4459,13 @@
       <c r="M59" s="201"/>
       <c r="N59" s="202">
         <f>SUM(N56:N58)</f>
-        <v>-54414.502380000027</v>
+        <v>-88203.245760000107</v>
       </c>
       <c r="O59" s="201"/>
       <c r="P59" s="201"/>
       <c r="Q59" s="202">
         <f>SUM(Q56:Q58)</f>
-        <v>-310162.66356600012</v>
+        <v>-502758.50083200063</v>
       </c>
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.25">
@@ -4597,11 +4603,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T78"/>
+  <dimension ref="A1:T80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I62" sqref="I62"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -8047,7 +8053,7 @@
         <v>2750</v>
       </c>
       <c r="Q69" s="3">
-        <f t="shared" ref="Q69:Q75" si="7">E69*P69</f>
+        <f t="shared" ref="Q69:Q77" si="7">E69*P69</f>
         <v>13750</v>
       </c>
     </row>
@@ -8273,86 +8279,86 @@
       <c r="A75" s="2">
         <v>2025</v>
       </c>
+      <c r="B75" s="2" t="s">
+        <v>362</v>
+      </c>
       <c r="C75" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D75" s="159" t="s">
-        <v>331</v>
+        <v>364</v>
       </c>
       <c r="E75" s="213">
-        <f>2400-E66-E65-E67-E69-E70-E71-E72-E73-E74</f>
-        <v>2300</v>
+        <v>161</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H75" s="2">
-        <v>0</v>
+        <v>289</v>
       </c>
       <c r="I75" s="158">
-        <v>45992</v>
+        <v>46001</v>
       </c>
       <c r="J75" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K75" s="158">
-        <v>45992</v>
-      </c>
-      <c r="L75" s="158"/>
+        <f t="shared" ref="K75:K76" si="9">I75</f>
+        <v>46001</v>
+      </c>
+      <c r="L75" s="155"/>
+      <c r="M75" s="155"/>
       <c r="N75" s="3"/>
       <c r="P75" s="3">
-        <v>1600</v>
+        <v>2600</v>
       </c>
       <c r="Q75" s="3">
-        <f t="shared" si="7"/>
-        <v>3680000</v>
+        <f t="shared" ref="Q75:Q76" si="10">E75*P75</f>
+        <v>418600</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>2025</v>
       </c>
+      <c r="B76" s="2" t="s">
+        <v>363</v>
+      </c>
       <c r="C76" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D76" s="159" t="s">
-        <v>331</v>
-      </c>
-      <c r="E76" s="2">
-        <f>0.7*8000-4800-E77-E78-E68</f>
-        <v>286.49999999999994</v>
+        <v>364</v>
+      </c>
+      <c r="E76" s="213">
+        <v>75</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H76" s="2">
-        <v>0</v>
+        <v>289</v>
       </c>
       <c r="I76" s="158">
-        <v>45992</v>
+        <v>46001</v>
       </c>
       <c r="J76" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K76" s="158">
-        <v>45992</v>
-      </c>
-      <c r="L76" s="155">
-        <v>325</v>
-      </c>
-      <c r="M76" s="155">
-        <f>(L76+H76)*1.3228</f>
-        <v>429.90999999999997</v>
-      </c>
-      <c r="N76" s="3">
-        <f>M76*E76</f>
-        <v>123169.21499999997</v>
+        <f t="shared" si="9"/>
+        <v>46001</v>
+      </c>
+      <c r="L76" s="155"/>
+      <c r="M76" s="155"/>
+      <c r="N76" s="3"/>
+      <c r="P76" s="3">
+        <v>2600</v>
+      </c>
+      <c r="Q76" s="3">
+        <f t="shared" si="10"/>
+        <v>195000</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
@@ -8360,13 +8366,14 @@
         <v>2025</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D77" s="159" t="s">
         <v>331</v>
       </c>
-      <c r="E77" s="2">
-        <v>64.5</v>
+      <c r="E77" s="213">
+        <f>2400-E66-E65-E67-E69-E70-E71-E72-E73-E74-E75-E76</f>
+        <v>2064</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>32</v>
@@ -8378,24 +8385,22 @@
         <v>0</v>
       </c>
       <c r="I77" s="158">
-        <v>45992</v>
+        <v>46023</v>
       </c>
       <c r="J77" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K77" s="158">
-        <v>45992</v>
-      </c>
-      <c r="L77" s="155">
-        <v>330</v>
-      </c>
-      <c r="M77" s="155">
-        <f>(L77+H77)*1.3228</f>
-        <v>436.524</v>
-      </c>
-      <c r="N77" s="3">
-        <f>M77*E77</f>
-        <v>28155.797999999999</v>
+        <v>46023</v>
+      </c>
+      <c r="L77" s="158"/>
+      <c r="N77" s="3"/>
+      <c r="P77" s="3">
+        <v>1600</v>
+      </c>
+      <c r="Q77" s="3">
+        <f t="shared" si="7"/>
+        <v>3302400</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
@@ -8408,9 +8413,9 @@
       <c r="D78" s="159" t="s">
         <v>331</v>
       </c>
-      <c r="E78" s="213">
-        <f>449-E68</f>
-        <v>115.66666666666669</v>
+      <c r="E78" s="2">
+        <f>0.7*8000-4800-E79-E80-E68</f>
+        <v>286.49999999999994</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>32</v>
@@ -8422,13 +8427,13 @@
         <v>0</v>
       </c>
       <c r="I78" s="158">
-        <v>46082</v>
+        <v>46023</v>
       </c>
       <c r="J78" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K78" s="158">
-        <v>46082</v>
+        <v>46023</v>
       </c>
       <c r="L78" s="155">
         <v>325</v>
@@ -8439,13 +8444,100 @@
       </c>
       <c r="N78" s="3">
         <f>M78*E78</f>
+        <v>123169.21499999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A79" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D79" s="159" t="s">
+        <v>331</v>
+      </c>
+      <c r="E79" s="2">
+        <v>64.5</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H79" s="2">
+        <v>0</v>
+      </c>
+      <c r="I79" s="158">
+        <v>46023</v>
+      </c>
+      <c r="J79" s="2">
+        <v>1</v>
+      </c>
+      <c r="K79" s="158">
+        <v>46023</v>
+      </c>
+      <c r="L79" s="155">
+        <v>330</v>
+      </c>
+      <c r="M79" s="155">
+        <f>(L79+H79)*1.3228</f>
+        <v>436.524</v>
+      </c>
+      <c r="N79" s="3">
+        <f>M79*E79</f>
+        <v>28155.797999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D80" s="159" t="s">
+        <v>331</v>
+      </c>
+      <c r="E80" s="213">
+        <f>449-E68</f>
+        <v>115.66666666666669</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H80" s="2">
+        <v>0</v>
+      </c>
+      <c r="I80" s="158">
+        <v>46082</v>
+      </c>
+      <c r="J80" s="2">
+        <v>1</v>
+      </c>
+      <c r="K80" s="158">
+        <v>46082</v>
+      </c>
+      <c r="L80" s="155">
+        <v>325</v>
+      </c>
+      <c r="M80" s="155">
+        <f>(L80+H80)*1.3228</f>
+        <v>429.90999999999997</v>
+      </c>
+      <c r="N80" s="3">
+        <f>M80*E80</f>
         <v>49726.256666666668</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q78" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q78">
-      <sortCondition ref="B1:B78"/>
+  <autoFilter ref="A1:Q80" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q80">
+      <sortCondition ref="B1:B80"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -8485,7 +8577,7 @@
         <v>270</v>
       </c>
       <c r="D1" s="162">
-        <v>45985</v>
+        <v>45992</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8493,11 +8585,11 @@
         <v>46021</v>
       </c>
       <c r="B2" s="155">
-        <v>399.9</v>
+        <v>407.1</v>
       </c>
       <c r="C2" s="155">
         <f t="shared" ref="C2:C11" si="0">B2*1.3228</f>
-        <v>528.98771999999997</v>
+        <v>538.51188000000002</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8505,11 +8597,11 @@
         <v>46112</v>
       </c>
       <c r="B3" s="155">
-        <v>369.4</v>
+        <v>375.6</v>
       </c>
       <c r="C3" s="155">
         <f t="shared" si="0"/>
-        <v>488.64231999999998</v>
+        <v>496.84368000000001</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -8517,11 +8609,11 @@
         <v>46173</v>
       </c>
       <c r="B4" s="155">
-        <v>351.85</v>
+        <v>358.65</v>
       </c>
       <c r="C4" s="155">
         <f t="shared" si="0"/>
-        <v>465.42718000000002</v>
+        <v>474.42221999999998</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -8529,11 +8621,11 @@
         <v>46231</v>
       </c>
       <c r="B5" s="155">
-        <v>337.35</v>
+        <v>344.65</v>
       </c>
       <c r="C5" s="155">
         <f t="shared" si="0"/>
-        <v>446.24657999999999</v>
+        <v>455.90301999999997</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -8541,11 +8633,11 @@
         <v>46295</v>
       </c>
       <c r="B6" s="155">
-        <v>326.64999999999998</v>
+        <v>332.75</v>
       </c>
       <c r="C6" s="155">
         <f t="shared" si="0"/>
-        <v>432.09261999999995</v>
+        <v>440.1617</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -8553,11 +8645,11 @@
         <v>46386</v>
       </c>
       <c r="B7" s="155">
-        <v>319.5</v>
+        <v>324.8</v>
       </c>
       <c r="C7" s="155">
         <f t="shared" si="0"/>
-        <v>422.63459999999998</v>
+        <v>429.64544000000001</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -8565,11 +8657,11 @@
         <v>46477</v>
       </c>
       <c r="B8" s="155">
-        <v>315.45</v>
+        <v>325.89999999999998</v>
       </c>
       <c r="C8" s="155">
         <f t="shared" si="0"/>
-        <v>417.27725999999996</v>
+        <v>431.10051999999996</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8577,11 +8669,11 @@
         <v>46538</v>
       </c>
       <c r="B9" s="155">
-        <v>312.64999999999998</v>
+        <v>322.7</v>
       </c>
       <c r="C9" s="155">
         <f t="shared" si="0"/>
-        <v>413.57341999999994</v>
+        <v>426.86755999999997</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -8589,11 +8681,11 @@
         <v>46596</v>
       </c>
       <c r="B10" s="155">
-        <v>312</v>
+        <v>318.89999999999998</v>
       </c>
       <c r="C10" s="155">
         <f t="shared" si="0"/>
-        <v>412.71359999999999</v>
+        <v>421.84091999999998</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -8601,11 +8693,11 @@
         <v>46660</v>
       </c>
       <c r="B11" s="155">
-        <v>306.14999999999998</v>
+        <v>314.64999999999998</v>
       </c>
       <c r="C11" s="155">
         <f t="shared" si="0"/>
-        <v>404.97521999999998</v>
+        <v>416.21901999999994</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -8613,11 +8705,11 @@
         <v>46751</v>
       </c>
       <c r="B12" s="155">
-        <v>301.3</v>
+        <v>309.35000000000002</v>
       </c>
       <c r="C12" s="155">
         <f>B12*1.3228</f>
-        <v>398.55964</v>
+        <v>409.20818000000003</v>
       </c>
     </row>
   </sheetData>
@@ -8631,8 +8723,8 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22:D31"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L22" sqref="L22:L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8816,15 +8908,14 @@
         <v>45602</v>
       </c>
       <c r="L4" s="215">
-        <f t="shared" si="2"/>
-        <v>-329805.88641000004</v>
+        <f>N4/M4</f>
+        <v>-432777.9808400122</v>
       </c>
       <c r="M4" s="160">
         <v>5.7694000000000001</v>
       </c>
       <c r="N4" s="215">
-        <f t="shared" si="3"/>
-        <v>-1902782.0810538542</v>
+        <v>-2496869.2826583665</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -8864,15 +8955,14 @@
         <v>45602</v>
       </c>
       <c r="L5" s="215">
-        <f t="shared" si="2"/>
-        <v>-709788.61926000006</v>
+        <f>N5/M5</f>
+        <v>-855160.98786707607</v>
       </c>
       <c r="M5" s="160">
         <v>5.7694000000000001</v>
       </c>
       <c r="N5" s="215">
-        <f t="shared" si="3"/>
-        <v>-4095054.4599586446</v>
+        <v>-4933765.8034003088</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -9374,7 +9464,7 @@
         <f>D16*(G16-H16)*1.3228</f>
         <v>11775.433319999993</v>
       </c>
-      <c r="M16" s="222">
+      <c r="M16" s="160">
         <f>N16/L16</f>
         <v>5.3660513615816594</v>
       </c>
@@ -9600,43 +9690,43 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="223" t="s">
+      <c r="A22" s="222" t="s">
         <v>296</v>
       </c>
-      <c r="B22" s="223" t="s">
+      <c r="B22" s="222" t="s">
         <v>329</v>
       </c>
-      <c r="C22" s="224">
+      <c r="C22" s="223">
         <v>29487625</v>
       </c>
-      <c r="D22" s="225">
+      <c r="D22" s="224">
         <f t="shared" si="0"/>
         <v>1701</v>
       </c>
-      <c r="E22" s="225" t="s">
+      <c r="E22" s="224" t="s">
         <v>345</v>
       </c>
-      <c r="F22" s="226">
+      <c r="F22" s="225">
         <v>6</v>
       </c>
-      <c r="G22" s="226">
+      <c r="G22" s="225">
         <v>325</v>
       </c>
-      <c r="H22" s="226">
+      <c r="H22" s="225">
         <f>futuros!B3</f>
-        <v>369.4</v>
-      </c>
-      <c r="I22" s="224"/>
-      <c r="J22" s="227">
+        <v>375.6</v>
+      </c>
+      <c r="I22" s="223"/>
+      <c r="J22" s="226">
         <v>46063</v>
       </c>
-      <c r="K22" s="227"/>
-      <c r="L22" s="228">
+      <c r="K22" s="226"/>
+      <c r="L22" s="227">
         <f t="shared" si="2"/>
-        <v>-99903.676319999955</v>
-      </c>
-      <c r="M22" s="229"/>
-      <c r="N22" s="228"/>
+        <v>-113854.18968000004</v>
+      </c>
+      <c r="M22" s="228"/>
+      <c r="N22" s="227"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
@@ -9662,7 +9752,7 @@
       </c>
       <c r="H23" s="155">
         <f>futuros!B7</f>
-        <v>319.5</v>
+        <v>324.8</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="162">
@@ -9671,7 +9761,7 @@
       <c r="K23" s="162"/>
       <c r="L23" s="215">
         <f t="shared" si="2"/>
-        <v>-63114.822539999965</v>
+        <v>-81002.980800000005</v>
       </c>
       <c r="M23" s="160"/>
       <c r="N23" s="215"/>
@@ -9699,7 +9789,7 @@
       </c>
       <c r="H24" s="155">
         <f>futuros!B7</f>
-        <v>319.5</v>
+        <v>324.8</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="162">
@@ -9708,7 +9798,7 @@
       <c r="K24" s="162"/>
       <c r="L24" s="215">
         <f t="shared" si="2"/>
-        <v>8700.3201599999302</v>
+        <v>-7200.2649600001023</v>
       </c>
       <c r="M24" s="160"/>
       <c r="N24" s="215"/>
@@ -9736,7 +9826,7 @@
       </c>
       <c r="H25" s="155">
         <f>futuros!B7</f>
-        <v>319.5</v>
+        <v>324.8</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="162">
@@ -9745,7 +9835,7 @@
       <c r="K25" s="162"/>
       <c r="L25" s="215">
         <f t="shared" si="2"/>
-        <v>-36901.357920000031</v>
+        <v>-52801.943040000071</v>
       </c>
       <c r="M25" s="160"/>
       <c r="N25" s="215"/>
@@ -9774,7 +9864,7 @@
       </c>
       <c r="H26" s="217">
         <f>futuros!B7</f>
-        <v>319.5</v>
+        <v>324.8</v>
       </c>
       <c r="I26" s="208"/>
       <c r="J26" s="219">
@@ -9783,7 +9873,7 @@
       <c r="K26" s="219"/>
       <c r="L26" s="220">
         <f t="shared" si="2"/>
-        <v>-330762.1716</v>
+        <v>-386414.2195200001</v>
       </c>
       <c r="M26" s="218"/>
       <c r="N26" s="220"/>
@@ -9812,7 +9902,7 @@
       </c>
       <c r="H27" s="155">
         <f>futuros!B12</f>
-        <v>301.3</v>
+        <v>309.35000000000002</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="162">
@@ -9821,7 +9911,7 @@
       <c r="K27" s="162"/>
       <c r="L27" s="215">
         <f t="shared" si="2"/>
-        <v>-215745.43914000006</v>
+        <v>-248952.91113000008</v>
       </c>
       <c r="M27" s="160"/>
       <c r="N27" s="215"/>
@@ -9847,7 +9937,7 @@
       </c>
       <c r="H28" s="155">
         <f>futuros!B12</f>
-        <v>301.3</v>
+        <v>309.35000000000002</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="162">
@@ -9856,7 +9946,7 @@
       <c r="K28" s="162"/>
       <c r="L28" s="215">
         <f t="shared" ref="L28" si="7">D28*(G28-H28)*1.3228</f>
-        <v>-198907.31952000002</v>
+        <v>-223058.20824000007</v>
       </c>
       <c r="M28" s="160"/>
       <c r="N28" s="215"/>
@@ -9882,7 +9972,7 @@
       </c>
       <c r="H29" s="155">
         <f>futuros!B12</f>
-        <v>301.3</v>
+        <v>309.35000000000002</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="162">
@@ -9891,7 +9981,7 @@
       <c r="K29" s="162"/>
       <c r="L29" s="215">
         <f t="shared" ref="L29" si="9">D29*(G29-H29)*1.3228</f>
-        <v>-94315.97070000002</v>
+        <v>-109410.27615000003</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -9915,7 +10005,7 @@
       </c>
       <c r="H30" s="155">
         <f>futuros!B12</f>
-        <v>301.3</v>
+        <v>309.35000000000002</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="162">
@@ -9924,7 +10014,7 @@
       <c r="K30" s="162"/>
       <c r="L30" s="215">
         <f t="shared" ref="L30" si="11">D30*(G30-H30)*1.3228</f>
-        <v>-71815.142700000011</v>
+        <v>-86909.44815000004</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
@@ -9948,7 +10038,7 @@
       </c>
       <c r="H31" s="155">
         <f>futuros!B12</f>
-        <v>301.3</v>
+        <v>309.35000000000002</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="162">
@@ -9957,7 +10047,7 @@
       <c r="K31" s="162"/>
       <c r="L31" s="215">
         <f t="shared" ref="L31" si="13">D31*(G31-H31)*1.3228</f>
-        <v>9712.8574199999712</v>
+        <v>-11419.170210000058</v>
       </c>
     </row>
   </sheetData>
@@ -10689,10 +10779,10 @@
       <c r="M3" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="N3" s="230" t="s">
+      <c r="N3" s="229" t="s">
         <v>112</v>
       </c>
-      <c r="O3" s="230"/>
+      <c r="O3" s="229"/>
       <c r="P3" s="55" t="s">
         <v>113</v>
       </c>
@@ -13773,8 +13863,8 @@
       <c r="K74" s="83"/>
       <c r="L74" s="83"/>
       <c r="M74" s="83"/>
-      <c r="N74" s="231"/>
-      <c r="O74" s="231"/>
+      <c r="N74" s="230"/>
+      <c r="O74" s="230"/>
       <c r="P74" s="83"/>
       <c r="Q74" s="83"/>
       <c r="R74" s="83"/>
@@ -16131,8 +16221,8 @@
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="232"/>
-      <c r="C9" s="233"/>
+      <c r="B9" s="231"/>
+      <c r="C9" s="232"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
         <v>48</v>
@@ -16734,10 +16824,10 @@
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B43" s="41"/>
-      <c r="C43" s="234" t="s">
+      <c r="C43" s="233" t="s">
         <v>74</v>
       </c>
-      <c r="D43" s="234"/>
+      <c r="D43" s="233"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B44" s="42"/>
@@ -16747,10 +16837,10 @@
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B45" s="43"/>
-      <c r="C45" s="234" t="s">
+      <c r="C45" s="233" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="234"/>
+      <c r="D45" s="233"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B46" s="44"/>

</xml_diff>

<commit_message>
Atualizacao 29/12 e datas BL
</commit_message>
<xml_diff>
--- a/vendas_cafe_em_reais.xlsx
+++ b/vendas_cafe_em_reais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotocastro/PycharmProjects/Vendas Cafe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A415B8E2-3D36-EC4E-A522-1B95010FDFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3033C8C-410D-344D-BB09-F2DBB915F562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="660" windowWidth="25720" windowHeight="18460" activeTab="2" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
+    <workbookView xWindow="14720" yWindow="660" windowWidth="14680" windowHeight="18460" activeTab="1" xr2:uid="{AC82ADC5-E628-F847-8939-89BAF5623AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2 (2)" sheetId="16" state="hidden" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="CashFlow_Edson_Luiz" sheetId="3" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Q$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Q$85</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'VENDA CAFÉ 220125'!$A$3:$Z$61</definedName>
     <definedName name="LITRAGEM" localSheetId="7">#REF!</definedName>
     <definedName name="LITRAGEM" localSheetId="5">#REF!</definedName>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="372">
   <si>
     <t>026/24</t>
   </si>
@@ -1174,6 +1174,18 @@
   </si>
   <si>
     <t>083/25</t>
+  </si>
+  <si>
+    <t>061A/25</t>
+  </si>
+  <si>
+    <t>061B/25</t>
+  </si>
+  <si>
+    <t>063A/25</t>
+  </si>
+  <si>
+    <t>063B/25</t>
   </si>
 </sst>
 </file>
@@ -4612,11 +4624,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:T83"/>
+  <dimension ref="A1:T85"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q77" sqref="Q77:Q79"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I80" sqref="I80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -6964,7 +6976,7 @@
         <v>18316.27</v>
       </c>
     </row>
-    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>2025</v>
       </c>
@@ -7106,11 +7118,11 @@
         <v>571.44960000000003</v>
       </c>
       <c r="N48" s="3">
-        <f t="shared" ref="N48:N62" si="4">M48*E48</f>
+        <f t="shared" ref="N48:N64" si="4">M48*E48</f>
         <v>182863.872</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>2025</v>
       </c>
@@ -7157,7 +7169,7 @@
         <v>182863.872</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>2025</v>
       </c>
@@ -7204,7 +7216,7 @@
         <v>152386.56</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>2025</v>
       </c>
@@ -7251,7 +7263,7 @@
         <v>187520.128</v>
       </c>
     </row>
-    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>2025</v>
       </c>
@@ -7298,7 +7310,7 @@
         <v>152386.56</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>2025</v>
       </c>
@@ -7340,7 +7352,7 @@
         <v>117120</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>2025</v>
       </c>
@@ -7382,7 +7394,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>2026</v>
       </c>
@@ -7425,7 +7437,7 @@
         <v>135360</v>
       </c>
     </row>
-    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>2026</v>
       </c>
@@ -7468,7 +7480,7 @@
         <v>139520</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>2025</v>
       </c>
@@ -7500,14 +7512,14 @@
         <v>1</v>
       </c>
       <c r="K57" s="158">
-        <f t="shared" ref="K57:K62" si="5">I57+65</f>
+        <f t="shared" ref="K57:K64" si="5">I57+65</f>
         <v>46018</v>
       </c>
       <c r="L57" s="155">
         <v>402</v>
       </c>
       <c r="M57" s="155">
-        <f t="shared" ref="M57:M62" si="6">(L57+H57)*1.3228</f>
+        <f t="shared" ref="M57:M64" si="6">(L57+H57)*1.3228</f>
         <v>568.80399999999997</v>
       </c>
       <c r="N57" s="3">
@@ -7515,12 +7527,12 @@
         <v>182017.28</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>2025</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>284</v>
+        <v>368</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>42</v>
@@ -7547,7 +7559,7 @@
         <v>1</v>
       </c>
       <c r="K58" s="158">
-        <f t="shared" si="5"/>
+        <f>I58+65</f>
         <v>46056</v>
       </c>
       <c r="L58" s="155">
@@ -7562,12 +7574,12 @@
         <v>149423.48800000001</v>
       </c>
     </row>
-    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>2025</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>285</v>
+        <v>369</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>42</v>
@@ -7588,61 +7600,61 @@
         <v>28</v>
       </c>
       <c r="I59" s="158">
-        <v>46023</v>
+        <v>46008</v>
       </c>
       <c r="J59" s="2">
         <v>1</v>
       </c>
       <c r="K59" s="158">
+        <f>I59+65</f>
+        <v>46073</v>
+      </c>
+      <c r="L59" s="155">
+        <v>325</v>
+      </c>
+      <c r="M59" s="155">
+        <f t="shared" ref="M59" si="7">(L59+H59)*1.3228</f>
+        <v>466.94839999999999</v>
+      </c>
+      <c r="N59" s="3">
+        <f t="shared" ref="N59" si="8">M59*E59</f>
+        <v>149423.48800000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="159" t="s">
+        <v>264</v>
+      </c>
+      <c r="E60" s="2">
+        <v>320</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H60" s="2">
+        <v>28</v>
+      </c>
+      <c r="I60" s="158">
+        <v>46023</v>
+      </c>
+      <c r="J60" s="2">
+        <v>1</v>
+      </c>
+      <c r="K60" s="158">
         <f t="shared" si="5"/>
         <v>46088</v>
-      </c>
-      <c r="L59" s="155">
-        <v>325</v>
-      </c>
-      <c r="M59" s="155">
-        <f t="shared" si="6"/>
-        <v>466.94839999999999</v>
-      </c>
-      <c r="N59" s="3">
-        <f t="shared" si="4"/>
-        <v>149423.48800000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="2">
-        <v>2025</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D60" s="159" t="s">
-        <v>264</v>
-      </c>
-      <c r="E60" s="2">
-        <v>320</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H60" s="2">
-        <v>28</v>
-      </c>
-      <c r="I60" s="158">
-        <v>46082</v>
-      </c>
-      <c r="J60" s="2">
-        <v>1</v>
-      </c>
-      <c r="K60" s="158">
-        <f t="shared" si="5"/>
-        <v>46147</v>
       </c>
       <c r="L60" s="155">
         <v>325</v>
@@ -7656,12 +7668,12 @@
         <v>149423.48800000001</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>2025</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>287</v>
+        <v>370</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>42</v>
@@ -7673,42 +7685,42 @@
         <v>320</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="H61" s="2">
-        <v>-22</v>
+        <v>28</v>
       </c>
       <c r="I61" s="158">
-        <v>45992</v>
+        <v>45990</v>
       </c>
       <c r="J61" s="2">
         <v>1</v>
       </c>
       <c r="K61" s="158">
         <f t="shared" si="5"/>
-        <v>46057</v>
+        <v>46055</v>
       </c>
       <c r="L61" s="155">
         <v>325</v>
       </c>
       <c r="M61" s="155">
         <f t="shared" si="6"/>
-        <v>400.80840000000001</v>
+        <v>466.94839999999999</v>
       </c>
       <c r="N61" s="3">
         <f t="shared" si="4"/>
-        <v>128258.68799999999</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+        <v>149423.48800000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>2025</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>288</v>
+        <v>371</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>42</v>
@@ -7723,229 +7735,233 @@
         <v>27</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>290</v>
+        <v>37</v>
       </c>
       <c r="H62" s="2">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="I62" s="158">
-        <v>45974</v>
+        <v>46008</v>
       </c>
       <c r="J62" s="2">
         <v>1</v>
       </c>
       <c r="K62" s="158">
+        <f t="shared" ref="K62" si="9">I62+65</f>
+        <v>46073</v>
+      </c>
+      <c r="L62" s="155">
+        <v>325</v>
+      </c>
+      <c r="M62" s="155">
+        <f t="shared" ref="M62" si="10">(L62+H62)*1.3228</f>
+        <v>466.94839999999999</v>
+      </c>
+      <c r="N62" s="3">
+        <f t="shared" ref="N62" si="11">M62*E62</f>
+        <v>149423.48800000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63" s="159" t="s">
+        <v>264</v>
+      </c>
+      <c r="E63" s="2">
+        <v>320</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H63" s="2">
+        <v>-22</v>
+      </c>
+      <c r="I63" s="158">
+        <v>45992</v>
+      </c>
+      <c r="J63" s="2">
+        <v>1</v>
+      </c>
+      <c r="K63" s="158">
+        <f t="shared" si="5"/>
+        <v>46057</v>
+      </c>
+      <c r="L63" s="155">
+        <v>325</v>
+      </c>
+      <c r="M63" s="155">
+        <f t="shared" si="6"/>
+        <v>400.80840000000001</v>
+      </c>
+      <c r="N63" s="3">
+        <f t="shared" si="4"/>
+        <v>128258.68799999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D64" s="159" t="s">
+        <v>264</v>
+      </c>
+      <c r="E64" s="2">
+        <v>320</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="H64" s="2">
+        <v>53</v>
+      </c>
+      <c r="I64" s="158">
+        <v>45974</v>
+      </c>
+      <c r="J64" s="2">
+        <v>1</v>
+      </c>
+      <c r="K64" s="158">
         <f t="shared" si="5"/>
         <v>46039</v>
       </c>
-      <c r="L62" s="155">
+      <c r="L64" s="155">
         <v>330</v>
       </c>
-      <c r="M62" s="155">
+      <c r="M64" s="155">
         <f t="shared" si="6"/>
         <v>506.63240000000002</v>
       </c>
-      <c r="N62" s="3">
+      <c r="N64" s="3">
         <f t="shared" si="4"/>
         <v>162122.36800000002</v>
       </c>
     </row>
-    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="2">
-        <v>2024</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D63" s="159" t="s">
-        <v>349</v>
-      </c>
-      <c r="E63" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="H63" s="2">
-        <v>0</v>
-      </c>
-      <c r="I63" s="158">
-        <v>45809</v>
-      </c>
-      <c r="J63" s="2">
-        <v>1</v>
-      </c>
-      <c r="K63" s="158">
-        <v>45809</v>
-      </c>
-      <c r="L63" s="155"/>
-      <c r="M63" s="155"/>
-      <c r="N63" s="3"/>
-      <c r="P63" s="3">
-        <v>3000</v>
-      </c>
-      <c r="Q63" s="3">
-        <f>E63*P63</f>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="2">
-        <v>2025</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D64" s="159" t="s">
-        <v>350</v>
-      </c>
-      <c r="E64" s="2">
-        <v>320</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H64" s="2">
-        <v>0</v>
-      </c>
-      <c r="I64" s="158">
-        <v>45931</v>
-      </c>
-      <c r="J64" s="2">
-        <v>1</v>
-      </c>
-      <c r="K64" s="158">
-        <v>45931</v>
-      </c>
-      <c r="L64" s="155"/>
-      <c r="M64" s="155">
-        <v>463.2</v>
-      </c>
-      <c r="N64" s="3">
-        <f>M64*E64</f>
-        <v>148224</v>
-      </c>
-    </row>
     <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D65" s="159" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E65" s="2">
-        <v>12</v>
+        <v>0.5</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>37</v>
+        <v>290</v>
       </c>
       <c r="H65" s="2">
         <v>0</v>
       </c>
       <c r="I65" s="158">
-        <v>45880</v>
+        <v>45809</v>
       </c>
       <c r="J65" s="2">
         <v>1</v>
       </c>
       <c r="K65" s="158">
-        <v>45880</v>
+        <v>45809</v>
       </c>
       <c r="L65" s="155"/>
       <c r="M65" s="155"/>
       <c r="N65" s="3"/>
       <c r="P65" s="3">
-        <v>2350</v>
+        <v>3000</v>
       </c>
       <c r="Q65" s="3">
         <f>E65*P65</f>
-        <v>28200</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>2025</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="D66" s="159" t="s">
-        <v>257</v>
+        <v>350</v>
       </c>
       <c r="E66" s="2">
-        <v>20</v>
+        <v>320</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H66" s="2">
         <v>0</v>
       </c>
       <c r="I66" s="158">
-        <v>45887</v>
+        <v>45931</v>
       </c>
       <c r="J66" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K66" s="158">
-        <v>45880</v>
+        <v>45931</v>
       </c>
       <c r="L66" s="155"/>
-      <c r="M66" s="155"/>
-      <c r="N66" s="3"/>
-      <c r="P66" s="3">
-        <v>2250</v>
-      </c>
-      <c r="Q66" s="3">
-        <f>E66*P66</f>
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M66" s="155">
+        <v>463.2</v>
+      </c>
+      <c r="N66" s="3">
+        <f>M66*E66</f>
+        <v>148224</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>2025</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D67" s="159" t="s">
-        <v>24</v>
+        <v>351</v>
       </c>
       <c r="E67" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>37</v>
@@ -7954,23 +7970,23 @@
         <v>0</v>
       </c>
       <c r="I67" s="158">
-        <v>45889</v>
+        <v>45880</v>
       </c>
       <c r="J67" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K67" s="158">
-        <v>45920</v>
+        <v>45880</v>
       </c>
       <c r="L67" s="155"/>
       <c r="M67" s="155"/>
       <c r="N67" s="3"/>
       <c r="P67" s="3">
-        <v>2500</v>
+        <v>2350</v>
       </c>
       <c r="Q67" s="3">
         <f>E67*P67</f>
-        <v>7500</v>
+        <v>28200</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
@@ -7978,54 +7994,52 @@
         <v>2025</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D68" s="159" t="s">
-        <v>46</v>
-      </c>
-      <c r="E68" s="213">
-        <f>20000/60</f>
-        <v>333.33333333333331</v>
+        <v>257</v>
+      </c>
+      <c r="E68" s="2">
+        <v>20</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>289</v>
+        <v>37</v>
       </c>
       <c r="H68" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I68" s="158">
-        <v>45901</v>
+        <v>45887</v>
       </c>
       <c r="J68" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K68" s="158">
-        <v>46049</v>
-      </c>
-      <c r="L68" s="155">
-        <f>M68/1.3228</f>
-        <v>417.28000000000003</v>
-      </c>
-      <c r="M68" s="155">
-        <v>551.97798399999999</v>
-      </c>
-      <c r="N68" s="3">
-        <f>M68*E68</f>
-        <v>183992.66133333332</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+        <v>45880</v>
+      </c>
+      <c r="L68" s="155"/>
+      <c r="M68" s="155"/>
+      <c r="N68" s="3"/>
+      <c r="P68" s="3">
+        <v>2250</v>
+      </c>
+      <c r="Q68" s="3">
+        <f>E68*P68</f>
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>2025</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>89</v>
@@ -8033,8 +8047,8 @@
       <c r="D69" s="159" t="s">
         <v>24</v>
       </c>
-      <c r="E69" s="213">
-        <v>5</v>
+      <c r="E69" s="2">
+        <v>3</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>33</v>
@@ -8046,78 +8060,78 @@
         <v>0</v>
       </c>
       <c r="I69" s="158">
-        <v>45923</v>
+        <v>45889</v>
       </c>
       <c r="J69" s="2">
         <v>2</v>
       </c>
       <c r="K69" s="158">
-        <f>I69+20</f>
-        <v>45943</v>
+        <v>45920</v>
       </c>
       <c r="L69" s="155"/>
       <c r="M69" s="155"/>
       <c r="N69" s="3"/>
       <c r="P69" s="3">
-        <v>2750</v>
+        <v>2500</v>
       </c>
       <c r="Q69" s="3">
-        <f t="shared" ref="Q69:Q80" si="7">E69*P69</f>
-        <v>13750</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+        <f>E69*P69</f>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>2025</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="D70" s="159" t="s">
-        <v>351</v>
+        <v>46</v>
       </c>
       <c r="E70" s="213">
-        <v>10</v>
+        <f>20000/60</f>
+        <v>333.33333333333331</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H70" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I70" s="158">
-        <v>45923</v>
+        <v>45901</v>
       </c>
       <c r="J70" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K70" s="158">
-        <f>I70+20</f>
-        <v>45943</v>
-      </c>
-      <c r="L70" s="155"/>
-      <c r="M70" s="155"/>
-      <c r="N70" s="3"/>
-      <c r="P70" s="3">
-        <v>3200</v>
-      </c>
-      <c r="Q70" s="3">
-        <f t="shared" si="7"/>
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+        <v>46080</v>
+      </c>
+      <c r="L70" s="155">
+        <f>M70/1.3228</f>
+        <v>417.28000000000003</v>
+      </c>
+      <c r="M70" s="155">
+        <v>551.97798399999999</v>
+      </c>
+      <c r="N70" s="3">
+        <f>M70*E70</f>
+        <v>183992.66133333332</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>2025</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>89</v>
@@ -8126,7 +8140,7 @@
         <v>24</v>
       </c>
       <c r="E71" s="213">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>33</v>
@@ -8138,24 +8152,24 @@
         <v>0</v>
       </c>
       <c r="I71" s="158">
-        <v>45979</v>
+        <v>45923</v>
       </c>
       <c r="J71" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K71" s="158">
-        <f>I71</f>
-        <v>45979</v>
+        <f>I71+20</f>
+        <v>45943</v>
       </c>
       <c r="L71" s="155"/>
       <c r="M71" s="155"/>
       <c r="N71" s="3"/>
       <c r="P71" s="3">
-        <v>2650</v>
+        <v>2750</v>
       </c>
       <c r="Q71" s="3">
-        <f t="shared" si="7"/>
-        <v>7950</v>
+        <f t="shared" ref="Q71:Q82" si="12">E71*P71</f>
+        <v>13750</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
@@ -8163,81 +8177,81 @@
         <v>2025</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D72" s="159" t="s">
-        <v>24</v>
+        <v>351</v>
       </c>
       <c r="E72" s="213">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>37</v>
+        <v>290</v>
       </c>
       <c r="H72" s="2">
         <v>0</v>
       </c>
       <c r="I72" s="158">
-        <v>46023</v>
+        <v>45923</v>
       </c>
       <c r="J72" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K72" s="158">
-        <f t="shared" ref="K72:K74" si="8">I72</f>
-        <v>46023</v>
+        <f>I72+20</f>
+        <v>45943</v>
       </c>
       <c r="L72" s="155"/>
       <c r="M72" s="155"/>
       <c r="N72" s="3"/>
       <c r="P72" s="3">
-        <v>2650</v>
+        <v>3200</v>
       </c>
       <c r="Q72" s="3">
-        <f t="shared" si="7"/>
-        <v>31800</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="12"/>
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>2025</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D73" s="159" t="s">
-        <v>257</v>
+        <v>24</v>
       </c>
       <c r="E73" s="213">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H73" s="2">
         <v>0</v>
       </c>
       <c r="I73" s="158">
-        <v>45986</v>
+        <v>45979</v>
       </c>
       <c r="J73" s="2">
         <v>1</v>
       </c>
       <c r="K73" s="158">
-        <f t="shared" si="8"/>
-        <v>45986</v>
+        <f>I73</f>
+        <v>45979</v>
       </c>
       <c r="L73" s="155"/>
       <c r="M73" s="155"/>
@@ -8246,54 +8260,54 @@
         <v>2650</v>
       </c>
       <c r="Q73" s="3">
-        <f t="shared" si="7"/>
-        <v>79500</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="12"/>
+        <v>7950</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>2025</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D74" s="159" t="s">
-        <v>361</v>
+        <v>24</v>
       </c>
       <c r="E74" s="213">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>290</v>
+        <v>37</v>
       </c>
       <c r="H74" s="2">
         <v>0</v>
       </c>
       <c r="I74" s="158">
-        <v>45979</v>
+        <v>46023</v>
       </c>
       <c r="J74" s="2">
         <v>1</v>
       </c>
       <c r="K74" s="158">
-        <f t="shared" si="8"/>
-        <v>45979</v>
+        <f t="shared" ref="K74:K76" si="13">I74</f>
+        <v>46023</v>
       </c>
       <c r="L74" s="155"/>
       <c r="M74" s="155"/>
       <c r="N74" s="3"/>
       <c r="P74" s="3">
-        <v>2300</v>
+        <v>2650</v>
       </c>
       <c r="Q74" s="3">
-        <f t="shared" si="7"/>
-        <v>11500</v>
+        <f t="shared" si="12"/>
+        <v>31800</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
@@ -8301,45 +8315,45 @@
         <v>2025</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D75" s="159" t="s">
-        <v>364</v>
+        <v>257</v>
       </c>
       <c r="E75" s="213">
-        <v>161</v>
+        <v>30</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>289</v>
+        <v>35</v>
       </c>
       <c r="H75" s="2">
         <v>0</v>
       </c>
       <c r="I75" s="158">
-        <v>46014</v>
+        <v>45986</v>
       </c>
       <c r="J75" s="2">
         <v>1</v>
       </c>
       <c r="K75" s="158">
-        <f t="shared" ref="K75:K79" si="9">I75</f>
-        <v>46014</v>
+        <f t="shared" si="13"/>
+        <v>45986</v>
       </c>
       <c r="L75" s="155"/>
       <c r="M75" s="155"/>
       <c r="N75" s="3"/>
       <c r="P75" s="3">
-        <v>2600</v>
+        <v>2650</v>
       </c>
       <c r="Q75" s="3">
-        <f t="shared" ref="Q75:Q76" si="10">E75*P75</f>
-        <v>418600</v>
+        <f t="shared" si="12"/>
+        <v>79500</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
@@ -8347,45 +8361,45 @@
         <v>2025</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D76" s="159" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E76" s="213">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H76" s="2">
         <v>0</v>
       </c>
       <c r="I76" s="158">
-        <v>46014</v>
+        <v>45979</v>
       </c>
       <c r="J76" s="2">
         <v>1</v>
       </c>
       <c r="K76" s="158">
-        <f t="shared" si="9"/>
-        <v>46014</v>
+        <f t="shared" si="13"/>
+        <v>45979</v>
       </c>
       <c r="L76" s="155"/>
       <c r="M76" s="155"/>
       <c r="N76" s="3"/>
       <c r="P76" s="3">
-        <v>2600</v>
+        <v>2300</v>
       </c>
       <c r="Q76" s="3">
-        <f t="shared" si="10"/>
-        <v>195000</v>
+        <f t="shared" si="12"/>
+        <v>11500</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
@@ -8393,7 +8407,7 @@
         <v>2025</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>89</v>
@@ -8402,13 +8416,13 @@
         <v>364</v>
       </c>
       <c r="E77" s="213">
-        <v>4</v>
+        <v>161</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>32</v>
+        <v>289</v>
       </c>
       <c r="H77" s="2">
         <v>0</v>
@@ -8420,7 +8434,7 @@
         <v>1</v>
       </c>
       <c r="K77" s="158">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="K77:K81" si="14">I77</f>
         <v>46014</v>
       </c>
       <c r="L77" s="155"/>
@@ -8430,8 +8444,8 @@
         <v>2600</v>
       </c>
       <c r="Q77" s="3">
-        <f t="shared" ref="Q77:Q79" si="11">E77*P77</f>
-        <v>10400</v>
+        <f t="shared" ref="Q77:Q78" si="15">E77*P77</f>
+        <v>418600</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
@@ -8439,7 +8453,7 @@
         <v>2025</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>89</v>
@@ -8448,13 +8462,13 @@
         <v>364</v>
       </c>
       <c r="E78" s="213">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>32</v>
+        <v>289</v>
       </c>
       <c r="H78" s="2">
         <v>0</v>
@@ -8466,7 +8480,7 @@
         <v>1</v>
       </c>
       <c r="K78" s="158">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>46014</v>
       </c>
       <c r="L78" s="155"/>
@@ -8476,8 +8490,8 @@
         <v>2600</v>
       </c>
       <c r="Q78" s="3">
-        <f t="shared" si="11"/>
-        <v>26000</v>
+        <f t="shared" si="15"/>
+        <v>195000</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
@@ -8485,7 +8499,7 @@
         <v>2025</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>89</v>
@@ -8494,7 +8508,7 @@
         <v>364</v>
       </c>
       <c r="E79" s="213">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>27</v>
@@ -8512,36 +8526,38 @@
         <v>1</v>
       </c>
       <c r="K79" s="158">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>46014</v>
       </c>
       <c r="L79" s="155"/>
       <c r="M79" s="155"/>
       <c r="N79" s="3"/>
       <c r="P79" s="3">
-        <v>2600</v>
+        <v>5000</v>
       </c>
       <c r="Q79" s="3">
-        <f t="shared" si="11"/>
-        <v>26000</v>
+        <f t="shared" ref="Q79:Q81" si="16">E79*P79</f>
+        <v>20000</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>2025</v>
       </c>
+      <c r="B80" s="2" t="s">
+        <v>366</v>
+      </c>
       <c r="C80" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D80" s="159" t="s">
-        <v>331</v>
+        <v>364</v>
       </c>
       <c r="E80" s="213">
-        <f>2400-E66-E65-E67-E69-E70-E71-E72-E73-E74-E75-E76-E77-E78-E79</f>
-        <v>2040</v>
+        <v>10</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>32</v>
@@ -8550,40 +8566,44 @@
         <v>0</v>
       </c>
       <c r="I80" s="158">
-        <v>46023</v>
+        <v>46014</v>
       </c>
       <c r="J80" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K80" s="158">
-        <v>46023</v>
-      </c>
-      <c r="L80" s="158"/>
+        <f t="shared" si="14"/>
+        <v>46014</v>
+      </c>
+      <c r="L80" s="155"/>
+      <c r="M80" s="155"/>
       <c r="N80" s="3"/>
       <c r="P80" s="3">
-        <v>1600</v>
+        <v>4600</v>
       </c>
       <c r="Q80" s="3">
-        <f t="shared" si="7"/>
-        <v>3264000</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="16"/>
+        <v>46000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>2025</v>
       </c>
+      <c r="B81" s="2" t="s">
+        <v>367</v>
+      </c>
       <c r="C81" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D81" s="159" t="s">
-        <v>331</v>
-      </c>
-      <c r="E81" s="2">
-        <f>0.7*8000-4800-E82-E83-E68</f>
-        <v>286.49999999999994</v>
+        <v>364</v>
+      </c>
+      <c r="E81" s="213">
+        <v>10</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>32</v>
@@ -8592,38 +8612,39 @@
         <v>0</v>
       </c>
       <c r="I81" s="158">
-        <v>46023</v>
+        <v>46014</v>
       </c>
       <c r="J81" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K81" s="158">
-        <v>46023</v>
-      </c>
-      <c r="L81" s="155">
-        <v>325</v>
-      </c>
-      <c r="M81" s="155">
-        <f>(L81+H81)*1.3228</f>
-        <v>429.90999999999997</v>
-      </c>
-      <c r="N81" s="3">
-        <f>M81*E81</f>
-        <v>123169.21499999997</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="14"/>
+        <v>46014</v>
+      </c>
+      <c r="L81" s="155"/>
+      <c r="M81" s="155"/>
+      <c r="N81" s="3"/>
+      <c r="P81" s="3">
+        <v>4600</v>
+      </c>
+      <c r="Q81" s="3">
+        <f t="shared" si="16"/>
+        <v>46000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>2025</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D82" s="159" t="s">
         <v>331</v>
       </c>
-      <c r="E82" s="2">
-        <v>64.5</v>
+      <c r="E82" s="213">
+        <f>2400-E68-E67-E69-E71-E72-E73-E74-E75-E76-E77-E78-E79-E80-E81</f>
+        <v>2040</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>32</v>
@@ -8638,24 +8659,22 @@
         <v>46023</v>
       </c>
       <c r="J82" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K82" s="158">
         <v>46023</v>
       </c>
-      <c r="L82" s="155">
-        <v>330</v>
-      </c>
-      <c r="M82" s="155">
-        <f>(L82+H82)*1.3228</f>
-        <v>436.524</v>
-      </c>
-      <c r="N82" s="3">
-        <f>M82*E82</f>
-        <v>28155.797999999999</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L82" s="158"/>
+      <c r="N82" s="3"/>
+      <c r="P82" s="3">
+        <v>1600</v>
+      </c>
+      <c r="Q82" s="3">
+        <f t="shared" si="12"/>
+        <v>3264000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>2025</v>
       </c>
@@ -8665,9 +8684,9 @@
       <c r="D83" s="159" t="s">
         <v>331</v>
       </c>
-      <c r="E83" s="213">
-        <f>449-E68</f>
-        <v>115.66666666666669</v>
+      <c r="E83" s="2">
+        <f>0.7*8000-4800-E84-E85-E70</f>
+        <v>286.49999999999994</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>32</v>
@@ -8679,13 +8698,13 @@
         <v>0</v>
       </c>
       <c r="I83" s="158">
-        <v>46082</v>
+        <v>46023</v>
       </c>
       <c r="J83" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K83" s="158">
-        <v>46082</v>
+        <v>46023</v>
       </c>
       <c r="L83" s="155">
         <v>325</v>
@@ -8696,20 +8715,105 @@
       </c>
       <c r="N83" s="3">
         <f>M83*E83</f>
+        <v>123169.21499999997</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A84" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D84" s="159" t="s">
+        <v>331</v>
+      </c>
+      <c r="E84" s="2">
+        <v>64.5</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H84" s="2">
+        <v>0</v>
+      </c>
+      <c r="I84" s="158">
+        <v>46023</v>
+      </c>
+      <c r="J84" s="2">
+        <v>1</v>
+      </c>
+      <c r="K84" s="158">
+        <v>46023</v>
+      </c>
+      <c r="L84" s="155">
+        <v>330</v>
+      </c>
+      <c r="M84" s="155">
+        <f>(L84+H84)*1.3228</f>
+        <v>436.524</v>
+      </c>
+      <c r="N84" s="3">
+        <f>M84*E84</f>
+        <v>28155.797999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A85" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D85" s="159" t="s">
+        <v>331</v>
+      </c>
+      <c r="E85" s="213">
+        <f>449-E70</f>
+        <v>115.66666666666669</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H85" s="2">
+        <v>0</v>
+      </c>
+      <c r="I85" s="158">
+        <v>46082</v>
+      </c>
+      <c r="J85" s="2">
+        <v>1</v>
+      </c>
+      <c r="K85" s="158">
+        <v>46082</v>
+      </c>
+      <c r="L85" s="155">
+        <v>325</v>
+      </c>
+      <c r="M85" s="155">
+        <f>(L85+H85)*1.3228</f>
+        <v>429.90999999999997</v>
+      </c>
+      <c r="N85" s="3">
+        <f>M85*E85</f>
         <v>49726.256666666668</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q83" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
-    <filterColumn colId="10">
+  <autoFilter ref="A1:Q85" xr:uid="{E433115D-D1E6-C943-B0EC-2BC4BD1B44BA}">
+    <filterColumn colId="0">
       <filters>
-        <dateGroupItem year="2026" month="1" dateTimeGrouping="month"/>
-        <dateGroupItem year="2026" month="2" dateTimeGrouping="month"/>
-        <dateGroupItem year="2025" month="12" dateTimeGrouping="month"/>
+        <filter val="2025"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q83">
-      <sortCondition ref="B1:B83"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q85">
+      <sortCondition ref="B1:B85"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -8725,7 +8829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62549E7F-C2F6-E740-8F49-EDB7C93FB4DD}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>